<commit_message>
P4-2238 - Write journeys tab on output spreadsheet
JPC_template.xlsx updated to contain the new tab

JourneysSheet - generates the rows for the new journey tab
Called from PricesSpreadsheetGenerator, displays the unique journeys
PricesSpreadsheetGenerator gets journeys from MoveService

MoveQueryRepository
uniqueJourneysInDateRange takes excludePriced parameter (defaults to true)

UniqueJourney
Add methods for unitPrice in pence / pounds and from / to site name

Person
Change latestNomisBookingId type to be Int? not String?
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonnycavell/p/calculate-people-move-prices/src/main/resources/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1646D3B-0C71-3B40-A702-F15661FB2D3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85A24CD-E0EF-2847-90F8-8FB012E9B092}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26800" windowHeight="17500" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="Redirections" sheetId="4" r:id="rId4"/>
     <sheet name="Lockouts" sheetId="5" r:id="rId5"/>
     <sheet name="Multi-type" sheetId="6" r:id="rId6"/>
-    <sheet name="Cancelled" sheetId="7" r:id="rId7"/>
-    <sheet name="JPC Price book" sheetId="8" r:id="rId8"/>
+    <sheet name="Cancelled" sheetId="9" r:id="rId7"/>
+    <sheet name="Journeys" sheetId="7" r:id="rId8"/>
+    <sheet name="JPC Price book" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
   <si>
     <t>Export date</t>
   </si>
@@ -337,6 +338,18 @@
   </si>
   <si>
     <t xml:space="preserve">prison to prison moves cancelled by PMU later than </t>
+  </si>
+  <si>
+    <t>TOTAL VOLUME BY LOCATION</t>
+  </si>
+  <si>
+    <t>Unit price</t>
+  </si>
+  <si>
+    <t>Total price</t>
+  </si>
+  <si>
+    <t>Total journey count</t>
   </si>
 </sst>
 </file>
@@ -959,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+    <sheetView zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -4311,7 +4324,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7A879C-62CC-6745-83D4-09C9DF326994}">
   <dimension ref="A1:AD10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4665,6 +4678,348 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AD10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="40.83203125" customWidth="1"/>
+    <col min="12" max="1025" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+    </row>
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+    </row>
+    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+    </row>
+    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+    </row>
+    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+    </row>
+    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+    </row>
+    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+    </row>
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+    </row>
+    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" s="26"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+    </row>
+    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
P4-2238 - Write journeys tab on output spreadsheet (#104)
JPC_template.xlsx updated to contain the new tab

JourneysSheet - generates the rows for the new journey tab
Called from PricesSpreadsheetGenerator, displays the unique journeys
PricesSpreadsheetGenerator gets journeys from MoveService

MoveQueryRepository
uniqueJourneysInDateRange takes excludePriced parameter (defaults to true)

UniqueJourney
Add methods for unitPrice in pence / pounds and from / to site name

Person
Change latestNomisBookingId type to be Int? not String?
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonnycavell/p/calculate-people-move-prices/src/main/resources/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1646D3B-0C71-3B40-A702-F15661FB2D3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85A24CD-E0EF-2847-90F8-8FB012E9B092}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26800" windowHeight="17500" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="Redirections" sheetId="4" r:id="rId4"/>
     <sheet name="Lockouts" sheetId="5" r:id="rId5"/>
     <sheet name="Multi-type" sheetId="6" r:id="rId6"/>
-    <sheet name="Cancelled" sheetId="7" r:id="rId7"/>
-    <sheet name="JPC Price book" sheetId="8" r:id="rId8"/>
+    <sheet name="Cancelled" sheetId="9" r:id="rId7"/>
+    <sheet name="Journeys" sheetId="7" r:id="rId8"/>
+    <sheet name="JPC Price book" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
   <si>
     <t>Export date</t>
   </si>
@@ -337,6 +338,18 @@
   </si>
   <si>
     <t xml:space="preserve">prison to prison moves cancelled by PMU later than </t>
+  </si>
+  <si>
+    <t>TOTAL VOLUME BY LOCATION</t>
+  </si>
+  <si>
+    <t>Unit price</t>
+  </si>
+  <si>
+    <t>Total price</t>
+  </si>
+  <si>
+    <t>Total journey count</t>
   </si>
 </sst>
 </file>
@@ -959,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+    <sheetView zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -4311,7 +4324,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7A879C-62CC-6745-83D4-09C9DF326994}">
   <dimension ref="A1:AD10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4665,6 +4678,348 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AD10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="40.83203125" customWidth="1"/>
+    <col min="12" max="1025" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+    </row>
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+    </row>
+    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+    </row>
+    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+    </row>
+    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+    </row>
+    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+    </row>
+    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+    </row>
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+    </row>
+    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" s="26"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+    </row>
+    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
P4-2517 extracts prices from the DB when generating output spreadsheet instead of original prices files.
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonnycavell/p/calculate-people-move-prices/src/main/resources/spreadsheets/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85A24CD-E0EF-2847-90F8-8FB012E9B092}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26800" windowHeight="17500" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Standard" sheetId="2" r:id="rId2"/>
-    <sheet name="Long haul" sheetId="3" r:id="rId3"/>
-    <sheet name="Redirections" sheetId="4" r:id="rId4"/>
-    <sheet name="Lockouts" sheetId="5" r:id="rId5"/>
-    <sheet name="Multi-type" sheetId="6" r:id="rId6"/>
-    <sheet name="Cancelled" sheetId="9" r:id="rId7"/>
-    <sheet name="Journeys" sheetId="7" r:id="rId8"/>
-    <sheet name="JPC Price book" sheetId="8" r:id="rId9"/>
+    <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Standard" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Long haul" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Redirections" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Lockouts" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Multi-type" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Cancelled" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Journeys" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="JPC Price book" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -33,81 +28,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
-  <si>
-    <t>Export date</t>
-  </si>
-  <si>
-    <t>Calculate Journey Variable Payments (S2B)</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
-  <si>
-    <t>Date Range</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>OUTPUT SUMMARY</t>
-  </si>
-  <si>
-    <t>Move type</t>
-  </si>
-  <si>
-    <t>Percentage</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="74">
+  <si>
+    <t xml:space="preserve">Export date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate Journey Variable Payments (S2B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTPUT SUMMARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage</t>
   </si>
   <si>
     <t xml:space="preserve"> Move volume</t>
   </si>
   <si>
-    <t>Move volume without prices</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Standard move</t>
-  </si>
-  <si>
-    <t>includes single journeys, cross supplier and redirects before the move has started</t>
+    <t xml:space="preserve">Move volume without prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes single journeys, cross supplier and redirects before the move has started</t>
   </si>
   <si>
     <t xml:space="preserve">Long haul </t>
   </si>
   <si>
-    <t>a completed move made up of 2 or more journeys</t>
-  </si>
-  <si>
-    <t>Redirections</t>
-  </si>
-  <si>
-    <t>a redirection after the move has started</t>
-  </si>
-  <si>
-    <t>Lockouts</t>
-  </si>
-  <si>
-    <t>refused admission to prison</t>
-  </si>
-  <si>
-    <t>Multi-type moves</t>
-  </si>
-  <si>
-    <t>includes combinations of the above</t>
-  </si>
-  <si>
-    <t>Total %</t>
-  </si>
-  <si>
-    <t>Total volume</t>
-  </si>
-  <si>
-    <t>Total volume without prices</t>
-  </si>
-  <si>
-    <t>Total Price</t>
+    <t xml:space="preserve">a completed move made up of 2 or more journeys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redirections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a redirection after the move has started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lockouts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refused admission to prison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-type moves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes combinations of the above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancelled moves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prison to prison moves cancelled by PMU later than </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3pm the day before the move date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total volume without prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Price</t>
   </si>
   <si>
     <r>
@@ -122,104 +126,104 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(includes single journeys, cross supplier and redirects before the move has started)</t>
+      <t xml:space="preserve">(includes single journeys, cross supplier and redirects before the move has started)</t>
     </r>
   </si>
   <si>
-    <t>Move Ref ID</t>
-  </si>
-  <si>
-    <t>Pick up</t>
-  </si>
-  <si>
-    <t>Location Type</t>
-  </si>
-  <si>
-    <t>Drop off</t>
-  </si>
-  <si>
-    <t>Pick up date</t>
-  </si>
-  <si>
-    <t>Pick up time</t>
-  </si>
-  <si>
-    <t>Drop off date</t>
-  </si>
-  <si>
-    <t>Drop off time</t>
+    <t xml:space="preserve">Move Ref ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off time</t>
   </si>
   <si>
     <t xml:space="preserve">Vehicle Reg </t>
   </si>
   <si>
-    <t>NOMIS Prison ID</t>
-  </si>
-  <si>
-    <t>LONG HAUL</t>
-  </si>
-  <si>
-    <t>Move ID</t>
-  </si>
-  <si>
-    <t>Vehicle Reg</t>
-  </si>
-  <si>
-    <t>Billable?</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>MX1234</t>
-  </si>
-  <si>
-    <t>BRADFORD POLICE STATION (TRAFALGAR HOUSE)</t>
-  </si>
-  <si>
-    <t>LEEDS MAGISTRATES COURT</t>
-  </si>
-  <si>
-    <t>XXX9876</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>Journey 1</t>
-  </si>
-  <si>
-    <t>PS</t>
-  </si>
-  <si>
-    <t>DERBY POLICE CUSTODY</t>
-  </si>
-  <si>
-    <t>GD-5555</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>Long journey, ovenight stay.</t>
-  </si>
-  <si>
-    <t>Journey 2</t>
-  </si>
-  <si>
-    <t>MC</t>
-  </si>
-  <si>
-    <t>XX-5786</t>
-  </si>
-  <si>
-    <t>SERCO</t>
+    <t xml:space="preserve">NOMIS Prison ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LONG HAUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billable?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MX1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRADFORD POLICE STATION (TRAFALGAR HOUSE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEEDS MAGISTRATES COURT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XXX9876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journey 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DERBY POLICE CUSTODY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GD-5555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long journey, ovenight stay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journey 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XX-5786</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERCO</t>
   </si>
   <si>
     <r>
@@ -234,20 +238,20 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(a redirection after the move has started)</t>
+      <t xml:space="preserve">(a redirection after the move has started)</t>
     </r>
   </si>
   <si>
-    <t>Contractor Billable?</t>
-  </si>
-  <si>
-    <t>Notes (Reason codes or supplier notes)</t>
+    <t xml:space="preserve">Contractor Billable?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes (Reason codes or supplier notes)</t>
   </si>
   <si>
     <r>
@@ -262,17 +266,17 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="9"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(refused admission to prison)</t>
+      <t xml:space="preserve">(refused admission to prison)</t>
     </r>
   </si>
   <si>
-    <t>Date range</t>
+    <t xml:space="preserve">Date range</t>
   </si>
   <si>
     <r>
@@ -283,11 +287,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>MULTI-TYPE MOVES</t>
+      <t xml:space="preserve">MULTI-TYPE MOVES</t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -309,62 +313,74 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(includes prison to prison transfer moves that have been cancelled by the population mangement unit after 3pm on the day before the move)</t>
+      <t xml:space="preserve">(includes prison to prison transfer moves that have been cancelled by the population mangement unit after 3pm on the day before the move)</t>
     </r>
   </si>
   <si>
-    <t>Move date</t>
-  </si>
-  <si>
-    <t>Cancellation date</t>
-  </si>
-  <si>
-    <t>Cancellation time</t>
-  </si>
-  <si>
-    <t>Dev notes:</t>
-  </si>
-  <si>
-    <t>3pm the day before the move date</t>
-  </si>
-  <si>
-    <t>Cancelled moves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prison to prison moves cancelled by PMU later than </t>
-  </si>
-  <si>
-    <t>TOTAL VOLUME BY LOCATION</t>
-  </si>
-  <si>
-    <t>Unit price</t>
-  </si>
-  <si>
-    <t>Total price</t>
-  </si>
-  <si>
-    <t>Total journey count</t>
+    <t xml:space="preserve">Move date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancellation date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancellation time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev notes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL VOLUME BY LOCATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total journey count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="\£#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="0%"/>
+    <numFmt numFmtId="167" formatCode="#,##0"/>
+    <numFmt numFmtId="168" formatCode="\£#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="HH:MM"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -374,7 +390,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -382,7 +398,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -390,14 +406,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -410,7 +426,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -480,7 +496,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -488,112 +504,225 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="46">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -652,340 +781,32 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +837,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1044,7 +865,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
     </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1072,7 +893,7 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1102,7 +923,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
     </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1132,7 +953,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1164,7 +985,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1193,7 +1014,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -1224,7 +1045,7 @@
       <c r="Z8" s="9"/>
       <c r="AA8" s="9"/>
     </row>
-    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
@@ -1263,7 +1084,7 @@
       <c r="Z9" s="13"/>
       <c r="AA9" s="13"/>
     </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
         <v>11</v>
       </c>
@@ -1294,7 +1115,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
         <v>12</v>
       </c>
@@ -1325,7 +1146,7 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="18"/>
@@ -1354,7 +1175,7 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="s">
         <v>13</v>
       </c>
@@ -1385,7 +1206,7 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
         <v>14</v>
       </c>
@@ -1412,7 +1233,7 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="17"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1441,7 +1262,7 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
@@ -1472,7 +1293,7 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
         <v>16</v>
       </c>
@@ -1503,7 +1324,7 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1532,7 +1353,7 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="s">
         <v>17</v>
       </c>
@@ -1563,7 +1384,7 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="17" t="s">
         <v>18</v>
       </c>
@@ -1594,7 +1415,7 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1623,7 +1444,7 @@
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
         <v>19</v>
       </c>
@@ -1654,7 +1475,7 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="17" t="s">
         <v>20</v>
       </c>
@@ -1685,7 +1506,7 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1714,9 +1535,9 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1745,9 +1566,9 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="17" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1776,9 +1597,9 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="17" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1807,19 +1628,19 @@
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
     </row>
-    <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="22"/>
       <c r="B28" s="23" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1844,7 +1665,7 @@
       <c r="Z28" s="4"/>
       <c r="AA28" s="4"/>
     </row>
-    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1873,7 +1694,7 @@
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
       <c r="B30" s="20"/>
       <c r="C30" s="1"/>
@@ -1902,7 +1723,7 @@
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1932,33 +1753,41 @@
       <c r="AA31" s="24"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="19.5" customWidth="1"/>
-    <col min="11" max="11" width="15.5" customWidth="1"/>
-    <col min="12" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1994,7 +1823,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2028,7 +1857,7 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
-    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2062,7 +1891,7 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -2098,7 +1927,7 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
-    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2134,7 +1963,7 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
-    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2172,7 +2001,7 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
-    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2206,9 +2035,9 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2242,39 +2071,39 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="L9" s="27" t="s">
         <v>10</v>
@@ -2300,7 +2129,7 @@
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
     </row>
-    <row r="10" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2334,7 +2163,7 @@
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
     </row>
-    <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2368,7 +2197,7 @@
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
     </row>
-    <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2402,7 +2231,7 @@
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
     </row>
-    <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2436,7 +2265,7 @@
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
     </row>
-    <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2470,7 +2299,7 @@
       <c r="AE14" s="28"/>
       <c r="AF14" s="28"/>
     </row>
-    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2504,7 +2333,7 @@
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
     </row>
-    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2538,7 +2367,7 @@
       <c r="AE16" s="28"/>
       <c r="AF16" s="28"/>
     </row>
-    <row r="17" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2572,7 +2401,7 @@
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
     </row>
-    <row r="18" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2606,7 +2435,7 @@
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
     </row>
-    <row r="19" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2640,7 +2469,7 @@
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
     </row>
-    <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2674,7 +2503,7 @@
       <c r="AE20" s="28"/>
       <c r="AF20" s="28"/>
     </row>
-    <row r="21" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2708,7 +2537,7 @@
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
     </row>
-    <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2742,7 +2571,7 @@
       <c r="AE22" s="28"/>
       <c r="AF22" s="28"/>
     </row>
-    <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2776,7 +2605,7 @@
       <c r="AE23" s="28"/>
       <c r="AF23" s="28"/>
     </row>
-    <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2810,7 +2639,7 @@
       <c r="AE24" s="28"/>
       <c r="AF24" s="28"/>
     </row>
-    <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2844,7 +2673,7 @@
       <c r="AE25" s="28"/>
       <c r="AF25" s="28"/>
     </row>
-    <row r="26" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2879,38 +2708,46 @@
       <c r="AF26" s="28"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" customWidth="1"/>
-    <col min="12" max="12" width="10.1640625" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="50" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2928,7 +2765,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -2944,7 +2781,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
@@ -2960,7 +2797,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -2978,7 +2815,7 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2996,7 +2833,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3016,7 +2853,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3032,9 +2869,9 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3050,48 +2887,48 @@
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J9" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="26" t="s">
         <v>38</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>35</v>
       </c>
       <c r="L9" s="27" t="s">
         <v>10</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="O9" s="31"/>
       <c r="P9" s="31"/>
@@ -3106,153 +2943,161 @@
       <c r="Y9" s="31"/>
       <c r="Z9" s="31"/>
     </row>
-    <row r="10" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="10" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="32">
+      <c r="F10" s="32" t="n">
         <v>43845</v>
       </c>
-      <c r="G10" s="33">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="H10" s="32">
+      <c r="G10" s="33" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H10" s="32" t="n">
         <v>43846</v>
       </c>
-      <c r="I10" s="33">
-        <v>0.74305555555555602</v>
+      <c r="I10" s="33" t="n">
+        <v>0.743055555555556</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="34" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L10" s="35" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="11" customFormat="false" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="36">
+        <v>50</v>
+      </c>
+      <c r="F11" s="36" t="n">
         <v>43845</v>
       </c>
-      <c r="G11" s="37">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="H11" s="36">
+      <c r="G11" s="37" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H11" s="36" t="n">
         <v>43845</v>
       </c>
-      <c r="I11" s="37">
-        <v>0.60416666666666696</v>
+      <c r="I11" s="37" t="n">
+        <v>0.604166666666667</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="39" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="M11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="36" t="n">
+        <v>43846</v>
+      </c>
+      <c r="G12" s="37" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H12" s="36" t="n">
+        <v>43846</v>
+      </c>
+      <c r="I12" s="37" t="n">
+        <v>0.743055555555556</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="40" t="n">
+        <v>33.58</v>
+      </c>
+      <c r="M12" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="36">
-        <v>43846</v>
-      </c>
-      <c r="G12" s="37">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="H12" s="36">
-        <v>43846</v>
-      </c>
-      <c r="I12" s="37">
-        <v>0.74305555555555602</v>
-      </c>
-      <c r="J12" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="40">
-        <v>33.58</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="N12" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="52" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="16.5" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="43.6640625" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="43.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3286,7 +3131,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3318,7 +3163,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3350,7 +3195,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3384,12 +3229,12 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -3420,7 +3265,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3456,7 +3301,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3488,9 +3333,9 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3522,48 +3367,48 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J9" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="26" t="s">
         <v>38</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>35</v>
       </c>
       <c r="L9" s="27" t="s">
         <v>10</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -3583,35 +3428,43 @@
       <c r="AD9" s="14"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="28.5" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" customWidth="1"/>
-    <col min="12" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="48.33203125" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="48.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3647,7 +3500,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3681,7 +3534,7 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
-    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3715,7 +3568,7 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3751,7 +3604,7 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
-    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3787,7 +3640,7 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
-    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3825,7 +3678,7 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
-    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3859,9 +3712,9 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3895,48 +3748,48 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="25" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J9" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="26" t="s">
         <v>38</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>35</v>
       </c>
       <c r="L9" s="30" t="s">
         <v>10</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N9" s="25" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -3958,38 +3811,46 @@
       <c r="AF9" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="11" width="15.5" customWidth="1"/>
-    <col min="12" max="12" width="13.5" customWidth="1"/>
-    <col min="13" max="13" width="19.1640625" customWidth="1"/>
-    <col min="14" max="14" width="50.1640625" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4023,7 +3884,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -4055,7 +3916,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4087,7 +3948,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4121,7 +3982,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4155,9 +4016,9 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
@@ -4191,7 +4052,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4223,9 +4084,9 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4257,48 +4118,48 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J9" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="26" t="s">
         <v>38</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>35</v>
       </c>
       <c r="L9" s="30" t="s">
         <v>10</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="28"/>
@@ -4318,36 +4179,44 @@
       <c r="AD9" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7A879C-62CC-6745-83D4-09C9DF326994}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="40.83203125" customWidth="1"/>
-    <col min="12" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4381,7 +4250,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4412,7 +4281,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4444,7 +4313,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4478,7 +4347,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4512,7 +4381,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4548,7 +4417,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4580,9 +4449,9 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4614,42 +4483,42 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="43" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G9" s="43" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H9" s="43" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J9" s="27" t="s">
         <v>10</v>
       </c>
       <c r="K9" s="44" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L9" s="45" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="M9" s="26"/>
       <c r="N9" s="1"/>
@@ -4670,38 +4539,46 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="38.5" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="40.83203125" customWidth="1"/>
-    <col min="12" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4735,7 +4612,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4766,7 +4643,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4798,7 +4675,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4832,7 +4709,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4866,7 +4743,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4902,7 +4779,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4934,7 +4811,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>70</v>
       </c>
@@ -4968,21 +4845,21 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>73</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>72</v>
       </c>
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
@@ -4991,7 +4868,7 @@
       <c r="J9" s="27"/>
       <c r="K9" s="44"/>
       <c r="L9" s="45" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="M9" s="26"/>
       <c r="N9" s="1"/>
@@ -5012,27 +4889,82 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" width="10.6640625" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.65"/>
   </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
P4-2517 extracts prices from the DB when generating output spreadsheet instead of original prices files. (#145)
* P4-2517 extracts prices from the DB when generating output spreadsheet instead of original prices files.
* P4-2517 applying sorting by location names to the outputted prices.
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonnycavell/p/calculate-people-move-prices/src/main/resources/spreadsheets/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85A24CD-E0EF-2847-90F8-8FB012E9B092}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26800" windowHeight="17500" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Standard" sheetId="2" r:id="rId2"/>
-    <sheet name="Long haul" sheetId="3" r:id="rId3"/>
-    <sheet name="Redirections" sheetId="4" r:id="rId4"/>
-    <sheet name="Lockouts" sheetId="5" r:id="rId5"/>
-    <sheet name="Multi-type" sheetId="6" r:id="rId6"/>
-    <sheet name="Cancelled" sheetId="9" r:id="rId7"/>
-    <sheet name="Journeys" sheetId="7" r:id="rId8"/>
-    <sheet name="JPC Price book" sheetId="8" r:id="rId9"/>
+    <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Standard" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Long haul" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Redirections" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Lockouts" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Multi-type" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Cancelled" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Journeys" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="JPC Price book" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -33,81 +28,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
-  <si>
-    <t>Export date</t>
-  </si>
-  <si>
-    <t>Calculate Journey Variable Payments (S2B)</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
-  <si>
-    <t>Date Range</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>OUTPUT SUMMARY</t>
-  </si>
-  <si>
-    <t>Move type</t>
-  </si>
-  <si>
-    <t>Percentage</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="74">
+  <si>
+    <t xml:space="preserve">Export date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate Journey Variable Payments (S2B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTPUT SUMMARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage</t>
   </si>
   <si>
     <t xml:space="preserve"> Move volume</t>
   </si>
   <si>
-    <t>Move volume without prices</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Standard move</t>
-  </si>
-  <si>
-    <t>includes single journeys, cross supplier and redirects before the move has started</t>
+    <t xml:space="preserve">Move volume without prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes single journeys, cross supplier and redirects before the move has started</t>
   </si>
   <si>
     <t xml:space="preserve">Long haul </t>
   </si>
   <si>
-    <t>a completed move made up of 2 or more journeys</t>
-  </si>
-  <si>
-    <t>Redirections</t>
-  </si>
-  <si>
-    <t>a redirection after the move has started</t>
-  </si>
-  <si>
-    <t>Lockouts</t>
-  </si>
-  <si>
-    <t>refused admission to prison</t>
-  </si>
-  <si>
-    <t>Multi-type moves</t>
-  </si>
-  <si>
-    <t>includes combinations of the above</t>
-  </si>
-  <si>
-    <t>Total %</t>
-  </si>
-  <si>
-    <t>Total volume</t>
-  </si>
-  <si>
-    <t>Total volume without prices</t>
-  </si>
-  <si>
-    <t>Total Price</t>
+    <t xml:space="preserve">a completed move made up of 2 or more journeys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redirections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a redirection after the move has started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lockouts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refused admission to prison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-type moves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes combinations of the above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancelled moves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prison to prison moves cancelled by PMU later than </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3pm the day before the move date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total volume without prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Price</t>
   </si>
   <si>
     <r>
@@ -122,104 +126,104 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(includes single journeys, cross supplier and redirects before the move has started)</t>
+      <t xml:space="preserve">(includes single journeys, cross supplier and redirects before the move has started)</t>
     </r>
   </si>
   <si>
-    <t>Move Ref ID</t>
-  </si>
-  <si>
-    <t>Pick up</t>
-  </si>
-  <si>
-    <t>Location Type</t>
-  </si>
-  <si>
-    <t>Drop off</t>
-  </si>
-  <si>
-    <t>Pick up date</t>
-  </si>
-  <si>
-    <t>Pick up time</t>
-  </si>
-  <si>
-    <t>Drop off date</t>
-  </si>
-  <si>
-    <t>Drop off time</t>
+    <t xml:space="preserve">Move Ref ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off time</t>
   </si>
   <si>
     <t xml:space="preserve">Vehicle Reg </t>
   </si>
   <si>
-    <t>NOMIS Prison ID</t>
-  </si>
-  <si>
-    <t>LONG HAUL</t>
-  </si>
-  <si>
-    <t>Move ID</t>
-  </si>
-  <si>
-    <t>Vehicle Reg</t>
-  </si>
-  <si>
-    <t>Billable?</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>MX1234</t>
-  </si>
-  <si>
-    <t>BRADFORD POLICE STATION (TRAFALGAR HOUSE)</t>
-  </si>
-  <si>
-    <t>LEEDS MAGISTRATES COURT</t>
-  </si>
-  <si>
-    <t>XXX9876</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>Journey 1</t>
-  </si>
-  <si>
-    <t>PS</t>
-  </si>
-  <si>
-    <t>DERBY POLICE CUSTODY</t>
-  </si>
-  <si>
-    <t>GD-5555</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>Long journey, ovenight stay.</t>
-  </si>
-  <si>
-    <t>Journey 2</t>
-  </si>
-  <si>
-    <t>MC</t>
-  </si>
-  <si>
-    <t>XX-5786</t>
-  </si>
-  <si>
-    <t>SERCO</t>
+    <t xml:space="preserve">NOMIS Prison ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LONG HAUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billable?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MX1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRADFORD POLICE STATION (TRAFALGAR HOUSE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEEDS MAGISTRATES COURT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XXX9876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journey 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DERBY POLICE CUSTODY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GD-5555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long journey, ovenight stay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journey 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XX-5786</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERCO</t>
   </si>
   <si>
     <r>
@@ -234,20 +238,20 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(a redirection after the move has started)</t>
+      <t xml:space="preserve">(a redirection after the move has started)</t>
     </r>
   </si>
   <si>
-    <t>Contractor Billable?</t>
-  </si>
-  <si>
-    <t>Notes (Reason codes or supplier notes)</t>
+    <t xml:space="preserve">Contractor Billable?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes (Reason codes or supplier notes)</t>
   </si>
   <si>
     <r>
@@ -262,17 +266,17 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="9"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(refused admission to prison)</t>
+      <t xml:space="preserve">(refused admission to prison)</t>
     </r>
   </si>
   <si>
-    <t>Date range</t>
+    <t xml:space="preserve">Date range</t>
   </si>
   <si>
     <r>
@@ -283,11 +287,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>MULTI-TYPE MOVES</t>
+      <t xml:space="preserve">MULTI-TYPE MOVES</t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -309,62 +313,74 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(includes prison to prison transfer moves that have been cancelled by the population mangement unit after 3pm on the day before the move)</t>
+      <t xml:space="preserve">(includes prison to prison transfer moves that have been cancelled by the population mangement unit after 3pm on the day before the move)</t>
     </r>
   </si>
   <si>
-    <t>Move date</t>
-  </si>
-  <si>
-    <t>Cancellation date</t>
-  </si>
-  <si>
-    <t>Cancellation time</t>
-  </si>
-  <si>
-    <t>Dev notes:</t>
-  </si>
-  <si>
-    <t>3pm the day before the move date</t>
-  </si>
-  <si>
-    <t>Cancelled moves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prison to prison moves cancelled by PMU later than </t>
-  </si>
-  <si>
-    <t>TOTAL VOLUME BY LOCATION</t>
-  </si>
-  <si>
-    <t>Unit price</t>
-  </si>
-  <si>
-    <t>Total price</t>
-  </si>
-  <si>
-    <t>Total journey count</t>
+    <t xml:space="preserve">Move date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancellation date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancellation time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev notes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL VOLUME BY LOCATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total journey count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="\£#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="0%"/>
+    <numFmt numFmtId="167" formatCode="#,##0"/>
+    <numFmt numFmtId="168" formatCode="\£#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="HH:MM"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -374,7 +390,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -382,7 +398,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -390,14 +406,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -410,7 +426,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -480,7 +496,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -488,112 +504,225 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="46">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -652,340 +781,32 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +837,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1044,7 +865,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
     </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1072,7 +893,7 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1102,7 +923,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
     </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1132,7 +953,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1164,7 +985,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1193,7 +1014,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -1224,7 +1045,7 @@
       <c r="Z8" s="9"/>
       <c r="AA8" s="9"/>
     </row>
-    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
@@ -1263,7 +1084,7 @@
       <c r="Z9" s="13"/>
       <c r="AA9" s="13"/>
     </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
         <v>11</v>
       </c>
@@ -1294,7 +1115,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
         <v>12</v>
       </c>
@@ -1325,7 +1146,7 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="18"/>
@@ -1354,7 +1175,7 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="s">
         <v>13</v>
       </c>
@@ -1385,7 +1206,7 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
         <v>14</v>
       </c>
@@ -1412,7 +1233,7 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="17"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1441,7 +1262,7 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
@@ -1472,7 +1293,7 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
         <v>16</v>
       </c>
@@ -1503,7 +1324,7 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1532,7 +1353,7 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="s">
         <v>17</v>
       </c>
@@ -1563,7 +1384,7 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="17" t="s">
         <v>18</v>
       </c>
@@ -1594,7 +1415,7 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1623,7 +1444,7 @@
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
         <v>19</v>
       </c>
@@ -1654,7 +1475,7 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="17" t="s">
         <v>20</v>
       </c>
@@ -1685,7 +1506,7 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1714,9 +1535,9 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1745,9 +1566,9 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="17" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1776,9 +1597,9 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="17" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1807,19 +1628,19 @@
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
     </row>
-    <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="22"/>
       <c r="B28" s="23" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1844,7 +1665,7 @@
       <c r="Z28" s="4"/>
       <c r="AA28" s="4"/>
     </row>
-    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1873,7 +1694,7 @@
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
       <c r="B30" s="20"/>
       <c r="C30" s="1"/>
@@ -1902,7 +1723,7 @@
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1932,33 +1753,41 @@
       <c r="AA31" s="24"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="19.5" customWidth="1"/>
-    <col min="11" max="11" width="15.5" customWidth="1"/>
-    <col min="12" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1994,7 +1823,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2028,7 +1857,7 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
-    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2062,7 +1891,7 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -2098,7 +1927,7 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
-    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2134,7 +1963,7 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
-    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2172,7 +2001,7 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
-    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2206,9 +2035,9 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2242,39 +2071,39 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="L9" s="27" t="s">
         <v>10</v>
@@ -2300,7 +2129,7 @@
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
     </row>
-    <row r="10" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2334,7 +2163,7 @@
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
     </row>
-    <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2368,7 +2197,7 @@
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
     </row>
-    <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2402,7 +2231,7 @@
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
     </row>
-    <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2436,7 +2265,7 @@
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
     </row>
-    <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2470,7 +2299,7 @@
       <c r="AE14" s="28"/>
       <c r="AF14" s="28"/>
     </row>
-    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2504,7 +2333,7 @@
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
     </row>
-    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2538,7 +2367,7 @@
       <c r="AE16" s="28"/>
       <c r="AF16" s="28"/>
     </row>
-    <row r="17" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2572,7 +2401,7 @@
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
     </row>
-    <row r="18" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2606,7 +2435,7 @@
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
     </row>
-    <row r="19" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2640,7 +2469,7 @@
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
     </row>
-    <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2674,7 +2503,7 @@
       <c r="AE20" s="28"/>
       <c r="AF20" s="28"/>
     </row>
-    <row r="21" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2708,7 +2537,7 @@
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
     </row>
-    <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2742,7 +2571,7 @@
       <c r="AE22" s="28"/>
       <c r="AF22" s="28"/>
     </row>
-    <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2776,7 +2605,7 @@
       <c r="AE23" s="28"/>
       <c r="AF23" s="28"/>
     </row>
-    <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2810,7 +2639,7 @@
       <c r="AE24" s="28"/>
       <c r="AF24" s="28"/>
     </row>
-    <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2844,7 +2673,7 @@
       <c r="AE25" s="28"/>
       <c r="AF25" s="28"/>
     </row>
-    <row r="26" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2879,38 +2708,46 @@
       <c r="AF26" s="28"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" customWidth="1"/>
-    <col min="12" max="12" width="10.1640625" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="50" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2928,7 +2765,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -2944,7 +2781,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
@@ -2960,7 +2797,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -2978,7 +2815,7 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2996,7 +2833,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3016,7 +2853,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3032,9 +2869,9 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3050,48 +2887,48 @@
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J9" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="26" t="s">
         <v>38</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>35</v>
       </c>
       <c r="L9" s="27" t="s">
         <v>10</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="O9" s="31"/>
       <c r="P9" s="31"/>
@@ -3106,153 +2943,161 @@
       <c r="Y9" s="31"/>
       <c r="Z9" s="31"/>
     </row>
-    <row r="10" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="10" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="32">
+      <c r="F10" s="32" t="n">
         <v>43845</v>
       </c>
-      <c r="G10" s="33">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="H10" s="32">
+      <c r="G10" s="33" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H10" s="32" t="n">
         <v>43846</v>
       </c>
-      <c r="I10" s="33">
-        <v>0.74305555555555602</v>
+      <c r="I10" s="33" t="n">
+        <v>0.743055555555556</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="34" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L10" s="35" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="11" customFormat="false" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="36">
+        <v>50</v>
+      </c>
+      <c r="F11" s="36" t="n">
         <v>43845</v>
       </c>
-      <c r="G11" s="37">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="H11" s="36">
+      <c r="G11" s="37" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H11" s="36" t="n">
         <v>43845</v>
       </c>
-      <c r="I11" s="37">
-        <v>0.60416666666666696</v>
+      <c r="I11" s="37" t="n">
+        <v>0.604166666666667</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="39" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="M11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="36" t="n">
+        <v>43846</v>
+      </c>
+      <c r="G12" s="37" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H12" s="36" t="n">
+        <v>43846</v>
+      </c>
+      <c r="I12" s="37" t="n">
+        <v>0.743055555555556</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="40" t="n">
+        <v>33.58</v>
+      </c>
+      <c r="M12" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="36">
-        <v>43846</v>
-      </c>
-      <c r="G12" s="37">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="H12" s="36">
-        <v>43846</v>
-      </c>
-      <c r="I12" s="37">
-        <v>0.74305555555555602</v>
-      </c>
-      <c r="J12" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="40">
-        <v>33.58</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="N12" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="52" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="16.5" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="43.6640625" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="43.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3286,7 +3131,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3318,7 +3163,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3350,7 +3195,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3384,12 +3229,12 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -3420,7 +3265,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3456,7 +3301,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3488,9 +3333,9 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3522,48 +3367,48 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J9" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="26" t="s">
         <v>38</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>35</v>
       </c>
       <c r="L9" s="27" t="s">
         <v>10</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -3583,35 +3428,43 @@
       <c r="AD9" s="14"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="28.5" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" customWidth="1"/>
-    <col min="12" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="48.33203125" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="48.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3647,7 +3500,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3681,7 +3534,7 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
-    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3715,7 +3568,7 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3751,7 +3604,7 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
-    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3787,7 +3640,7 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
-    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3825,7 +3678,7 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
-    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3859,9 +3712,9 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3895,48 +3748,48 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="25" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J9" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="26" t="s">
         <v>38</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>35</v>
       </c>
       <c r="L9" s="30" t="s">
         <v>10</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N9" s="25" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -3958,38 +3811,46 @@
       <c r="AF9" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="11" width="15.5" customWidth="1"/>
-    <col min="12" max="12" width="13.5" customWidth="1"/>
-    <col min="13" max="13" width="19.1640625" customWidth="1"/>
-    <col min="14" max="14" width="50.1640625" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4023,7 +3884,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -4055,7 +3916,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4087,7 +3948,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4121,7 +3982,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4155,9 +4016,9 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
@@ -4191,7 +4052,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4223,9 +4084,9 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4257,48 +4118,48 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J9" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="26" t="s">
         <v>38</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>35</v>
       </c>
       <c r="L9" s="30" t="s">
         <v>10</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="28"/>
@@ -4318,36 +4179,44 @@
       <c r="AD9" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7A879C-62CC-6745-83D4-09C9DF326994}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="40.83203125" customWidth="1"/>
-    <col min="12" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4381,7 +4250,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4412,7 +4281,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4444,7 +4313,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4478,7 +4347,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4512,7 +4381,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4548,7 +4417,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4580,9 +4449,9 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4614,42 +4483,42 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="43" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G9" s="43" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H9" s="43" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J9" s="27" t="s">
         <v>10</v>
       </c>
       <c r="K9" s="44" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L9" s="45" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="M9" s="26"/>
       <c r="N9" s="1"/>
@@ -4670,38 +4539,46 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="38.5" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="40.83203125" customWidth="1"/>
-    <col min="12" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4735,7 +4612,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4766,7 +4643,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4798,7 +4675,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4832,7 +4709,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4866,7 +4743,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4902,7 +4779,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4934,7 +4811,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>70</v>
       </c>
@@ -4968,21 +4845,21 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>73</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>72</v>
       </c>
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
@@ -4991,7 +4868,7 @@
       <c r="J9" s="27"/>
       <c r="K9" s="44"/>
       <c r="L9" s="45" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="M9" s="26"/>
       <c r="N9" s="1"/>
@@ -5012,27 +4889,82 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" width="10.6640625" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.65"/>
   </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
P4-2551 Fix Spreadsheet issue
Fix the amount of time it takes to download the spreadsheet.
Do not create CellStyles at run-time; instead create the ones we need once
Create CellStyle once for each color / format combination.

Remove limit from queries so all moves are shown

Remove developer notes from Excel Template

Ensure template is saved on summary view
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonnycavell/p/calculate-people-move-prices/src/main/resources/spreadsheets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE3C0F6-E4AA-184B-A880-B634A104D96D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33000" windowHeight="19680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Standard" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Long haul" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Redirections" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Lockouts" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Multi-type" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Cancelled" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Journeys" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="JPC Price book" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Standard" sheetId="2" r:id="rId2"/>
+    <sheet name="Long haul" sheetId="3" r:id="rId3"/>
+    <sheet name="Redirections" sheetId="4" r:id="rId4"/>
+    <sheet name="Lockouts" sheetId="5" r:id="rId5"/>
+    <sheet name="Multi-type" sheetId="6" r:id="rId6"/>
+    <sheet name="Cancelled" sheetId="7" r:id="rId7"/>
+    <sheet name="Journeys" sheetId="8" r:id="rId8"/>
+    <sheet name="JPC Price book" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,90 +33,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="74">
-  <si>
-    <t xml:space="preserve">Export date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculate Journey Variable Payments (S2B)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date Range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUTPUT SUMMARY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="73">
+  <si>
+    <t>Export date</t>
+  </si>
+  <si>
+    <t>Calculate Journey Variable Payments (S2B)</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Date Range</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>OUTPUT SUMMARY</t>
+  </si>
+  <si>
+    <t>Move type</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
   <si>
     <t xml:space="preserve"> Move volume</t>
   </si>
   <si>
-    <t xml:space="preserve">Move volume without prices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard move</t>
-  </si>
-  <si>
-    <t xml:space="preserve">includes single journeys, cross supplier and redirects before the move has started</t>
+    <t>Move volume without prices</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Standard move</t>
+  </si>
+  <si>
+    <t>includes single journeys, cross supplier and redirects before the move has started</t>
   </si>
   <si>
     <t xml:space="preserve">Long haul </t>
   </si>
   <si>
-    <t xml:space="preserve">a completed move made up of 2 or more journeys</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redirections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a redirection after the move has started</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lockouts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">refused admission to prison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-type moves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">includes combinations of the above</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancelled moves</t>
+    <t>a completed move made up of 2 or more journeys</t>
+  </si>
+  <si>
+    <t>Redirections</t>
+  </si>
+  <si>
+    <t>a redirection after the move has started</t>
+  </si>
+  <si>
+    <t>Lockouts</t>
+  </si>
+  <si>
+    <t>refused admission to prison</t>
+  </si>
+  <si>
+    <t>Multi-type moves</t>
+  </si>
+  <si>
+    <t>includes combinations of the above</t>
+  </si>
+  <si>
+    <t>Cancelled moves</t>
   </si>
   <si>
     <t xml:space="preserve">prison to prison moves cancelled by PMU later than </t>
   </si>
   <si>
-    <t xml:space="preserve">3pm the day before the move date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total volume without prices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Price</t>
+    <t>3pm the day before the move date</t>
+  </si>
+  <si>
+    <t>Total %</t>
+  </si>
+  <si>
+    <t>Total volume</t>
+  </si>
+  <si>
+    <t>Total volume without prices</t>
+  </si>
+  <si>
+    <t>Total Price</t>
   </si>
   <si>
     <r>
@@ -126,104 +131,104 @@
     </r>
     <r>
       <rPr>
-        <i val="true"/>
+        <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(includes single journeys, cross supplier and redirects before the move has started)</t>
+      <t>(includes single journeys, cross supplier and redirects before the move has started)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Move Ref ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pick up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drop off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pick up date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pick up time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drop off date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drop off time</t>
+    <t>Move Ref ID</t>
+  </si>
+  <si>
+    <t>Pick up</t>
+  </si>
+  <si>
+    <t>Location Type</t>
+  </si>
+  <si>
+    <t>Drop off</t>
+  </si>
+  <si>
+    <t>Pick up date</t>
+  </si>
+  <si>
+    <t>Pick up time</t>
+  </si>
+  <si>
+    <t>Drop off date</t>
+  </si>
+  <si>
+    <t>Drop off time</t>
   </si>
   <si>
     <t xml:space="preserve">Vehicle Reg </t>
   </si>
   <si>
-    <t xml:space="preserve">NOMIS Prison ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LONG HAUL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vehicle Reg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billable?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MX1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRADFORD POLICE STATION (TRAFALGAR HOUSE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEEDS MAGISTRATES COURT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XXX9876</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Journey 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DERBY POLICE CUSTODY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GD-5555</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Long journey, ovenight stay.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Journey 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XX-5786</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SERCO</t>
+    <t>NOMIS Prison ID</t>
+  </si>
+  <si>
+    <t>LONG HAUL</t>
+  </si>
+  <si>
+    <t>Move ID</t>
+  </si>
+  <si>
+    <t>Vehicle Reg</t>
+  </si>
+  <si>
+    <t>Billable?</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>MX1234</t>
+  </si>
+  <si>
+    <t>BRADFORD POLICE STATION (TRAFALGAR HOUSE)</t>
+  </si>
+  <si>
+    <t>LEEDS MAGISTRATES COURT</t>
+  </si>
+  <si>
+    <t>XXX9876</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Journey 1</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>DERBY POLICE CUSTODY</t>
+  </si>
+  <si>
+    <t>GD-5555</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Long journey, ovenight stay.</t>
+  </si>
+  <si>
+    <t>Journey 2</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>XX-5786</t>
+  </si>
+  <si>
+    <t>SERCO</t>
   </si>
   <si>
     <r>
@@ -238,20 +243,20 @@
     </r>
     <r>
       <rPr>
-        <i val="true"/>
+        <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(a redirection after the move has started)</t>
+      <t>(a redirection after the move has started)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Contractor Billable?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes (Reason codes or supplier notes)</t>
+    <t>Contractor Billable?</t>
+  </si>
+  <si>
+    <t>Notes (Reason codes or supplier notes)</t>
   </si>
   <si>
     <r>
@@ -266,17 +271,17 @@
     </r>
     <r>
       <rPr>
-        <i val="true"/>
+        <i/>
         <sz val="9"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(refused admission to prison)</t>
+      <t>(refused admission to prison)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Date range</t>
+    <t>Date range</t>
   </si>
   <si>
     <r>
@@ -287,11 +292,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">MULTI-TYPE MOVES</t>
+      <t>MULTI-TYPE MOVES</t>
     </r>
     <r>
       <rPr>
-        <i val="true"/>
+        <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -313,74 +318,50 @@
     </r>
     <r>
       <rPr>
-        <i val="true"/>
+        <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(includes prison to prison transfer moves that have been cancelled by the population mangement unit after 3pm on the day before the move)</t>
+      <t>(includes prison to prison transfer moves that have been cancelled by the population mangement unit after 3pm on the day before the move)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Move date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancellation date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancellation time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dev notes:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTAL VOLUME BY LOCATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total journey count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total price</t>
+    <t>Move date</t>
+  </si>
+  <si>
+    <t>Cancellation date</t>
+  </si>
+  <si>
+    <t>Cancellation time</t>
+  </si>
+  <si>
+    <t>TOTAL VOLUME BY LOCATION</t>
+  </si>
+  <si>
+    <t>Total journey count</t>
+  </si>
+  <si>
+    <t>Unit price</t>
+  </si>
+  <si>
+    <t>Total price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="0%"/>
-    <numFmt numFmtId="167" formatCode="#,##0"/>
-    <numFmt numFmtId="168" formatCode="\£#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="HH:MM"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="\£#,##0.00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -390,7 +371,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -398,7 +379,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -406,14 +387,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -426,14 +407,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -488,15 +469,9 @@
         <bgColor rgb="FF800000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -504,225 +479,113 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="46">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="20" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -781,32 +644,340 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.5"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,7 +1008,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -865,7 +1036,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -893,7 +1064,7 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -923,7 +1094,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -953,7 +1124,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -985,7 +1156,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1014,7 +1185,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -1045,7 +1216,7 @@
       <c r="Z8" s="9"/>
       <c r="AA8" s="9"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
@@ -1084,14 +1255,14 @@
       <c r="Z9" s="13"/>
       <c r="AA9" s="13"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="43"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1115,14 +1286,14 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
+    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1146,12 +1317,12 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1175,14 +1346,14 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="1"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="43"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1206,10 +1377,14 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
+      <c r="B14" s="48"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1233,12 +1408,12 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="15"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1262,14 +1437,14 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="1"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1293,14 +1468,14 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
+    <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1324,12 +1499,12 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1353,14 +1528,14 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="43"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1384,14 +1559,14 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="17" t="s">
+    <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1415,12 +1590,12 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="19"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1444,14 +1619,14 @@
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="1"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1475,14 +1650,14 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="17" t="s">
+    <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1506,12 +1681,12 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1535,14 +1710,14 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1566,14 +1741,14 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1597,14 +1772,14 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="17" t="s">
+    <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1628,18 +1803,18 @@
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="22"/>
-      <c r="B28" s="23" t="s">
+    <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="19"/>
+      <c r="B28" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="20" t="s">
         <v>27</v>
       </c>
       <c r="F28" s="4"/>
@@ -1665,9 +1840,9 @@
       <c r="Z28" s="4"/>
       <c r="AA28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1694,9 +1869,9 @@
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
-      <c r="B30" s="20"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1723,7 +1898,7 @@
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1750,44 +1925,34 @@
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
-      <c r="AA31" s="24"/>
+      <c r="AA31" s="21"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="19.5" customWidth="1"/>
+    <col min="11" max="11" width="15.5" customWidth="1"/>
+    <col min="12" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1823,7 +1988,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1857,7 +2022,7 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1891,7 +2056,7 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1927,7 +2092,7 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1963,7 +2128,7 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2001,7 +2166,7 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2035,7 +2200,7 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
@@ -2071,7 +2236,7 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>29</v>
       </c>
@@ -2087,30 +2252,30 @@
       <c r="E9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="26"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="26"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="23"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -2129,7 +2294,7 @@
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2163,7 +2328,7 @@
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2197,12 +2362,12 @@
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -2231,7 +2396,7 @@
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2265,7 +2430,7 @@
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2296,10 +2461,10 @@
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
-      <c r="AE14" s="28"/>
-      <c r="AF14" s="28"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE14" s="25"/>
+      <c r="AF14" s="25"/>
+    </row>
+    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2333,7 +2498,7 @@
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2364,10 +2529,10 @@
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
-      <c r="AE16" s="28"/>
-      <c r="AF16" s="28"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE16" s="25"/>
+      <c r="AF16" s="25"/>
+    </row>
+    <row r="17" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2401,7 +2566,7 @@
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2435,7 +2600,7 @@
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2469,7 +2634,7 @@
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2500,10 +2665,10 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
-      <c r="AE20" s="28"/>
-      <c r="AF20" s="28"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE20" s="25"/>
+      <c r="AF20" s="25"/>
+    </row>
+    <row r="21" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2537,7 +2702,7 @@
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2568,10 +2733,10 @@
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
-      <c r="AE22" s="28"/>
-      <c r="AF22" s="28"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE22" s="25"/>
+      <c r="AF22" s="25"/>
+    </row>
+    <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2602,10 +2767,10 @@
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
-      <c r="AE23" s="28"/>
-      <c r="AF23" s="28"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE23" s="25"/>
+      <c r="AF23" s="25"/>
+    </row>
+    <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2636,10 +2801,10 @@
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
-      <c r="AE24" s="28"/>
-      <c r="AF24" s="28"/>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE24" s="25"/>
+      <c r="AF24" s="25"/>
+    </row>
+    <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2670,10 +2835,10 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
-      <c r="AE25" s="28"/>
-      <c r="AF25" s="28"/>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE25" s="25"/>
+      <c r="AF25" s="25"/>
+    </row>
+    <row r="26" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2704,55 +2869,47 @@
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
-      <c r="AE26" s="28"/>
-      <c r="AF26" s="28"/>
+      <c r="AE26" s="25"/>
+      <c r="AF26" s="25"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="5" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="50" customWidth="1"/>
+    <col min="15" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="29"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2765,10 +2922,10 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2781,10 +2938,10 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -2797,7 +2954,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -2815,7 +2972,7 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2833,7 +2990,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2853,7 +3010,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2869,7 +3026,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
@@ -2887,20 +3044,20 @@
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="22" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="22" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -2915,35 +3072,35 @@
       <c r="I9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="27" t="s">
         <v>42</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="31"/>
-      <c r="V9" s="31"/>
-      <c r="W9" s="31"/>
-      <c r="X9" s="31"/>
-      <c r="Y9" s="31"/>
-      <c r="Z9" s="31"/>
-    </row>
-    <row r="10" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28"/>
+    </row>
+    <row r="10" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13" t="s">
         <v>44</v>
       </c>
@@ -2955,29 +3112,29 @@
         <v>46</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="32" t="n">
+      <c r="F10" s="29">
         <v>43845</v>
       </c>
-      <c r="G10" s="33" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="H10" s="32" t="n">
+      <c r="G10" s="30">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H10" s="29">
         <v>43846</v>
       </c>
-      <c r="I10" s="33" t="n">
-        <v>0.743055555555556</v>
+      <c r="I10" s="30">
+        <v>0.74305555555555602</v>
       </c>
       <c r="J10" s="13"/>
-      <c r="K10" s="34" t="s">
+      <c r="K10" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="L10" s="32" t="s">
         <v>48</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:26" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -2993,23 +3150,23 @@
       <c r="E11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="36" t="n">
+      <c r="F11" s="33">
         <v>43845</v>
       </c>
-      <c r="G11" s="37" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="H11" s="36" t="n">
+      <c r="G11" s="34">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H11" s="33">
         <v>43845</v>
       </c>
-      <c r="I11" s="37" t="n">
-        <v>0.604166666666667</v>
-      </c>
-      <c r="J11" s="38" t="s">
+      <c r="I11" s="34">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="J11" s="35" t="s">
         <v>52</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="39" t="s">
+      <c r="L11" s="36" t="s">
         <v>48</v>
       </c>
       <c r="M11" s="8" t="s">
@@ -3019,7 +3176,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:26" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -3035,23 +3192,23 @@
       <c r="E12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="36" t="n">
+      <c r="F12" s="33">
         <v>43846</v>
       </c>
-      <c r="G12" s="37" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="H12" s="36" t="n">
+      <c r="G12" s="34">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H12" s="33">
         <v>43846</v>
       </c>
-      <c r="I12" s="37" t="n">
-        <v>0.743055555555556</v>
-      </c>
-      <c r="J12" s="38" t="s">
+      <c r="I12" s="34">
+        <v>0.74305555555555602</v>
+      </c>
+      <c r="J12" s="35" t="s">
         <v>57</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="L12" s="40" t="n">
+      <c r="L12" s="37">
         <v>33.58</v>
       </c>
       <c r="M12" s="8" t="s">
@@ -3060,44 +3217,36 @@
       <c r="N12" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="43.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="52" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="43.6640625" customWidth="1"/>
+    <col min="15" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3131,7 +3280,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3163,7 +3312,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3195,7 +3344,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3229,7 +3378,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3265,7 +3414,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3301,7 +3450,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3333,7 +3482,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>59</v>
       </c>
@@ -3367,20 +3516,20 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="22" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="22" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -3395,16 +3544,16 @@
       <c r="I9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="27" t="s">
         <v>60</v>
       </c>
       <c r="N9" s="14" t="s">
@@ -3428,43 +3577,35 @@
       <c r="AD9" s="14"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="48.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="28.5" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+    <col min="12" max="13" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="48.33203125" customWidth="1"/>
+    <col min="15" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3500,7 +3641,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3534,7 +3675,7 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3568,7 +3709,7 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3584,7 +3725,7 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
-      <c r="N4" s="22"/>
+      <c r="N4" s="19"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -3604,7 +3745,7 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3640,7 +3781,7 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3678,7 +3819,7 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3712,7 +3853,7 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>62</v>
       </c>
@@ -3728,7 +3869,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-      <c r="N8" s="22"/>
+      <c r="N8" s="19"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -3748,47 +3889,47 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="25" t="s">
+      <c r="N9" s="22" t="s">
         <v>43</v>
       </c>
       <c r="O9" s="1"/>
@@ -3811,46 +3952,38 @@
       <c r="AF9" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="15.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="66.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="11" width="15.5" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" customWidth="1"/>
+    <col min="14" max="14" width="50.1640625" customWidth="1"/>
+    <col min="15" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3884,7 +4017,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3916,7 +4049,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3948,7 +4081,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3982,7 +4115,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4016,7 +4149,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>63</v>
       </c>
@@ -4052,7 +4185,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4084,7 +4217,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>64</v>
       </c>
@@ -4118,51 +4251,51 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="27" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="27" t="s">
         <v>60</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>43</v>
       </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="28"/>
+      <c r="P9" s="25"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -4179,48 +4312,40 @@
       <c r="AD9" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="40.83203125" customWidth="1"/>
+    <col min="12" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="38"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4250,7 +4375,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4281,7 +4406,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4313,7 +4438,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4326,7 +4451,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="42"/>
+      <c r="K4" s="39"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -4347,7 +4472,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4381,7 +4506,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4417,7 +4542,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4449,7 +4574,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>65</v>
       </c>
@@ -4462,7 +4587,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="42"/>
+      <c r="K8" s="39"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -4483,7 +4608,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>29</v>
       </c>
@@ -4499,28 +4624,26 @@
       <c r="E9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="43" t="s">
+      <c r="H9" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="44" t="s">
+      <c r="K9" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="M9" s="26"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="23"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -4539,50 +4662,42 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="40.83203125" customWidth="1"/>
+    <col min="12" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="38"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4612,7 +4727,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4643,7 +4758,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4675,7 +4790,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4688,7 +4803,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="42"/>
+      <c r="K4" s="39"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -4709,7 +4824,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4743,7 +4858,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4779,7 +4894,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4811,9 +4926,9 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4824,7 +4939,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="42"/>
+      <c r="K8" s="39"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -4845,7 +4960,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>30</v>
       </c>
@@ -4853,24 +4968,22 @@
         <v>32</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="M9" s="26"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="23"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -4889,66 +5002,62 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.65"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="38.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43.1640625" customWidth="1"/>
+    <col min="5" max="1025" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4959,12 +5068,7 @@
       <c r="D6" s="7"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
P4-2551 Fix Spreadsheet issue (#151)
Fix the amount of time it takes to download the spreadsheet.
Do not create CellStyles at run-time; instead create the ones we need once
Create CellStyle once for each color / format combination.

Remove limit from queries so all moves are shown

Remove developer notes from Excel Template

Ensure template is saved on summary view
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonnycavell/p/calculate-people-move-prices/src/main/resources/spreadsheets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE3C0F6-E4AA-184B-A880-B634A104D96D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33000" windowHeight="19680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Standard" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Long haul" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Redirections" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Lockouts" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Multi-type" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Cancelled" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Journeys" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="JPC Price book" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Standard" sheetId="2" r:id="rId2"/>
+    <sheet name="Long haul" sheetId="3" r:id="rId3"/>
+    <sheet name="Redirections" sheetId="4" r:id="rId4"/>
+    <sheet name="Lockouts" sheetId="5" r:id="rId5"/>
+    <sheet name="Multi-type" sheetId="6" r:id="rId6"/>
+    <sheet name="Cancelled" sheetId="7" r:id="rId7"/>
+    <sheet name="Journeys" sheetId="8" r:id="rId8"/>
+    <sheet name="JPC Price book" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,90 +33,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="74">
-  <si>
-    <t xml:space="preserve">Export date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculate Journey Variable Payments (S2B)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date Range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUTPUT SUMMARY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="73">
+  <si>
+    <t>Export date</t>
+  </si>
+  <si>
+    <t>Calculate Journey Variable Payments (S2B)</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Date Range</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>OUTPUT SUMMARY</t>
+  </si>
+  <si>
+    <t>Move type</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
   <si>
     <t xml:space="preserve"> Move volume</t>
   </si>
   <si>
-    <t xml:space="preserve">Move volume without prices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard move</t>
-  </si>
-  <si>
-    <t xml:space="preserve">includes single journeys, cross supplier and redirects before the move has started</t>
+    <t>Move volume without prices</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Standard move</t>
+  </si>
+  <si>
+    <t>includes single journeys, cross supplier and redirects before the move has started</t>
   </si>
   <si>
     <t xml:space="preserve">Long haul </t>
   </si>
   <si>
-    <t xml:space="preserve">a completed move made up of 2 or more journeys</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redirections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a redirection after the move has started</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lockouts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">refused admission to prison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-type moves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">includes combinations of the above</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancelled moves</t>
+    <t>a completed move made up of 2 or more journeys</t>
+  </si>
+  <si>
+    <t>Redirections</t>
+  </si>
+  <si>
+    <t>a redirection after the move has started</t>
+  </si>
+  <si>
+    <t>Lockouts</t>
+  </si>
+  <si>
+    <t>refused admission to prison</t>
+  </si>
+  <si>
+    <t>Multi-type moves</t>
+  </si>
+  <si>
+    <t>includes combinations of the above</t>
+  </si>
+  <si>
+    <t>Cancelled moves</t>
   </si>
   <si>
     <t xml:space="preserve">prison to prison moves cancelled by PMU later than </t>
   </si>
   <si>
-    <t xml:space="preserve">3pm the day before the move date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total volume without prices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Price</t>
+    <t>3pm the day before the move date</t>
+  </si>
+  <si>
+    <t>Total %</t>
+  </si>
+  <si>
+    <t>Total volume</t>
+  </si>
+  <si>
+    <t>Total volume without prices</t>
+  </si>
+  <si>
+    <t>Total Price</t>
   </si>
   <si>
     <r>
@@ -126,104 +131,104 @@
     </r>
     <r>
       <rPr>
-        <i val="true"/>
+        <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(includes single journeys, cross supplier and redirects before the move has started)</t>
+      <t>(includes single journeys, cross supplier and redirects before the move has started)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Move Ref ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pick up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drop off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pick up date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pick up time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drop off date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drop off time</t>
+    <t>Move Ref ID</t>
+  </si>
+  <si>
+    <t>Pick up</t>
+  </si>
+  <si>
+    <t>Location Type</t>
+  </si>
+  <si>
+    <t>Drop off</t>
+  </si>
+  <si>
+    <t>Pick up date</t>
+  </si>
+  <si>
+    <t>Pick up time</t>
+  </si>
+  <si>
+    <t>Drop off date</t>
+  </si>
+  <si>
+    <t>Drop off time</t>
   </si>
   <si>
     <t xml:space="preserve">Vehicle Reg </t>
   </si>
   <si>
-    <t xml:space="preserve">NOMIS Prison ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LONG HAUL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vehicle Reg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billable?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MX1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRADFORD POLICE STATION (TRAFALGAR HOUSE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEEDS MAGISTRATES COURT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XXX9876</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Journey 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DERBY POLICE CUSTODY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GD-5555</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Long journey, ovenight stay.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Journey 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XX-5786</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SERCO</t>
+    <t>NOMIS Prison ID</t>
+  </si>
+  <si>
+    <t>LONG HAUL</t>
+  </si>
+  <si>
+    <t>Move ID</t>
+  </si>
+  <si>
+    <t>Vehicle Reg</t>
+  </si>
+  <si>
+    <t>Billable?</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>MX1234</t>
+  </si>
+  <si>
+    <t>BRADFORD POLICE STATION (TRAFALGAR HOUSE)</t>
+  </si>
+  <si>
+    <t>LEEDS MAGISTRATES COURT</t>
+  </si>
+  <si>
+    <t>XXX9876</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Journey 1</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>DERBY POLICE CUSTODY</t>
+  </si>
+  <si>
+    <t>GD-5555</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Long journey, ovenight stay.</t>
+  </si>
+  <si>
+    <t>Journey 2</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>XX-5786</t>
+  </si>
+  <si>
+    <t>SERCO</t>
   </si>
   <si>
     <r>
@@ -238,20 +243,20 @@
     </r>
     <r>
       <rPr>
-        <i val="true"/>
+        <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(a redirection after the move has started)</t>
+      <t>(a redirection after the move has started)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Contractor Billable?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes (Reason codes or supplier notes)</t>
+    <t>Contractor Billable?</t>
+  </si>
+  <si>
+    <t>Notes (Reason codes or supplier notes)</t>
   </si>
   <si>
     <r>
@@ -266,17 +271,17 @@
     </r>
     <r>
       <rPr>
-        <i val="true"/>
+        <i/>
         <sz val="9"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(refused admission to prison)</t>
+      <t>(refused admission to prison)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Date range</t>
+    <t>Date range</t>
   </si>
   <si>
     <r>
@@ -287,11 +292,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">MULTI-TYPE MOVES</t>
+      <t>MULTI-TYPE MOVES</t>
     </r>
     <r>
       <rPr>
-        <i val="true"/>
+        <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -313,74 +318,50 @@
     </r>
     <r>
       <rPr>
-        <i val="true"/>
+        <i/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(includes prison to prison transfer moves that have been cancelled by the population mangement unit after 3pm on the day before the move)</t>
+      <t>(includes prison to prison transfer moves that have been cancelled by the population mangement unit after 3pm on the day before the move)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Move date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancellation date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancellation time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dev notes:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTAL VOLUME BY LOCATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total journey count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total price</t>
+    <t>Move date</t>
+  </si>
+  <si>
+    <t>Cancellation date</t>
+  </si>
+  <si>
+    <t>Cancellation time</t>
+  </si>
+  <si>
+    <t>TOTAL VOLUME BY LOCATION</t>
+  </si>
+  <si>
+    <t>Total journey count</t>
+  </si>
+  <si>
+    <t>Unit price</t>
+  </si>
+  <si>
+    <t>Total price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="0%"/>
-    <numFmt numFmtId="167" formatCode="#,##0"/>
-    <numFmt numFmtId="168" formatCode="\£#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="HH:MM"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="\£#,##0.00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -390,7 +371,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -398,7 +379,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -406,14 +387,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -426,14 +407,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -488,15 +469,9 @@
         <bgColor rgb="FF800000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -504,225 +479,113 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="46">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="20" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -781,32 +644,340 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.5"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,7 +1008,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -865,7 +1036,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -893,7 +1064,7 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -923,7 +1094,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -953,7 +1124,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -985,7 +1156,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1014,7 +1185,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -1045,7 +1216,7 @@
       <c r="Z8" s="9"/>
       <c r="AA8" s="9"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
@@ -1084,14 +1255,14 @@
       <c r="Z9" s="13"/>
       <c r="AA9" s="13"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="43"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1115,14 +1286,14 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
+    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1146,12 +1317,12 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1175,14 +1346,14 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="1"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="43"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1206,10 +1377,14 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
+      <c r="B14" s="48"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1233,12 +1408,12 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="15"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1262,14 +1437,14 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="1"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1293,14 +1468,14 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
+    <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1324,12 +1499,12 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1353,14 +1528,14 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="43"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1384,14 +1559,14 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="17" t="s">
+    <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1415,12 +1590,12 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="19"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1444,14 +1619,14 @@
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="1"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1475,14 +1650,14 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="17" t="s">
+    <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1506,12 +1681,12 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1535,14 +1710,14 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1566,14 +1741,14 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1597,14 +1772,14 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="17" t="s">
+    <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1628,18 +1803,18 @@
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="22"/>
-      <c r="B28" s="23" t="s">
+    <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="19"/>
+      <c r="B28" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="20" t="s">
         <v>27</v>
       </c>
       <c r="F28" s="4"/>
@@ -1665,9 +1840,9 @@
       <c r="Z28" s="4"/>
       <c r="AA28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1694,9 +1869,9 @@
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
-      <c r="B30" s="20"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1723,7 +1898,7 @@
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1750,44 +1925,34 @@
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
-      <c r="AA31" s="24"/>
+      <c r="AA31" s="21"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="19.5" customWidth="1"/>
+    <col min="11" max="11" width="15.5" customWidth="1"/>
+    <col min="12" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1823,7 +1988,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1857,7 +2022,7 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1891,7 +2056,7 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1927,7 +2092,7 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1963,7 +2128,7 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2001,7 +2166,7 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2035,7 +2200,7 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
@@ -2071,7 +2236,7 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>29</v>
       </c>
@@ -2087,30 +2252,30 @@
       <c r="E9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="26"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="26"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="23"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -2129,7 +2294,7 @@
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2163,7 +2328,7 @@
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2197,12 +2362,12 @@
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -2231,7 +2396,7 @@
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2265,7 +2430,7 @@
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2296,10 +2461,10 @@
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
-      <c r="AE14" s="28"/>
-      <c r="AF14" s="28"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE14" s="25"/>
+      <c r="AF14" s="25"/>
+    </row>
+    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2333,7 +2498,7 @@
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2364,10 +2529,10 @@
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
-      <c r="AE16" s="28"/>
-      <c r="AF16" s="28"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE16" s="25"/>
+      <c r="AF16" s="25"/>
+    </row>
+    <row r="17" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2401,7 +2566,7 @@
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2435,7 +2600,7 @@
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2469,7 +2634,7 @@
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2500,10 +2665,10 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
-      <c r="AE20" s="28"/>
-      <c r="AF20" s="28"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE20" s="25"/>
+      <c r="AF20" s="25"/>
+    </row>
+    <row r="21" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2537,7 +2702,7 @@
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2568,10 +2733,10 @@
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
-      <c r="AE22" s="28"/>
-      <c r="AF22" s="28"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE22" s="25"/>
+      <c r="AF22" s="25"/>
+    </row>
+    <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2602,10 +2767,10 @@
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
-      <c r="AE23" s="28"/>
-      <c r="AF23" s="28"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE23" s="25"/>
+      <c r="AF23" s="25"/>
+    </row>
+    <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2636,10 +2801,10 @@
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
-      <c r="AE24" s="28"/>
-      <c r="AF24" s="28"/>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE24" s="25"/>
+      <c r="AF24" s="25"/>
+    </row>
+    <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2670,10 +2835,10 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
-      <c r="AE25" s="28"/>
-      <c r="AF25" s="28"/>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AE25" s="25"/>
+      <c r="AF25" s="25"/>
+    </row>
+    <row r="26" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2704,55 +2869,47 @@
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
-      <c r="AE26" s="28"/>
-      <c r="AF26" s="28"/>
+      <c r="AE26" s="25"/>
+      <c r="AF26" s="25"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="5" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="50" customWidth="1"/>
+    <col min="15" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="29"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2765,10 +2922,10 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2781,10 +2938,10 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -2797,7 +2954,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -2815,7 +2972,7 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2833,7 +2990,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2853,7 +3010,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2869,7 +3026,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
@@ -2887,20 +3044,20 @@
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="22" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="22" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -2915,35 +3072,35 @@
       <c r="I9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="27" t="s">
         <v>42</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="31"/>
-      <c r="V9" s="31"/>
-      <c r="W9" s="31"/>
-      <c r="X9" s="31"/>
-      <c r="Y9" s="31"/>
-      <c r="Z9" s="31"/>
-    </row>
-    <row r="10" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28"/>
+    </row>
+    <row r="10" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13" t="s">
         <v>44</v>
       </c>
@@ -2955,29 +3112,29 @@
         <v>46</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="32" t="n">
+      <c r="F10" s="29">
         <v>43845</v>
       </c>
-      <c r="G10" s="33" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="H10" s="32" t="n">
+      <c r="G10" s="30">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H10" s="29">
         <v>43846</v>
       </c>
-      <c r="I10" s="33" t="n">
-        <v>0.743055555555556</v>
+      <c r="I10" s="30">
+        <v>0.74305555555555602</v>
       </c>
       <c r="J10" s="13"/>
-      <c r="K10" s="34" t="s">
+      <c r="K10" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="L10" s="32" t="s">
         <v>48</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:26" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -2993,23 +3150,23 @@
       <c r="E11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="36" t="n">
+      <c r="F11" s="33">
         <v>43845</v>
       </c>
-      <c r="G11" s="37" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="H11" s="36" t="n">
+      <c r="G11" s="34">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H11" s="33">
         <v>43845</v>
       </c>
-      <c r="I11" s="37" t="n">
-        <v>0.604166666666667</v>
-      </c>
-      <c r="J11" s="38" t="s">
+      <c r="I11" s="34">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="J11" s="35" t="s">
         <v>52</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="39" t="s">
+      <c r="L11" s="36" t="s">
         <v>48</v>
       </c>
       <c r="M11" s="8" t="s">
@@ -3019,7 +3176,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:26" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -3035,23 +3192,23 @@
       <c r="E12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="36" t="n">
+      <c r="F12" s="33">
         <v>43846</v>
       </c>
-      <c r="G12" s="37" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="H12" s="36" t="n">
+      <c r="G12" s="34">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H12" s="33">
         <v>43846</v>
       </c>
-      <c r="I12" s="37" t="n">
-        <v>0.743055555555556</v>
-      </c>
-      <c r="J12" s="38" t="s">
+      <c r="I12" s="34">
+        <v>0.74305555555555602</v>
+      </c>
+      <c r="J12" s="35" t="s">
         <v>57</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="L12" s="40" t="n">
+      <c r="L12" s="37">
         <v>33.58</v>
       </c>
       <c r="M12" s="8" t="s">
@@ -3060,44 +3217,36 @@
       <c r="N12" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="43.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="52" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="43.6640625" customWidth="1"/>
+    <col min="15" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3131,7 +3280,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3163,7 +3312,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3195,7 +3344,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3229,7 +3378,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3265,7 +3414,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3301,7 +3450,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3333,7 +3482,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>59</v>
       </c>
@@ -3367,20 +3516,20 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="22" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="22" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -3395,16 +3544,16 @@
       <c r="I9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="27" t="s">
         <v>60</v>
       </c>
       <c r="N9" s="14" t="s">
@@ -3428,43 +3577,35 @@
       <c r="AD9" s="14"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="48.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="28.5" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+    <col min="12" max="13" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="48.33203125" customWidth="1"/>
+    <col min="15" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3500,7 +3641,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3534,7 +3675,7 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3568,7 +3709,7 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3584,7 +3725,7 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
-      <c r="N4" s="22"/>
+      <c r="N4" s="19"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -3604,7 +3745,7 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3640,7 +3781,7 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3678,7 +3819,7 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3712,7 +3853,7 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>62</v>
       </c>
@@ -3728,7 +3869,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-      <c r="N8" s="22"/>
+      <c r="N8" s="19"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -3748,47 +3889,47 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="25" t="s">
+      <c r="N9" s="22" t="s">
         <v>43</v>
       </c>
       <c r="O9" s="1"/>
@@ -3811,46 +3952,38 @@
       <c r="AF9" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="15.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="66.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="11" width="15.5" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" customWidth="1"/>
+    <col min="14" max="14" width="50.1640625" customWidth="1"/>
+    <col min="15" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3884,7 +4017,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3916,7 +4049,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3948,7 +4081,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3982,7 +4115,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4016,7 +4149,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>63</v>
       </c>
@@ -4052,7 +4185,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4084,7 +4217,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>64</v>
       </c>
@@ -4118,51 +4251,51 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="27" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="27" t="s">
         <v>60</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>43</v>
       </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="28"/>
+      <c r="P9" s="25"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -4179,48 +4312,40 @@
       <c r="AD9" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="40.83203125" customWidth="1"/>
+    <col min="12" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="38"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4250,7 +4375,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4281,7 +4406,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4313,7 +4438,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4326,7 +4451,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="42"/>
+      <c r="K4" s="39"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -4347,7 +4472,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4381,7 +4506,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4417,7 +4542,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4449,7 +4574,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>65</v>
       </c>
@@ -4462,7 +4587,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="42"/>
+      <c r="K8" s="39"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -4483,7 +4608,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>29</v>
       </c>
@@ -4499,28 +4624,26 @@
       <c r="E9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="43" t="s">
+      <c r="H9" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="44" t="s">
+      <c r="K9" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="M9" s="26"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="23"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -4539,50 +4662,42 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="40.83203125" customWidth="1"/>
+    <col min="12" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="38"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4612,7 +4727,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4643,7 +4758,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4675,7 +4790,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4688,7 +4803,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="42"/>
+      <c r="K4" s="39"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -4709,7 +4824,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4743,7 +4858,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4779,7 +4894,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4811,9 +4926,9 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4824,7 +4939,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="42"/>
+      <c r="K8" s="39"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -4845,7 +4960,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>30</v>
       </c>
@@ -4853,24 +4968,22 @@
         <v>32</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="M9" s="26"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="23"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -4889,66 +5002,62 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.65"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="38.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43.1640625" customWidth="1"/>
+    <col min="5" max="1025" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4959,12 +5068,7 @@
       <c r="D6" s="7"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
P4-2551 spreadsheet changes.  Background row colour now solid, changed text on journeys tab. If no unit price on journeys tab then display 'NOT PRESENT'
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonnycavell/p/calculate-people-move-prices/src/main/resources/spreadsheets/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE3C0F6-E4AA-184B-A880-B634A104D96D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33000" windowHeight="19680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Standard" sheetId="2" r:id="rId2"/>
-    <sheet name="Long haul" sheetId="3" r:id="rId3"/>
-    <sheet name="Redirections" sheetId="4" r:id="rId4"/>
-    <sheet name="Lockouts" sheetId="5" r:id="rId5"/>
-    <sheet name="Multi-type" sheetId="6" r:id="rId6"/>
-    <sheet name="Cancelled" sheetId="7" r:id="rId7"/>
-    <sheet name="Journeys" sheetId="8" r:id="rId8"/>
-    <sheet name="JPC Price book" sheetId="9" r:id="rId9"/>
+    <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Standard" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Long haul" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Redirections" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Lockouts" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Multi-type" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Cancelled" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Journeys" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="JPC Price book" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -35,88 +30,88 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="73">
   <si>
-    <t>Export date</t>
-  </si>
-  <si>
-    <t>Calculate Journey Variable Payments (S2B)</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
-  <si>
-    <t>Date Range</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>OUTPUT SUMMARY</t>
-  </si>
-  <si>
-    <t>Move type</t>
-  </si>
-  <si>
-    <t>Percentage</t>
+    <t xml:space="preserve">Export date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate Journey Variable Payments (S2B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTPUT SUMMARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage</t>
   </si>
   <si>
     <t xml:space="preserve"> Move volume</t>
   </si>
   <si>
-    <t>Move volume without prices</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Standard move</t>
-  </si>
-  <si>
-    <t>includes single journeys, cross supplier and redirects before the move has started</t>
+    <t xml:space="preserve">Move volume without prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes single journeys, cross supplier and redirects before the move has started</t>
   </si>
   <si>
     <t xml:space="preserve">Long haul </t>
   </si>
   <si>
-    <t>a completed move made up of 2 or more journeys</t>
-  </si>
-  <si>
-    <t>Redirections</t>
-  </si>
-  <si>
-    <t>a redirection after the move has started</t>
-  </si>
-  <si>
-    <t>Lockouts</t>
-  </si>
-  <si>
-    <t>refused admission to prison</t>
-  </si>
-  <si>
-    <t>Multi-type moves</t>
-  </si>
-  <si>
-    <t>includes combinations of the above</t>
-  </si>
-  <si>
-    <t>Cancelled moves</t>
+    <t xml:space="preserve">a completed move made up of 2 or more journeys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redirections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a redirection after the move has started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lockouts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refused admission to prison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-type moves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes combinations of the above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancelled moves</t>
   </si>
   <si>
     <t xml:space="preserve">prison to prison moves cancelled by PMU later than </t>
   </si>
   <si>
-    <t>3pm the day before the move date</t>
-  </si>
-  <si>
-    <t>Total %</t>
-  </si>
-  <si>
-    <t>Total volume</t>
-  </si>
-  <si>
-    <t>Total volume without prices</t>
-  </si>
-  <si>
-    <t>Total Price</t>
+    <t xml:space="preserve">3pm the day before the move date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total volume without prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Price</t>
   </si>
   <si>
     <r>
@@ -131,104 +126,104 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(includes single journeys, cross supplier and redirects before the move has started)</t>
+      <t xml:space="preserve">(includes single journeys, cross supplier and redirects before the move has started)</t>
     </r>
   </si>
   <si>
-    <t>Move Ref ID</t>
-  </si>
-  <si>
-    <t>Pick up</t>
-  </si>
-  <si>
-    <t>Location Type</t>
-  </si>
-  <si>
-    <t>Drop off</t>
-  </si>
-  <si>
-    <t>Pick up date</t>
-  </si>
-  <si>
-    <t>Pick up time</t>
-  </si>
-  <si>
-    <t>Drop off date</t>
-  </si>
-  <si>
-    <t>Drop off time</t>
+    <t xml:space="preserve">Move Ref ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off time</t>
   </si>
   <si>
     <t xml:space="preserve">Vehicle Reg </t>
   </si>
   <si>
-    <t>NOMIS Prison ID</t>
-  </si>
-  <si>
-    <t>LONG HAUL</t>
-  </si>
-  <si>
-    <t>Move ID</t>
-  </si>
-  <si>
-    <t>Vehicle Reg</t>
-  </si>
-  <si>
-    <t>Billable?</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>MX1234</t>
-  </si>
-  <si>
-    <t>BRADFORD POLICE STATION (TRAFALGAR HOUSE)</t>
-  </si>
-  <si>
-    <t>LEEDS MAGISTRATES COURT</t>
-  </si>
-  <si>
-    <t>XXX9876</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>Journey 1</t>
-  </si>
-  <si>
-    <t>PS</t>
-  </si>
-  <si>
-    <t>DERBY POLICE CUSTODY</t>
-  </si>
-  <si>
-    <t>GD-5555</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>Long journey, ovenight stay.</t>
-  </si>
-  <si>
-    <t>Journey 2</t>
-  </si>
-  <si>
-    <t>MC</t>
-  </si>
-  <si>
-    <t>XX-5786</t>
-  </si>
-  <si>
-    <t>SERCO</t>
+    <t xml:space="preserve">NOMIS Prison ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LONG HAUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billable?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MX1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRADFORD POLICE STATION (TRAFALGAR HOUSE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEEDS MAGISTRATES COURT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XXX9876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journey 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DERBY POLICE CUSTODY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GD-5555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long journey, ovenight stay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journey 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XX-5786</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERCO</t>
   </si>
   <si>
     <r>
@@ -243,20 +238,20 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(a redirection after the move has started)</t>
+      <t xml:space="preserve">(a redirection after the move has started)</t>
     </r>
   </si>
   <si>
-    <t>Contractor Billable?</t>
-  </si>
-  <si>
-    <t>Notes (Reason codes or supplier notes)</t>
+    <t xml:space="preserve">Contractor Billable?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes (Reason codes or supplier notes)</t>
   </si>
   <si>
     <r>
@@ -271,17 +266,17 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="9"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(refused admission to prison)</t>
+      <t xml:space="preserve">(refused admission to prison)</t>
     </r>
   </si>
   <si>
-    <t>Date range</t>
+    <t xml:space="preserve">Date range</t>
   </si>
   <si>
     <r>
@@ -292,11 +287,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>MULTI-TYPE MOVES</t>
+      <t xml:space="preserve">MULTI-TYPE MOVES</t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -318,50 +313,71 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(includes prison to prison transfer moves that have been cancelled by the population mangement unit after 3pm on the day before the move)</t>
+      <t xml:space="preserve">(includes prison to prison transfer moves that have been cancelled by the population mangement unit after 3pm on the day before the move)</t>
     </r>
   </si>
   <si>
-    <t>Move date</t>
-  </si>
-  <si>
-    <t>Cancellation date</t>
-  </si>
-  <si>
-    <t>Cancellation time</t>
-  </si>
-  <si>
-    <t>TOTAL VOLUME BY LOCATION</t>
-  </si>
-  <si>
-    <t>Total journey count</t>
-  </si>
-  <si>
-    <t>Unit price</t>
-  </si>
-  <si>
-    <t>Total price</t>
+    <t xml:space="preserve">Move date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancellation date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancellation time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL VOLUME BY JOURNEY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total journey count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="\£#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="167" formatCode="0%"/>
+    <numFmt numFmtId="168" formatCode="\£#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="HH:MM"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -371,7 +387,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -379,7 +395,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -387,14 +403,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -407,7 +423,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -471,7 +487,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -479,113 +495,237 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -644,340 +784,32 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1008,7 +840,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1036,7 +868,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
     </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1064,7 +896,7 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1094,7 +926,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
     </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1124,7 +956,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1156,7 +988,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1185,7 +1017,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -1216,7 +1048,7 @@
       <c r="Z8" s="9"/>
       <c r="AA8" s="9"/>
     </row>
-    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
@@ -1255,14 +1087,14 @@
       <c r="Z9" s="13"/>
       <c r="AA9" s="13"/>
     </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="43"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1286,14 +1118,14 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="15" t="s">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1317,12 +1149,12 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1346,14 +1178,14 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="43"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1377,14 +1209,14 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="15" t="s">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1408,12 +1240,12 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="15"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1437,14 +1269,14 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="43"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1468,14 +1300,14 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="15" t="s">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1499,12 +1331,12 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1528,14 +1360,14 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1559,14 +1391,14 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="15" t="s">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="47"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1590,12 +1422,12 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1619,14 +1451,14 @@
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="43"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1650,14 +1482,14 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="15" t="s">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1681,12 +1513,12 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1710,14 +1542,14 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="47"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1741,14 +1573,14 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="15" t="s">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1772,14 +1604,14 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="15" t="s">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1803,18 +1635,18 @@
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
     </row>
-    <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20" t="s">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="23"/>
+      <c r="B28" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="24" t="s">
         <v>27</v>
       </c>
       <c r="F28" s="4"/>
@@ -1840,9 +1672,9 @@
       <c r="Z28" s="4"/>
       <c r="AA28" s="4"/>
     </row>
-    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
-      <c r="B29" s="47"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1869,9 +1701,9 @@
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
-      <c r="B30" s="17"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1898,7 +1730,7 @@
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1925,34 +1757,44 @@
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
-      <c r="AA31" s="21"/>
+      <c r="AA31" s="26"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="19.5" customWidth="1"/>
-    <col min="11" max="11" width="15.5" customWidth="1"/>
-    <col min="12" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1988,7 +1830,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2022,7 +1864,7 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
-    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2056,7 +1898,7 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -2092,7 +1934,7 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
-    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2128,7 +1970,7 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
-    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2166,7 +2008,7 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
-    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2200,7 +2042,7 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
@@ -2236,7 +2078,7 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>29</v>
       </c>
@@ -2252,30 +2094,30 @@
       <c r="E9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="L9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="23"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="23"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="28"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -2294,7 +2136,7 @@
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
     </row>
-    <row r="10" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2328,7 +2170,7 @@
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
     </row>
-    <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2362,12 +2204,12 @@
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
     </row>
-    <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -2396,7 +2238,7 @@
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
     </row>
-    <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2430,7 +2272,7 @@
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
     </row>
-    <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2461,10 +2303,10 @@
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
-      <c r="AE14" s="25"/>
-      <c r="AF14" s="25"/>
-    </row>
-    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE14" s="31"/>
+      <c r="AF14" s="31"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2498,7 +2340,7 @@
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
     </row>
-    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2529,10 +2371,10 @@
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
-      <c r="AE16" s="25"/>
-      <c r="AF16" s="25"/>
-    </row>
-    <row r="17" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE16" s="31"/>
+      <c r="AF16" s="31"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2566,7 +2408,7 @@
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
     </row>
-    <row r="18" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2600,7 +2442,7 @@
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
     </row>
-    <row r="19" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2634,7 +2476,7 @@
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
     </row>
-    <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2665,10 +2507,10 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
-      <c r="AE20" s="25"/>
-      <c r="AF20" s="25"/>
-    </row>
-    <row r="21" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE20" s="31"/>
+      <c r="AF20" s="31"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2702,7 +2544,7 @@
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
     </row>
-    <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2733,10 +2575,10 @@
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
-      <c r="AE22" s="25"/>
-      <c r="AF22" s="25"/>
-    </row>
-    <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE22" s="31"/>
+      <c r="AF22" s="31"/>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2767,10 +2609,10 @@
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
-      <c r="AE23" s="25"/>
-      <c r="AF23" s="25"/>
-    </row>
-    <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE23" s="31"/>
+      <c r="AF23" s="31"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2801,10 +2643,10 @@
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
-      <c r="AE24" s="25"/>
-      <c r="AF24" s="25"/>
-    </row>
-    <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE24" s="31"/>
+      <c r="AF24" s="31"/>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2835,10 +2677,10 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
-      <c r="AE25" s="25"/>
-      <c r="AF25" s="25"/>
-    </row>
-    <row r="26" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE25" s="31"/>
+      <c r="AF25" s="31"/>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2869,47 +2711,55 @@
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
-      <c r="AE26" s="25"/>
-      <c r="AF26" s="25"/>
+      <c r="AE26" s="31"/>
+      <c r="AF26" s="31"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" customWidth="1"/>
-    <col min="12" max="12" width="10.1640625" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="50" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="26"/>
+      <c r="C1" s="32"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2922,10 +2772,10 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2938,10 +2788,10 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -2954,7 +2804,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -2972,7 +2822,7 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2990,7 +2840,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3010,7 +2860,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3026,7 +2876,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
@@ -3044,20 +2894,20 @@
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="27" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="27" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -3072,35 +2922,35 @@
       <c r="I9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="L9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="34" t="s">
         <v>42</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="28"/>
-    </row>
-    <row r="10" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
+      <c r="X9" s="35"/>
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="35"/>
+    </row>
+    <row r="10" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
         <v>44</v>
       </c>
@@ -3112,29 +2962,29 @@
         <v>46</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="29">
+      <c r="F10" s="36" t="n">
         <v>43845</v>
       </c>
-      <c r="G10" s="30">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="H10" s="29">
+      <c r="G10" s="37" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H10" s="36" t="n">
         <v>43846</v>
       </c>
-      <c r="I10" s="30">
-        <v>0.74305555555555602</v>
+      <c r="I10" s="37" t="n">
+        <v>0.743055555555556</v>
       </c>
       <c r="J10" s="13"/>
-      <c r="K10" s="31" t="s">
+      <c r="K10" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="32" t="s">
+      <c r="L10" s="39" t="s">
         <v>48</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="11" customFormat="false" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -3150,23 +3000,23 @@
       <c r="E11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="40" t="n">
         <v>43845</v>
       </c>
-      <c r="G11" s="34">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="H11" s="33">
+      <c r="G11" s="41" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H11" s="40" t="n">
         <v>43845</v>
       </c>
-      <c r="I11" s="34">
-        <v>0.60416666666666696</v>
-      </c>
-      <c r="J11" s="35" t="s">
+      <c r="I11" s="41" t="n">
+        <v>0.604166666666667</v>
+      </c>
+      <c r="J11" s="42" t="s">
         <v>52</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="36" t="s">
+      <c r="L11" s="43" t="s">
         <v>48</v>
       </c>
       <c r="M11" s="8" t="s">
@@ -3176,7 +3026,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="12" customFormat="false" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -3192,23 +3042,23 @@
       <c r="E12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="40" t="n">
         <v>43846</v>
       </c>
-      <c r="G12" s="34">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="H12" s="33">
+      <c r="G12" s="41" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H12" s="40" t="n">
         <v>43846</v>
       </c>
-      <c r="I12" s="34">
-        <v>0.74305555555555602</v>
-      </c>
-      <c r="J12" s="35" t="s">
+      <c r="I12" s="41" t="n">
+        <v>0.743055555555556</v>
+      </c>
+      <c r="J12" s="42" t="s">
         <v>57</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="L12" s="37">
+      <c r="L12" s="44" t="n">
         <v>33.58</v>
       </c>
       <c r="M12" s="8" t="s">
@@ -3217,36 +3067,44 @@
       <c r="N12" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="52" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="16.5" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="43.6640625" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="43.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3280,7 +3138,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3312,7 +3170,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3344,7 +3202,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3378,7 +3236,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3414,7 +3272,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3450,7 +3308,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3482,7 +3340,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>59</v>
       </c>
@@ -3516,20 +3374,20 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="27" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="27" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -3544,16 +3402,16 @@
       <c r="I9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="L9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="34" t="s">
         <v>60</v>
       </c>
       <c r="N9" s="14" t="s">
@@ -3577,35 +3435,43 @@
       <c r="AD9" s="14"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="28.5" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" customWidth="1"/>
-    <col min="12" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="48.33203125" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="48.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3641,7 +3507,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3675,7 +3541,7 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
-    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3709,7 +3575,7 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3725,7 +3591,7 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
-      <c r="N4" s="19"/>
+      <c r="N4" s="23"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -3745,7 +3611,7 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
-    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3781,7 +3647,7 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
-    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3819,7 +3685,7 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
-    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3853,7 +3719,7 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>62</v>
       </c>
@@ -3869,7 +3735,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-      <c r="N8" s="19"/>
+      <c r="N8" s="23"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -3889,47 +3755,47 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="22" t="s">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="22" t="s">
+      <c r="N9" s="27" t="s">
         <v>43</v>
       </c>
       <c r="O9" s="1"/>
@@ -3952,38 +3818,46 @@
       <c r="AF9" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="11" width="15.5" customWidth="1"/>
-    <col min="12" max="12" width="13.5" customWidth="1"/>
-    <col min="13" max="13" width="19.1640625" customWidth="1"/>
-    <col min="14" max="14" width="50.1640625" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4017,7 +3891,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -4049,7 +3923,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4081,7 +3955,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4115,7 +3989,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4149,7 +4023,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>63</v>
       </c>
@@ -4185,7 +4059,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4217,7 +4091,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>64</v>
       </c>
@@ -4251,51 +4125,51 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="34" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="34" t="s">
         <v>60</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>43</v>
       </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="25"/>
+      <c r="P9" s="31"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -4312,40 +4186,48 @@
       <c r="AD9" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="40.83203125" customWidth="1"/>
-    <col min="12" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="45"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4375,7 +4257,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4406,7 +4288,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4438,7 +4320,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4451,7 +4333,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="39"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -4472,7 +4354,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4506,7 +4388,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4542,7 +4424,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4574,7 +4456,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>65</v>
       </c>
@@ -4587,7 +4469,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="39"/>
+      <c r="K8" s="46"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -4608,7 +4490,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>29</v>
       </c>
@@ -4624,26 +4506,26 @@
       <c r="E9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="J9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="48" t="s">
         <v>43</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="23"/>
+      <c r="M9" s="28"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -4662,42 +4544,50 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="38.5" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="40.83203125" customWidth="1"/>
-    <col min="12" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="45"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4727,7 +4617,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4758,7 +4648,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4790,7 +4680,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4803,7 +4693,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="39"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -4824,7 +4714,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4858,7 +4748,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4894,7 +4784,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4926,7 +4816,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>69</v>
       </c>
@@ -4939,7 +4829,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="39"/>
+      <c r="K8" s="46"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -4960,7 +4850,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>30</v>
       </c>
@@ -4976,14 +4866,14 @@
       <c r="E9" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="41"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="48"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="23"/>
+      <c r="M9" s="28"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -5002,62 +4892,70 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="37.5" customWidth="1"/>
-    <col min="3" max="3" width="38.33203125" customWidth="1"/>
-    <col min="4" max="4" width="43.1640625" customWidth="1"/>
-    <col min="5" max="1025" width="10.6640625" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.66"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -5068,7 +4966,12 @@
       <c r="D6" s="7"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
P4-2551 spreadsheet changes.  Background row colour now solid, changed text on journeys tab. If no unit price on journeys tab then display 'NOT PRESENT' (#159)
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonnycavell/p/calculate-people-move-prices/src/main/resources/spreadsheets/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE3C0F6-E4AA-184B-A880-B634A104D96D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33000" windowHeight="19680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Standard" sheetId="2" r:id="rId2"/>
-    <sheet name="Long haul" sheetId="3" r:id="rId3"/>
-    <sheet name="Redirections" sheetId="4" r:id="rId4"/>
-    <sheet name="Lockouts" sheetId="5" r:id="rId5"/>
-    <sheet name="Multi-type" sheetId="6" r:id="rId6"/>
-    <sheet name="Cancelled" sheetId="7" r:id="rId7"/>
-    <sheet name="Journeys" sheetId="8" r:id="rId8"/>
-    <sheet name="JPC Price book" sheetId="9" r:id="rId9"/>
+    <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Standard" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Long haul" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Redirections" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Lockouts" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Multi-type" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Cancelled" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Journeys" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="JPC Price book" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -35,88 +30,88 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="73">
   <si>
-    <t>Export date</t>
-  </si>
-  <si>
-    <t>Calculate Journey Variable Payments (S2B)</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
-  <si>
-    <t>Date Range</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>OUTPUT SUMMARY</t>
-  </si>
-  <si>
-    <t>Move type</t>
-  </si>
-  <si>
-    <t>Percentage</t>
+    <t xml:space="preserve">Export date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate Journey Variable Payments (S2B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTPUT SUMMARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage</t>
   </si>
   <si>
     <t xml:space="preserve"> Move volume</t>
   </si>
   <si>
-    <t>Move volume without prices</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Standard move</t>
-  </si>
-  <si>
-    <t>includes single journeys, cross supplier and redirects before the move has started</t>
+    <t xml:space="preserve">Move volume without prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes single journeys, cross supplier and redirects before the move has started</t>
   </si>
   <si>
     <t xml:space="preserve">Long haul </t>
   </si>
   <si>
-    <t>a completed move made up of 2 or more journeys</t>
-  </si>
-  <si>
-    <t>Redirections</t>
-  </si>
-  <si>
-    <t>a redirection after the move has started</t>
-  </si>
-  <si>
-    <t>Lockouts</t>
-  </si>
-  <si>
-    <t>refused admission to prison</t>
-  </si>
-  <si>
-    <t>Multi-type moves</t>
-  </si>
-  <si>
-    <t>includes combinations of the above</t>
-  </si>
-  <si>
-    <t>Cancelled moves</t>
+    <t xml:space="preserve">a completed move made up of 2 or more journeys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redirections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a redirection after the move has started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lockouts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refused admission to prison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-type moves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes combinations of the above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancelled moves</t>
   </si>
   <si>
     <t xml:space="preserve">prison to prison moves cancelled by PMU later than </t>
   </si>
   <si>
-    <t>3pm the day before the move date</t>
-  </si>
-  <si>
-    <t>Total %</t>
-  </si>
-  <si>
-    <t>Total volume</t>
-  </si>
-  <si>
-    <t>Total volume without prices</t>
-  </si>
-  <si>
-    <t>Total Price</t>
+    <t xml:space="preserve">3pm the day before the move date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total volume without prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Price</t>
   </si>
   <si>
     <r>
@@ -131,104 +126,104 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(includes single journeys, cross supplier and redirects before the move has started)</t>
+      <t xml:space="preserve">(includes single journeys, cross supplier and redirects before the move has started)</t>
     </r>
   </si>
   <si>
-    <t>Move Ref ID</t>
-  </si>
-  <si>
-    <t>Pick up</t>
-  </si>
-  <si>
-    <t>Location Type</t>
-  </si>
-  <si>
-    <t>Drop off</t>
-  </si>
-  <si>
-    <t>Pick up date</t>
-  </si>
-  <si>
-    <t>Pick up time</t>
-  </si>
-  <si>
-    <t>Drop off date</t>
-  </si>
-  <si>
-    <t>Drop off time</t>
+    <t xml:space="preserve">Move Ref ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop off time</t>
   </si>
   <si>
     <t xml:space="preserve">Vehicle Reg </t>
   </si>
   <si>
-    <t>NOMIS Prison ID</t>
-  </si>
-  <si>
-    <t>LONG HAUL</t>
-  </si>
-  <si>
-    <t>Move ID</t>
-  </si>
-  <si>
-    <t>Vehicle Reg</t>
-  </si>
-  <si>
-    <t>Billable?</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>MX1234</t>
-  </si>
-  <si>
-    <t>BRADFORD POLICE STATION (TRAFALGAR HOUSE)</t>
-  </si>
-  <si>
-    <t>LEEDS MAGISTRATES COURT</t>
-  </si>
-  <si>
-    <t>XXX9876</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>Journey 1</t>
-  </si>
-  <si>
-    <t>PS</t>
-  </si>
-  <si>
-    <t>DERBY POLICE CUSTODY</t>
-  </si>
-  <si>
-    <t>GD-5555</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>Long journey, ovenight stay.</t>
-  </si>
-  <si>
-    <t>Journey 2</t>
-  </si>
-  <si>
-    <t>MC</t>
-  </si>
-  <si>
-    <t>XX-5786</t>
-  </si>
-  <si>
-    <t>SERCO</t>
+    <t xml:space="preserve">NOMIS Prison ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LONG HAUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billable?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MX1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRADFORD POLICE STATION (TRAFALGAR HOUSE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEEDS MAGISTRATES COURT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XXX9876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journey 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DERBY POLICE CUSTODY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GD-5555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long journey, ovenight stay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journey 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XX-5786</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERCO</t>
   </si>
   <si>
     <r>
@@ -243,20 +238,20 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(a redirection after the move has started)</t>
+      <t xml:space="preserve">(a redirection after the move has started)</t>
     </r>
   </si>
   <si>
-    <t>Contractor Billable?</t>
-  </si>
-  <si>
-    <t>Notes (Reason codes or supplier notes)</t>
+    <t xml:space="preserve">Contractor Billable?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes (Reason codes or supplier notes)</t>
   </si>
   <si>
     <r>
@@ -271,17 +266,17 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="9"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(refused admission to prison)</t>
+      <t xml:space="preserve">(refused admission to prison)</t>
     </r>
   </si>
   <si>
-    <t>Date range</t>
+    <t xml:space="preserve">Date range</t>
   </si>
   <si>
     <r>
@@ -292,11 +287,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>MULTI-TYPE MOVES</t>
+      <t xml:space="preserve">MULTI-TYPE MOVES</t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -318,50 +313,71 @@
     </r>
     <r>
       <rPr>
-        <i/>
+        <i val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(includes prison to prison transfer moves that have been cancelled by the population mangement unit after 3pm on the day before the move)</t>
+      <t xml:space="preserve">(includes prison to prison transfer moves that have been cancelled by the population mangement unit after 3pm on the day before the move)</t>
     </r>
   </si>
   <si>
-    <t>Move date</t>
-  </si>
-  <si>
-    <t>Cancellation date</t>
-  </si>
-  <si>
-    <t>Cancellation time</t>
-  </si>
-  <si>
-    <t>TOTAL VOLUME BY LOCATION</t>
-  </si>
-  <si>
-    <t>Total journey count</t>
-  </si>
-  <si>
-    <t>Unit price</t>
-  </si>
-  <si>
-    <t>Total price</t>
+    <t xml:space="preserve">Move date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancellation date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancellation time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL VOLUME BY JOURNEY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total journey count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="\£#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="167" formatCode="0%"/>
+    <numFmt numFmtId="168" formatCode="\£#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="HH:MM"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -371,7 +387,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -379,7 +395,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -387,14 +403,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <i val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -407,7 +423,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -471,7 +487,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -479,113 +495,237 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -644,340 +784,32 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1008,7 +840,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1036,7 +868,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
     </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1064,7 +896,7 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1094,7 +926,7 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
     </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1124,7 +956,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1156,7 +988,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1185,7 +1017,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -1216,7 +1048,7 @@
       <c r="Z8" s="9"/>
       <c r="AA8" s="9"/>
     </row>
-    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
@@ -1255,14 +1087,14 @@
       <c r="Z9" s="13"/>
       <c r="AA9" s="13"/>
     </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="43"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1286,14 +1118,14 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="15" t="s">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1317,12 +1149,12 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1346,14 +1178,14 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="43"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1377,14 +1209,14 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="15" t="s">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1408,12 +1240,12 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="15"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1437,14 +1269,14 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="43"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1468,14 +1300,14 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="15" t="s">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1499,12 +1331,12 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1528,14 +1360,14 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1559,14 +1391,14 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="15" t="s">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="47"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1590,12 +1422,12 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1619,14 +1451,14 @@
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="43"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1650,14 +1482,14 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="15" t="s">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1681,12 +1513,12 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1710,14 +1542,14 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="47"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1741,14 +1573,14 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="15" t="s">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1772,14 +1604,14 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="15" t="s">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1803,18 +1635,18 @@
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
     </row>
-    <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20" t="s">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="23"/>
+      <c r="B28" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="24" t="s">
         <v>27</v>
       </c>
       <c r="F28" s="4"/>
@@ -1840,9 +1672,9 @@
       <c r="Z28" s="4"/>
       <c r="AA28" s="4"/>
     </row>
-    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
-      <c r="B29" s="47"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1869,9 +1701,9 @@
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
-      <c r="B30" s="17"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1898,7 +1730,7 @@
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1925,34 +1757,44 @@
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
-      <c r="AA31" s="21"/>
+      <c r="AA31" s="26"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="19.5" customWidth="1"/>
-    <col min="11" max="11" width="15.5" customWidth="1"/>
-    <col min="12" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1988,7 +1830,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2022,7 +1864,7 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
-    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2056,7 +1898,7 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -2092,7 +1934,7 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
-    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2128,7 +1970,7 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
-    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2166,7 +2008,7 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
-    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2200,7 +2042,7 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
@@ -2236,7 +2078,7 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>29</v>
       </c>
@@ -2252,30 +2094,30 @@
       <c r="E9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="L9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="23"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="23"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="28"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -2294,7 +2136,7 @@
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
     </row>
-    <row r="10" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2328,7 +2170,7 @@
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
     </row>
-    <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2362,12 +2204,12 @@
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
     </row>
-    <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -2396,7 +2238,7 @@
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
     </row>
-    <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2430,7 +2272,7 @@
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
     </row>
-    <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2461,10 +2303,10 @@
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
-      <c r="AE14" s="25"/>
-      <c r="AF14" s="25"/>
-    </row>
-    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE14" s="31"/>
+      <c r="AF14" s="31"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2498,7 +2340,7 @@
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
     </row>
-    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2529,10 +2371,10 @@
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
-      <c r="AE16" s="25"/>
-      <c r="AF16" s="25"/>
-    </row>
-    <row r="17" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE16" s="31"/>
+      <c r="AF16" s="31"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2566,7 +2408,7 @@
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
     </row>
-    <row r="18" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2600,7 +2442,7 @@
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
     </row>
-    <row r="19" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2634,7 +2476,7 @@
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
     </row>
-    <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2665,10 +2507,10 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
-      <c r="AE20" s="25"/>
-      <c r="AF20" s="25"/>
-    </row>
-    <row r="21" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE20" s="31"/>
+      <c r="AF20" s="31"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2702,7 +2544,7 @@
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
     </row>
-    <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2733,10 +2575,10 @@
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
-      <c r="AE22" s="25"/>
-      <c r="AF22" s="25"/>
-    </row>
-    <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE22" s="31"/>
+      <c r="AF22" s="31"/>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2767,10 +2609,10 @@
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
-      <c r="AE23" s="25"/>
-      <c r="AF23" s="25"/>
-    </row>
-    <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE23" s="31"/>
+      <c r="AF23" s="31"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2801,10 +2643,10 @@
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
-      <c r="AE24" s="25"/>
-      <c r="AF24" s="25"/>
-    </row>
-    <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE24" s="31"/>
+      <c r="AF24" s="31"/>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2835,10 +2677,10 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
-      <c r="AE25" s="25"/>
-      <c r="AF25" s="25"/>
-    </row>
-    <row r="26" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE25" s="31"/>
+      <c r="AF25" s="31"/>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2869,47 +2711,55 @@
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
-      <c r="AE26" s="25"/>
-      <c r="AF26" s="25"/>
+      <c r="AE26" s="31"/>
+      <c r="AF26" s="31"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" customWidth="1"/>
-    <col min="12" max="12" width="10.1640625" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="50" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="26"/>
+      <c r="C1" s="32"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2922,10 +2772,10 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2938,10 +2788,10 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -2954,7 +2804,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -2972,7 +2822,7 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2990,7 +2840,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3010,7 +2860,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3026,7 +2876,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
@@ -3044,20 +2894,20 @@
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="27" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="27" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -3072,35 +2922,35 @@
       <c r="I9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="L9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="34" t="s">
         <v>42</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="28"/>
-    </row>
-    <row r="10" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
+      <c r="X9" s="35"/>
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="35"/>
+    </row>
+    <row r="10" customFormat="false" ht="13" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
         <v>44</v>
       </c>
@@ -3112,29 +2962,29 @@
         <v>46</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="29">
+      <c r="F10" s="36" t="n">
         <v>43845</v>
       </c>
-      <c r="G10" s="30">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="H10" s="29">
+      <c r="G10" s="37" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H10" s="36" t="n">
         <v>43846</v>
       </c>
-      <c r="I10" s="30">
-        <v>0.74305555555555602</v>
+      <c r="I10" s="37" t="n">
+        <v>0.743055555555556</v>
       </c>
       <c r="J10" s="13"/>
-      <c r="K10" s="31" t="s">
+      <c r="K10" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="32" t="s">
+      <c r="L10" s="39" t="s">
         <v>48</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="11" customFormat="false" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -3150,23 +3000,23 @@
       <c r="E11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="40" t="n">
         <v>43845</v>
       </c>
-      <c r="G11" s="34">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="H11" s="33">
+      <c r="G11" s="41" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H11" s="40" t="n">
         <v>43845</v>
       </c>
-      <c r="I11" s="34">
-        <v>0.60416666666666696</v>
-      </c>
-      <c r="J11" s="35" t="s">
+      <c r="I11" s="41" t="n">
+        <v>0.604166666666667</v>
+      </c>
+      <c r="J11" s="42" t="s">
         <v>52</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="36" t="s">
+      <c r="L11" s="43" t="s">
         <v>48</v>
       </c>
       <c r="M11" s="8" t="s">
@@ -3176,7 +3026,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="12" customFormat="false" ht="14" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -3192,23 +3042,23 @@
       <c r="E12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="40" t="n">
         <v>43846</v>
       </c>
-      <c r="G12" s="34">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="H12" s="33">
+      <c r="G12" s="41" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H12" s="40" t="n">
         <v>43846</v>
       </c>
-      <c r="I12" s="34">
-        <v>0.74305555555555602</v>
-      </c>
-      <c r="J12" s="35" t="s">
+      <c r="I12" s="41" t="n">
+        <v>0.743055555555556</v>
+      </c>
+      <c r="J12" s="42" t="s">
         <v>57</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="L12" s="37">
+      <c r="L12" s="44" t="n">
         <v>33.58</v>
       </c>
       <c r="M12" s="8" t="s">
@@ -3217,36 +3067,44 @@
       <c r="N12" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="52" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="16.5" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="43.6640625" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="43.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3280,7 +3138,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3312,7 +3170,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3344,7 +3202,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3378,7 +3236,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3414,7 +3272,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3450,7 +3308,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3482,7 +3340,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>59</v>
       </c>
@@ -3516,20 +3374,20 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="27" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="27" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -3544,16 +3402,16 @@
       <c r="I9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="L9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="34" t="s">
         <v>60</v>
       </c>
       <c r="N9" s="14" t="s">
@@ -3577,35 +3435,43 @@
       <c r="AD9" s="14"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="28.5" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" customWidth="1"/>
-    <col min="12" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="48.33203125" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="48.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3641,7 +3507,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3675,7 +3541,7 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
-    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3709,7 +3575,7 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3725,7 +3591,7 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
-      <c r="N4" s="19"/>
+      <c r="N4" s="23"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -3745,7 +3611,7 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
-    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3781,7 +3647,7 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
-    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3819,7 +3685,7 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
-    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3853,7 +3719,7 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>62</v>
       </c>
@@ -3869,7 +3735,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-      <c r="N8" s="19"/>
+      <c r="N8" s="23"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -3889,47 +3755,47 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="22" t="s">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="22" t="s">
+      <c r="N9" s="27" t="s">
         <v>43</v>
       </c>
       <c r="O9" s="1"/>
@@ -3952,38 +3818,46 @@
       <c r="AF9" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="11" width="15.5" customWidth="1"/>
-    <col min="12" max="12" width="13.5" customWidth="1"/>
-    <col min="13" max="13" width="19.1640625" customWidth="1"/>
-    <col min="14" max="14" width="50.1640625" customWidth="1"/>
-    <col min="15" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4017,7 +3891,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -4049,7 +3923,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4081,7 +3955,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4115,7 +3989,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4149,7 +4023,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>63</v>
       </c>
@@ -4185,7 +4059,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4217,7 +4091,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>64</v>
       </c>
@@ -4251,51 +4125,51 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="34" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="34" t="s">
         <v>60</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>43</v>
       </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="25"/>
+      <c r="P9" s="31"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -4312,40 +4186,48 @@
       <c r="AD9" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="40.83203125" customWidth="1"/>
-    <col min="12" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="45"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4375,7 +4257,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4406,7 +4288,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4438,7 +4320,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4451,7 +4333,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="39"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -4472,7 +4354,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4506,7 +4388,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4542,7 +4424,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4574,7 +4456,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>65</v>
       </c>
@@ -4587,7 +4469,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="39"/>
+      <c r="K8" s="46"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -4608,7 +4490,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>29</v>
       </c>
@@ -4624,26 +4506,26 @@
       <c r="E9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="J9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="48" t="s">
         <v>43</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="23"/>
+      <c r="M9" s="28"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -4662,42 +4544,50 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="38.5" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="40.83203125" customWidth="1"/>
-    <col min="12" max="1025" width="14.5" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="45"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4727,7 +4617,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4758,7 +4648,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4790,7 +4680,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -4803,7 +4693,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="39"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -4824,7 +4714,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4858,7 +4748,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4894,7 +4784,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4926,7 +4816,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>69</v>
       </c>
@@ -4939,7 +4829,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="39"/>
+      <c r="K8" s="46"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -4960,7 +4850,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>30</v>
       </c>
@@ -4976,14 +4866,14 @@
       <c r="E9" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="41"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="48"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="23"/>
+      <c r="M9" s="28"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -5002,62 +4892,70 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="37.5" customWidth="1"/>
-    <col min="3" max="3" width="38.33203125" customWidth="1"/>
-    <col min="4" max="4" width="43.1640625" customWidth="1"/>
-    <col min="5" max="1025" width="10.6640625" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.66"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -5068,7 +4966,12 @@
       <c r="D6" s="7"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
P4-2551 further small tweaks.  Also includes fix to test working with dates.
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Standard" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Long haul" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Redirections" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Lockouts" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Lockouts" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Long haul" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Redirections" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Multi-type" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Cancelled" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Journeys" sheetId="8" state="visible" r:id="rId9"/>
@@ -163,19 +163,44 @@
     <t xml:space="preserve">NOMIS Prison ID</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">LOCKOUTS </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(refused admission to prison)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contractor Billable?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">LONG HAUL</t>
   </si>
   <si>
     <t xml:space="preserve">Move ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Vehicle Reg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Billable?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
   </si>
   <si>
     <t xml:space="preserve">MX1234</t>
@@ -242,32 +267,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Contractor Billable?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Notes (Reason codes or supplier notes)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LOCKOUTS </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(refused admission to prison)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -670,12 +670,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -720,10 +724,6 @@
     </xf>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -817,8 +817,8 @@
   </sheetPr>
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1068,7 +1068,7 @@
       <c r="Z8" s="10"/>
       <c r="AA8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="24.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
@@ -1795,7 +1795,7 @@
   <dimension ref="A1:AF26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1817,15 +1817,15 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -1852,15 +1852,15 @@
       <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -1881,14 +1881,15 @@
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -1911,14 +1912,15 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -1939,14 +1941,15 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -1967,14 +1970,15 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -2711,776 +2715,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA12"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="7"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="N9" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
-      <c r="T9" s="34"/>
-      <c r="U9" s="34"/>
-      <c r="V9" s="34"/>
-      <c r="W9" s="34"/>
-      <c r="X9" s="34"/>
-      <c r="Y9" s="34"/>
-      <c r="Z9" s="34"/>
-    </row>
-    <row r="10" customFormat="false" ht="12" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="35" t="n">
-        <v>43845</v>
-      </c>
-      <c r="G10" s="36" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="H10" s="35" t="n">
-        <v>43846</v>
-      </c>
-      <c r="I10" s="36" t="n">
-        <v>0.743055555555556</v>
-      </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="M10" s="14"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="12" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="39" t="n">
-        <v>43845</v>
-      </c>
-      <c r="G11" s="40" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="H11" s="39" t="n">
-        <v>43845</v>
-      </c>
-      <c r="I11" s="40" t="n">
-        <v>0.604166666666667</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="M11" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="39" t="n">
-        <v>43846</v>
-      </c>
-      <c r="G12" s="40" t="n">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="H12" s="39" t="n">
-        <v>43846</v>
-      </c>
-      <c r="I12" s="40" t="n">
-        <v>0.743055555555556</v>
-      </c>
-      <c r="J12" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="44" t="n">
-        <v>33.58</v>
-      </c>
-      <c r="M12" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="N12" s="3"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AD9"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="43.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="7"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="N9" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="15"/>
-      <c r="AB9" s="15"/>
-      <c r="AC9" s="15"/>
-      <c r="AD9" s="15"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:AF9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3504,15 +2742,15 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -3539,15 +2777,15 @@
       <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -3568,14 +2806,15 @@
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -3598,14 +2837,15 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -3626,14 +2866,15 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -3654,14 +2895,15 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -3712,7 +2954,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -3726,7 +2968,7 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="45"/>
+      <c r="N8" s="32"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -3775,7 +3017,7 @@
         <v>35</v>
       </c>
       <c r="J9" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K9" s="28" t="s">
         <v>37</v>
@@ -3784,10 +3026,10 @@
         <v>9</v>
       </c>
       <c r="M9" s="33" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="N9" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
@@ -3819,32 +3061,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD9"/>
+  <dimension ref="A1:AA12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="15.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
@@ -3854,15 +3096,15 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -3889,15 +3131,15 @@
       <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -3918,14 +3160,15 @@
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -3948,14 +3191,15 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -3976,14 +3220,15 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -4004,14 +3249,441 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+    </row>
+    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
+      <c r="X9" s="35"/>
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="35"/>
+    </row>
+    <row r="10" customFormat="false" ht="12" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="36" t="n">
+        <v>43845</v>
+      </c>
+      <c r="G10" s="37" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H10" s="36" t="n">
+        <v>43846</v>
+      </c>
+      <c r="I10" s="37" t="n">
+        <v>0.743055555555556</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" s="14"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="12" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="40" t="n">
+        <v>43845</v>
+      </c>
+      <c r="G11" s="41" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H11" s="40" t="n">
+        <v>43845</v>
+      </c>
+      <c r="I11" s="41" t="n">
+        <v>0.604166666666667</v>
+      </c>
+      <c r="J11" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="M11" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="40" t="n">
+        <v>43846</v>
+      </c>
+      <c r="G12" s="41" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H12" s="40" t="n">
+        <v>43846</v>
+      </c>
+      <c r="I12" s="41" t="n">
+        <v>0.743055555555556</v>
+      </c>
+      <c r="J12" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="45" t="n">
+        <v>33.58</v>
+      </c>
+      <c r="M12" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="N12" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AD9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="43.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -4060,7 +3732,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -4075,8 +3747,8 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
@@ -4094,63 +3766,63 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="15" t="s">
         <v>35</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K9" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="33" t="s">
+      <c r="L9" s="29" t="s">
         <v>9</v>
       </c>
       <c r="M9" s="33" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="O9" s="3"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="15"/>
+      <c r="AC9" s="15"/>
+      <c r="AD9" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4163,31 +3835,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD10"/>
+  <dimension ref="A1:AD9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4196,15 +3870,15 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -4231,15 +3905,15 @@
       <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -4260,14 +3934,15 @@
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -4290,14 +3965,15 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -4318,14 +3994,15 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -4346,14 +4023,15 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -4402,7 +4080,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -4413,12 +4091,12 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
@@ -4434,45 +4112,51 @@
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="33" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="28" t="s">
+      <c r="F9" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="L9" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="3"/>
+      <c r="M9" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>41</v>
+      </c>
       <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
+      <c r="P9" s="31"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
@@ -4488,7 +4172,6 @@
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4500,7 +4183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4508,16 +4191,16 @@
   <dimension ref="A1:AD10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
@@ -4533,12 +4216,12 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -4568,12 +4251,12 @@
       <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -4597,11 +4280,12 @@
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
       <c r="E3" s="7"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -4627,11 +4311,12 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -4655,11 +4340,12 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
@@ -4683,11 +4369,12 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -4738,8 +4425,8 @@
       <c r="AD7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>66</v>
+      <c r="A8" s="26" t="s">
+        <v>62</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -4773,6 +4460,299 @@
     </row>
     <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AD10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="7"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -4833,7 +4813,7 @@
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
P4-2551 fixes issue with the default tab when opening the spreadsheet. Should now show the summary tab on first opening.
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -817,7 +817,7 @@
   </sheetPr>
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -4531,7 +4531,7 @@
   </sheetPr>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
P4-2551 fixes issue with the default tab when opening the spreadsheet. Should now show the summary tab on first opening. (#168)
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -817,7 +817,7 @@
   </sheetPr>
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -4531,7 +4531,7 @@
   </sheetPr>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove extra row between header and data in most tabs in download sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="56">
   <si>
     <t>Calculate Journey Variable Payments (S2B)</t>
   </si>
@@ -193,48 +193,6 @@
     <t>Billable?</t>
   </si>
   <si>
-    <t>MX1234</t>
-  </si>
-  <si>
-    <t>BRADFORD POLICE STATION (TRAFALGAR HOUSE)</t>
-  </si>
-  <si>
-    <t>LEEDS MAGISTRATES COURT</t>
-  </si>
-  <si>
-    <t>XXX9876</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>Journey 1</t>
-  </si>
-  <si>
-    <t>PS</t>
-  </si>
-  <si>
-    <t>DERBY POLICE CUSTODY</t>
-  </si>
-  <si>
-    <t>GD-5555</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>Long journey, ovenight stay.</t>
-  </si>
-  <si>
-    <t>Journey 2</t>
-  </si>
-  <si>
-    <t>MC</t>
-  </si>
-  <si>
-    <t>XX-5786</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -372,7 +330,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,18 +373,6 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEFEFEF"/>
-        <bgColor rgb="FFEFEFEF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFCC0000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border/>
@@ -440,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -537,35 +483,20 @@
     <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -6221,120 +6152,52 @@
       <c r="Y9" s="15"/>
       <c r="Z9" s="15"/>
     </row>
-    <row r="10" ht="12.0" hidden="1" customHeight="1">
-      <c r="A10" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="32">
-        <v>43845.0</v>
-      </c>
-      <c r="G10" s="33">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="H10" s="32">
-        <v>43846.0</v>
-      </c>
-      <c r="I10" s="33">
-        <v>0.743055555555556</v>
-      </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="L10" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="M10" s="14"/>
+    <row r="10" ht="12.0" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" ht="12.0" hidden="1" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="36">
-        <v>43845.0</v>
-      </c>
-      <c r="G11" s="37">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="H11" s="36">
-        <v>43845.0</v>
-      </c>
-      <c r="I11" s="37">
-        <v>0.604166666666667</v>
-      </c>
-      <c r="J11" s="38" t="s">
-        <v>53</v>
-      </c>
+    <row r="11" ht="12.0" customHeight="1">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="35"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="M11" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="L11" s="34"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="3"/>
     </row>
-    <row r="12" ht="12.0" hidden="1" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="36">
-        <v>43846.0</v>
-      </c>
-      <c r="G12" s="37">
-        <v>0.333333333333333</v>
-      </c>
-      <c r="H12" s="36">
-        <v>43846.0</v>
-      </c>
-      <c r="I12" s="37">
-        <v>0.743055555555556</v>
-      </c>
-      <c r="J12" s="38" t="s">
-        <v>58</v>
-      </c>
+    <row r="12" ht="12.0" customHeight="1">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="35"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="41">
-        <v>33.58</v>
-      </c>
-      <c r="M12" s="40" t="s">
-        <v>54</v>
-      </c>
+      <c r="L12" s="34"/>
+      <c r="M12" s="36"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" ht="12.0" customHeight="1"/>
@@ -7573,7 +7436,7 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -7646,7 +7509,7 @@
         <v>40</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
@@ -8906,7 +8769,7 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -10237,7 +10100,7 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -10248,7 +10111,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="42"/>
+      <c r="K8" s="37"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -10285,14 +10148,14 @@
       <c r="E9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="43" t="s">
-        <v>65</v>
+      <c r="F9" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>51</v>
       </c>
       <c r="I9" s="25" t="s">
         <v>37</v>
@@ -10300,7 +10163,7 @@
       <c r="J9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="44" t="s">
+      <c r="K9" s="39" t="s">
         <v>41</v>
       </c>
       <c r="L9" s="3"/>
@@ -11504,7 +11367,7 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -11533,20 +11396,20 @@
         <v>31</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
+        <v>55</v>
+      </c>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
       <c r="I9" s="25"/>
       <c r="J9" s="26"/>
-      <c r="K9" s="44"/>
+      <c r="K9" s="39"/>
       <c r="L9" s="3"/>
       <c r="M9" s="25"/>
       <c r="N9" s="3"/>
@@ -12747,18 +12610,18 @@
     </row>
     <row r="7" ht="12.0" customHeight="1"/>
     <row r="8" ht="12.0" customHeight="1"/>
-    <row r="9" ht="12.0" customHeight="1"/>
-    <row r="10" ht="12.0" customHeight="1">
-      <c r="A10" s="45" t="s">
+    <row r="9" ht="12.0" customHeight="1">
+      <c r="A9" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B9" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="45" t="s">
-        <v>68</v>
+      <c r="C9" s="40" t="s">
+        <v>54</v>
       </c>
     </row>
+    <row r="10" ht="12.0" customHeight="1"/>
     <row r="11" ht="12.0" customHeight="1"/>
     <row r="12" ht="12.0" customHeight="1"/>
     <row r="13" ht="12.0" customHeight="1"/>

</xml_diff>

<commit_message>
Add Billable journey count to Journeys tab in download sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -17,14 +17,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mi0n/zTwy/rSaR3OX/8pScEZh/4lQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mhf6KaviNSFEQVjUwiLv57fp3v1eg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="57">
   <si>
     <t>Calculate Journey Variable Payments (S2B)</t>
   </si>
@@ -268,6 +268,9 @@
     <t>Total journey count</t>
   </si>
   <si>
+    <t>Billable journeys count</t>
+  </si>
+  <si>
     <t>Unit price</t>
   </si>
   <si>
@@ -386,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -471,6 +474,9 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -506,6 +512,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -2643,8 +2652,8 @@
     <col customWidth="1" min="4" max="4" width="31.14"/>
     <col customWidth="1" min="5" max="5" width="16.29"/>
     <col customWidth="1" min="6" max="9" width="14.43"/>
-    <col customWidth="1" min="10" max="10" width="19.43"/>
-    <col customWidth="1" min="11" max="11" width="15.43"/>
+    <col customWidth="1" min="10" max="10" width="11.86"/>
+    <col customWidth="1" min="11" max="11" width="16.29"/>
     <col customWidth="1" min="12" max="32" width="14.43"/>
   </cols>
   <sheetData>
@@ -2968,7 +2977,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="J10" s="28"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -3125,8 +3134,8 @@
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
-      <c r="AE14" s="28"/>
-      <c r="AF14" s="28"/>
+      <c r="AE14" s="29"/>
+      <c r="AF14" s="29"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3"/>
@@ -3193,8 +3202,8 @@
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
-      <c r="AE16" s="28"/>
-      <c r="AF16" s="28"/>
+      <c r="AE16" s="29"/>
+      <c r="AF16" s="29"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="3"/>
@@ -3329,8 +3338,8 @@
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
-      <c r="AE20" s="28"/>
-      <c r="AF20" s="28"/>
+      <c r="AE20" s="29"/>
+      <c r="AF20" s="29"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
@@ -3397,8 +3406,8 @@
       <c r="AB22" s="3"/>
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
-      <c r="AE22" s="28"/>
-      <c r="AF22" s="28"/>
+      <c r="AE22" s="29"/>
+      <c r="AF22" s="29"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="3"/>
@@ -3431,8 +3440,8 @@
       <c r="AB23" s="3"/>
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
-      <c r="AE23" s="28"/>
-      <c r="AF23" s="28"/>
+      <c r="AE23" s="29"/>
+      <c r="AF23" s="29"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="3"/>
@@ -3465,8 +3474,8 @@
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
-      <c r="AE24" s="28"/>
-      <c r="AF24" s="28"/>
+      <c r="AE24" s="29"/>
+      <c r="AF24" s="29"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="3"/>
@@ -3499,8 +3508,8 @@
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
-      <c r="AE25" s="28"/>
-      <c r="AF25" s="28"/>
+      <c r="AE25" s="29"/>
+      <c r="AF25" s="29"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3"/>
@@ -3533,8 +3542,8 @@
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
-      <c r="AE26" s="28"/>
-      <c r="AF26" s="28"/>
+      <c r="AE26" s="29"/>
+      <c r="AF26" s="29"/>
     </row>
     <row r="27" ht="12.0" customHeight="1"/>
     <row r="28" ht="12.0" customHeight="1"/>
@@ -4530,13 +4539,14 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="49.43"/>
-    <col customWidth="1" min="3" max="3" width="13.43"/>
+    <col customWidth="1" min="3" max="3" width="15.14"/>
     <col customWidth="1" min="4" max="4" width="28.43"/>
-    <col customWidth="1" min="5" max="5" width="11.29"/>
+    <col customWidth="1" min="5" max="5" width="13.86"/>
     <col customWidth="1" min="6" max="9" width="14.43"/>
-    <col customWidth="1" min="10" max="10" width="17.71"/>
-    <col customWidth="1" min="11" max="11" width="15.71"/>
-    <col customWidth="1" min="12" max="13" width="14.43"/>
+    <col customWidth="1" min="10" max="10" width="11.86"/>
+    <col customWidth="1" min="11" max="11" width="16.29"/>
+    <col customWidth="1" min="12" max="12" width="14.43"/>
+    <col customWidth="1" min="13" max="13" width="19.29"/>
     <col customWidth="1" min="14" max="14" width="48.29"/>
     <col customWidth="1" min="15" max="32" width="14.43"/>
   </cols>
@@ -4773,7 +4783,7 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="29"/>
+      <c r="N8" s="30"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -4827,10 +4837,10 @@
       <c r="K9" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="31" t="s">
         <v>40</v>
       </c>
       <c r="N9" s="24" t="s">
@@ -5871,9 +5881,9 @@
     <col customWidth="1" min="5" max="6" width="15.86"/>
     <col customWidth="1" min="7" max="7" width="12.43"/>
     <col customWidth="1" min="8" max="8" width="14.43"/>
-    <col customWidth="1" min="9" max="9" width="12.14"/>
-    <col customWidth="1" min="10" max="10" width="13.14"/>
-    <col customWidth="1" min="11" max="11" width="16.86"/>
+    <col customWidth="1" min="9" max="9" width="13.0"/>
+    <col customWidth="1" min="10" max="10" width="11.86"/>
+    <col customWidth="1" min="11" max="11" width="16.29"/>
     <col customWidth="1" min="12" max="12" width="10.14"/>
     <col customWidth="1" min="13" max="13" width="12.71"/>
     <col customWidth="1" min="14" max="14" width="50.0"/>
@@ -6079,7 +6089,7 @@
       <c r="N7" s="3"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="32" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="9"/>
@@ -6133,7 +6143,7 @@
       <c r="L9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="31" t="s">
         <v>44</v>
       </c>
       <c r="N9" s="15" t="s">
@@ -6158,13 +6168,13 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="34"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
@@ -6174,14 +6184,14 @@
       <c r="C11" s="22"/>
       <c r="D11" s="3"/>
       <c r="E11" s="22"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="35"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="36"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="36"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="37"/>
       <c r="N11" s="3"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
@@ -6190,14 +6200,14 @@
       <c r="C12" s="22"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="35"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="36"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="36"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="37"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" ht="12.0" customHeight="1"/>
@@ -7208,14 +7218,14 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="52.0"/>
-    <col customWidth="1" min="3" max="3" width="13.14"/>
+    <col customWidth="1" min="3" max="3" width="15.14"/>
     <col customWidth="1" min="4" max="4" width="33.71"/>
-    <col customWidth="1" min="5" max="5" width="14.0"/>
+    <col customWidth="1" min="5" max="5" width="13.86"/>
     <col customWidth="1" min="6" max="9" width="14.43"/>
-    <col customWidth="1" min="10" max="10" width="16.43"/>
-    <col customWidth="1" min="11" max="11" width="19.71"/>
+    <col customWidth="1" min="10" max="10" width="11.86"/>
+    <col customWidth="1" min="11" max="11" width="16.29"/>
     <col customWidth="1" min="12" max="12" width="12.0"/>
-    <col customWidth="1" min="13" max="13" width="15.71"/>
+    <col customWidth="1" min="13" max="13" width="19.29"/>
     <col customWidth="1" min="14" max="14" width="43.71"/>
     <col customWidth="1" min="15" max="30" width="14.43"/>
   </cols>
@@ -7505,7 +7515,7 @@
       <c r="L9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="31" t="s">
         <v>40</v>
       </c>
       <c r="N9" s="15" t="s">
@@ -8539,16 +8549,16 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="66.71"/>
-    <col customWidth="1" min="3" max="3" width="13.0"/>
+    <col customWidth="1" min="3" max="3" width="15.14"/>
     <col customWidth="1" min="4" max="4" width="30.14"/>
-    <col customWidth="1" min="5" max="5" width="13.43"/>
-    <col customWidth="1" min="6" max="6" width="13.86"/>
+    <col customWidth="1" min="5" max="6" width="13.86"/>
     <col customWidth="1" min="7" max="7" width="12.86"/>
     <col customWidth="1" min="8" max="8" width="13.14"/>
     <col customWidth="1" min="9" max="9" width="14.43"/>
-    <col customWidth="1" min="10" max="11" width="15.43"/>
+    <col customWidth="1" min="10" max="10" width="11.86"/>
+    <col customWidth="1" min="11" max="11" width="16.29"/>
     <col customWidth="1" min="12" max="12" width="13.43"/>
-    <col customWidth="1" min="13" max="13" width="19.14"/>
+    <col customWidth="1" min="13" max="13" width="19.29"/>
     <col customWidth="1" min="14" max="14" width="50.14"/>
     <col customWidth="1" min="15" max="30" width="14.43"/>
   </cols>
@@ -8808,13 +8818,13 @@
       <c r="B9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="31" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="24" t="s">
@@ -8835,17 +8845,17 @@
       <c r="K9" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="31" t="s">
         <v>40</v>
       </c>
       <c r="N9" s="15" t="s">
         <v>41</v>
       </c>
       <c r="O9" s="3"/>
-      <c r="P9" s="28"/>
+      <c r="P9" s="29"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
@@ -9872,13 +9882,13 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="49.43"/>
-    <col customWidth="1" min="3" max="3" width="15.43"/>
+    <col customWidth="1" min="3" max="3" width="15.14"/>
     <col customWidth="1" min="4" max="4" width="31.14"/>
-    <col customWidth="1" min="5" max="5" width="14.14"/>
+    <col customWidth="1" min="5" max="5" width="13.86"/>
     <col customWidth="1" min="6" max="6" width="14.43"/>
     <col customWidth="1" min="7" max="7" width="17.71"/>
-    <col customWidth="1" min="8" max="8" width="16.29"/>
-    <col customWidth="1" min="9" max="9" width="15.86"/>
+    <col customWidth="1" min="8" max="8" width="16.86"/>
+    <col customWidth="1" min="9" max="9" width="16.29"/>
     <col customWidth="1" min="10" max="10" width="14.43"/>
     <col customWidth="1" min="11" max="11" width="40.86"/>
     <col customWidth="1" min="12" max="30" width="14.43"/>
@@ -10111,7 +10121,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="37"/>
+      <c r="K8" s="38"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -10148,13 +10158,13 @@
       <c r="E9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="39" t="s">
         <v>51</v>
       </c>
       <c r="I9" s="25" t="s">
@@ -10163,7 +10173,7 @@
       <c r="J9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="39" t="s">
+      <c r="K9" s="40" t="s">
         <v>41</v>
       </c>
       <c r="L9" s="3"/>
@@ -11197,17 +11207,18 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="35.0"/>
     <col customWidth="1" min="2" max="2" width="38.43"/>
-    <col customWidth="1" min="3" max="3" width="18.29"/>
-    <col customWidth="1" min="4" max="4" width="14.71"/>
-    <col customWidth="1" min="5" max="5" width="13.71"/>
-    <col customWidth="1" min="6" max="6" width="14.43"/>
-    <col customWidth="1" min="7" max="7" width="17.71"/>
-    <col customWidth="1" min="8" max="8" width="16.29"/>
-    <col customWidth="1" min="9" max="9" width="15.86"/>
-    <col customWidth="1" min="10" max="10" width="14.43"/>
-    <col customWidth="1" min="11" max="11" width="40.86"/>
-    <col customWidth="1" min="12" max="25" width="14.43"/>
-    <col customWidth="1" min="26" max="26" width="8.71"/>
+    <col customWidth="1" min="3" max="3" width="18.71"/>
+    <col customWidth="1" min="4" max="4" width="22.14"/>
+    <col customWidth="1" min="5" max="5" width="14.71"/>
+    <col customWidth="1" min="6" max="6" width="13.71"/>
+    <col customWidth="1" min="7" max="7" width="14.43"/>
+    <col customWidth="1" min="8" max="8" width="17.71"/>
+    <col customWidth="1" min="9" max="9" width="16.29"/>
+    <col customWidth="1" min="10" max="10" width="15.86"/>
+    <col customWidth="1" min="11" max="11" width="14.43"/>
+    <col customWidth="1" min="12" max="12" width="40.86"/>
+    <col customWidth="1" min="13" max="26" width="14.43"/>
+    <col customWidth="1" min="27" max="27" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -11216,7 +11227,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="L1" s="3"/>
+      <c r="F1" s="2"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -11230,6 +11241,7 @@
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
@@ -11243,7 +11255,7 @@
       <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="3"/>
+      <c r="F2" s="4"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -11257,14 +11269,15 @@
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="7"/>
-      <c r="L3" s="3"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="7"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
@@ -11275,9 +11288,10 @@
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
-      <c r="W3" s="8"/>
+      <c r="W3" s="3"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
@@ -11287,7 +11301,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="L4" s="3"/>
+      <c r="F4" s="5"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -11301,6 +11315,7 @@
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="5"/>
@@ -11308,7 +11323,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="L5" s="3"/>
+      <c r="F5" s="5"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -11322,6 +11337,7 @@
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="5"/>
@@ -11329,7 +11345,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="L6" s="3"/>
+      <c r="F6" s="5"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -11343,6 +11359,7 @@
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3"/>
@@ -11350,7 +11367,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="F7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -11364,6 +11381,7 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -11373,7 +11391,7 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="L8" s="3"/>
+      <c r="F8" s="9"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
@@ -11387,6 +11405,7 @@
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
     </row>
     <row r="9" ht="17.25" customHeight="1">
       <c r="A9" s="15" t="s">
@@ -11398,21 +11417,23 @@
       <c r="C9" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="41" t="s">
         <v>54</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="3"/>
+      <c r="F9" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="25"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
@@ -11424,6 +11445,7 @@
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
     </row>
     <row r="10" ht="15.75" customHeight="1"/>
     <row r="11" ht="12.0" customHeight="1"/>
@@ -12436,7 +12458,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="35.86"/>
     <col customWidth="1" min="2" max="2" width="37.43"/>
-    <col customWidth="1" min="3" max="3" width="17.14"/>
+    <col customWidth="1" min="3" max="3" width="15.14"/>
     <col customWidth="1" min="4" max="4" width="11.57"/>
     <col customWidth="1" min="5" max="25" width="10.71"/>
     <col customWidth="1" min="26" max="26" width="8.71"/>
@@ -12611,14 +12633,14 @@
     <row r="7" ht="12.0" customHeight="1"/>
     <row r="8" ht="12.0" customHeight="1"/>
     <row r="9" ht="12.0" customHeight="1">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="40" t="s">
-        <v>54</v>
+      <c r="C9" s="42" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" ht="12.0" customHeight="1"/>

</xml_diff>

<commit_message>
Add locations to download spreadsheet
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -12,19 +12,20 @@
     <sheet state="visible" name="Cancelled" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="Journeys" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="JPC Price book" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Locations" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mhf6KaviNSFEQVjUwiLv57fp3v1eg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mjzzXmz8O8REGjAAviJultF+4l2uA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="60">
   <si>
     <t>Calculate Journey Variable Payments (S2B)</t>
   </si>
@@ -276,6 +277,15 @@
   <si>
     <t>Total price</t>
   </si>
+  <si>
+    <t>Nomis Agency ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
 </sst>
 </file>
 
@@ -389,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -474,9 +484,6 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -513,9 +520,7 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -528,6 +533,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -769,9 +778,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="35.71"/>
     <col customWidth="1" min="2" max="2" width="16.14"/>
-    <col customWidth="1" min="3" max="4" width="14.43"/>
     <col customWidth="1" min="5" max="5" width="16.14"/>
-    <col customWidth="1" min="6" max="25" width="14.43"/>
     <col customWidth="1" min="26" max="26" width="8.71"/>
   </cols>
   <sheetData>
@@ -2636,6 +2643,1202 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="35.86"/>
+    <col customWidth="1" min="2" max="2" width="37.43"/>
+    <col customWidth="1" min="3" max="3" width="15.14"/>
+    <col customWidth="1" min="4" max="4" width="11.57"/>
+    <col customWidth="1" min="5" max="25" width="10.71"/>
+    <col customWidth="1" min="26" max="26" width="8.71"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="7"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+    </row>
+    <row r="7" ht="12.0" customHeight="1"/>
+    <row r="8" ht="12.0" customHeight="1"/>
+    <row r="9" ht="12.0" customHeight="1">
+      <c r="A9" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" ht="12.0" customHeight="1"/>
+    <row r="11" ht="12.0" customHeight="1"/>
+    <row r="12" ht="12.0" customHeight="1"/>
+    <row r="13" ht="12.0" customHeight="1"/>
+    <row r="14" ht="12.0" customHeight="1"/>
+    <row r="15" ht="12.0" customHeight="1"/>
+    <row r="16" ht="12.0" customHeight="1"/>
+    <row r="17" ht="12.0" customHeight="1"/>
+    <row r="18" ht="12.0" customHeight="1"/>
+    <row r="19" ht="12.0" customHeight="1"/>
+    <row r="20" ht="12.0" customHeight="1"/>
+    <row r="21" ht="12.0" customHeight="1"/>
+    <row r="22" ht="12.0" customHeight="1"/>
+    <row r="23" ht="12.0" customHeight="1"/>
+    <row r="24" ht="12.0" customHeight="1"/>
+    <row r="25" ht="12.0" customHeight="1"/>
+    <row r="26" ht="12.0" customHeight="1"/>
+    <row r="27" ht="12.0" customHeight="1"/>
+    <row r="28" ht="12.0" customHeight="1"/>
+    <row r="29" ht="12.0" customHeight="1"/>
+    <row r="30" ht="12.0" customHeight="1"/>
+    <row r="31" ht="12.0" customHeight="1"/>
+    <row r="32" ht="12.0" customHeight="1"/>
+    <row r="33" ht="12.0" customHeight="1"/>
+    <row r="34" ht="12.0" customHeight="1"/>
+    <row r="35" ht="12.0" customHeight="1"/>
+    <row r="36" ht="12.0" customHeight="1"/>
+    <row r="37" ht="12.0" customHeight="1"/>
+    <row r="38" ht="12.0" customHeight="1"/>
+    <row r="39" ht="12.0" customHeight="1"/>
+    <row r="40" ht="12.0" customHeight="1"/>
+    <row r="41" ht="12.0" customHeight="1"/>
+    <row r="42" ht="12.0" customHeight="1"/>
+    <row r="43" ht="12.0" customHeight="1"/>
+    <row r="44" ht="12.0" customHeight="1"/>
+    <row r="45" ht="12.0" customHeight="1"/>
+    <row r="46" ht="12.0" customHeight="1"/>
+    <row r="47" ht="12.0" customHeight="1"/>
+    <row r="48" ht="12.0" customHeight="1"/>
+    <row r="49" ht="12.0" customHeight="1"/>
+    <row r="50" ht="12.0" customHeight="1"/>
+    <row r="51" ht="12.0" customHeight="1"/>
+    <row r="52" ht="12.0" customHeight="1"/>
+    <row r="53" ht="12.0" customHeight="1"/>
+    <row r="54" ht="12.0" customHeight="1"/>
+    <row r="55" ht="12.0" customHeight="1"/>
+    <row r="56" ht="12.0" customHeight="1"/>
+    <row r="57" ht="12.0" customHeight="1"/>
+    <row r="58" ht="12.0" customHeight="1"/>
+    <row r="59" ht="12.0" customHeight="1"/>
+    <row r="60" ht="12.0" customHeight="1"/>
+    <row r="61" ht="12.0" customHeight="1"/>
+    <row r="62" ht="12.0" customHeight="1"/>
+    <row r="63" ht="12.0" customHeight="1"/>
+    <row r="64" ht="12.0" customHeight="1"/>
+    <row r="65" ht="12.0" customHeight="1"/>
+    <row r="66" ht="12.0" customHeight="1"/>
+    <row r="67" ht="12.0" customHeight="1"/>
+    <row r="68" ht="12.0" customHeight="1"/>
+    <row r="69" ht="12.0" customHeight="1"/>
+    <row r="70" ht="12.0" customHeight="1"/>
+    <row r="71" ht="12.0" customHeight="1"/>
+    <row r="72" ht="12.0" customHeight="1"/>
+    <row r="73" ht="12.0" customHeight="1"/>
+    <row r="74" ht="12.0" customHeight="1"/>
+    <row r="75" ht="12.0" customHeight="1"/>
+    <row r="76" ht="12.0" customHeight="1"/>
+    <row r="77" ht="12.0" customHeight="1"/>
+    <row r="78" ht="12.0" customHeight="1"/>
+    <row r="79" ht="12.0" customHeight="1"/>
+    <row r="80" ht="12.0" customHeight="1"/>
+    <row r="81" ht="12.0" customHeight="1"/>
+    <row r="82" ht="12.0" customHeight="1"/>
+    <row r="83" ht="12.0" customHeight="1"/>
+    <row r="84" ht="12.0" customHeight="1"/>
+    <row r="85" ht="12.0" customHeight="1"/>
+    <row r="86" ht="12.0" customHeight="1"/>
+    <row r="87" ht="12.0" customHeight="1"/>
+    <row r="88" ht="12.0" customHeight="1"/>
+    <row r="89" ht="12.0" customHeight="1"/>
+    <row r="90" ht="12.0" customHeight="1"/>
+    <row r="91" ht="12.0" customHeight="1"/>
+    <row r="92" ht="12.0" customHeight="1"/>
+    <row r="93" ht="12.0" customHeight="1"/>
+    <row r="94" ht="12.0" customHeight="1"/>
+    <row r="95" ht="12.0" customHeight="1"/>
+    <row r="96" ht="12.0" customHeight="1"/>
+    <row r="97" ht="12.0" customHeight="1"/>
+    <row r="98" ht="12.0" customHeight="1"/>
+    <row r="99" ht="12.0" customHeight="1"/>
+    <row r="100" ht="12.0" customHeight="1"/>
+    <row r="101" ht="12.0" customHeight="1"/>
+    <row r="102" ht="12.0" customHeight="1"/>
+    <row r="103" ht="12.0" customHeight="1"/>
+    <row r="104" ht="12.0" customHeight="1"/>
+    <row r="105" ht="12.0" customHeight="1"/>
+    <row r="106" ht="12.0" customHeight="1"/>
+    <row r="107" ht="12.0" customHeight="1"/>
+    <row r="108" ht="12.0" customHeight="1"/>
+    <row r="109" ht="12.0" customHeight="1"/>
+    <row r="110" ht="12.0" customHeight="1"/>
+    <row r="111" ht="12.0" customHeight="1"/>
+    <row r="112" ht="12.0" customHeight="1"/>
+    <row r="113" ht="12.0" customHeight="1"/>
+    <row r="114" ht="12.0" customHeight="1"/>
+    <row r="115" ht="12.0" customHeight="1"/>
+    <row r="116" ht="12.0" customHeight="1"/>
+    <row r="117" ht="12.0" customHeight="1"/>
+    <row r="118" ht="12.0" customHeight="1"/>
+    <row r="119" ht="12.0" customHeight="1"/>
+    <row r="120" ht="12.0" customHeight="1"/>
+    <row r="121" ht="12.0" customHeight="1"/>
+    <row r="122" ht="12.0" customHeight="1"/>
+    <row r="123" ht="12.0" customHeight="1"/>
+    <row r="124" ht="12.0" customHeight="1"/>
+    <row r="125" ht="12.0" customHeight="1"/>
+    <row r="126" ht="12.0" customHeight="1"/>
+    <row r="127" ht="12.0" customHeight="1"/>
+    <row r="128" ht="12.0" customHeight="1"/>
+    <row r="129" ht="12.0" customHeight="1"/>
+    <row r="130" ht="12.0" customHeight="1"/>
+    <row r="131" ht="12.0" customHeight="1"/>
+    <row r="132" ht="12.0" customHeight="1"/>
+    <row r="133" ht="12.0" customHeight="1"/>
+    <row r="134" ht="12.0" customHeight="1"/>
+    <row r="135" ht="12.0" customHeight="1"/>
+    <row r="136" ht="12.0" customHeight="1"/>
+    <row r="137" ht="12.0" customHeight="1"/>
+    <row r="138" ht="12.0" customHeight="1"/>
+    <row r="139" ht="12.0" customHeight="1"/>
+    <row r="140" ht="12.0" customHeight="1"/>
+    <row r="141" ht="12.0" customHeight="1"/>
+    <row r="142" ht="12.0" customHeight="1"/>
+    <row r="143" ht="12.0" customHeight="1"/>
+    <row r="144" ht="12.0" customHeight="1"/>
+    <row r="145" ht="12.0" customHeight="1"/>
+    <row r="146" ht="12.0" customHeight="1"/>
+    <row r="147" ht="12.0" customHeight="1"/>
+    <row r="148" ht="12.0" customHeight="1"/>
+    <row r="149" ht="12.0" customHeight="1"/>
+    <row r="150" ht="12.0" customHeight="1"/>
+    <row r="151" ht="12.0" customHeight="1"/>
+    <row r="152" ht="12.0" customHeight="1"/>
+    <row r="153" ht="12.0" customHeight="1"/>
+    <row r="154" ht="12.0" customHeight="1"/>
+    <row r="155" ht="12.0" customHeight="1"/>
+    <row r="156" ht="12.0" customHeight="1"/>
+    <row r="157" ht="12.0" customHeight="1"/>
+    <row r="158" ht="12.0" customHeight="1"/>
+    <row r="159" ht="12.0" customHeight="1"/>
+    <row r="160" ht="12.0" customHeight="1"/>
+    <row r="161" ht="12.0" customHeight="1"/>
+    <row r="162" ht="12.0" customHeight="1"/>
+    <row r="163" ht="12.0" customHeight="1"/>
+    <row r="164" ht="12.0" customHeight="1"/>
+    <row r="165" ht="12.0" customHeight="1"/>
+    <row r="166" ht="12.0" customHeight="1"/>
+    <row r="167" ht="12.0" customHeight="1"/>
+    <row r="168" ht="12.0" customHeight="1"/>
+    <row r="169" ht="12.0" customHeight="1"/>
+    <row r="170" ht="12.0" customHeight="1"/>
+    <row r="171" ht="12.0" customHeight="1"/>
+    <row r="172" ht="12.0" customHeight="1"/>
+    <row r="173" ht="12.0" customHeight="1"/>
+    <row r="174" ht="12.0" customHeight="1"/>
+    <row r="175" ht="12.0" customHeight="1"/>
+    <row r="176" ht="12.0" customHeight="1"/>
+    <row r="177" ht="12.0" customHeight="1"/>
+    <row r="178" ht="12.0" customHeight="1"/>
+    <row r="179" ht="12.0" customHeight="1"/>
+    <row r="180" ht="12.0" customHeight="1"/>
+    <row r="181" ht="12.0" customHeight="1"/>
+    <row r="182" ht="12.0" customHeight="1"/>
+    <row r="183" ht="12.0" customHeight="1"/>
+    <row r="184" ht="12.0" customHeight="1"/>
+    <row r="185" ht="12.0" customHeight="1"/>
+    <row r="186" ht="12.0" customHeight="1"/>
+    <row r="187" ht="12.0" customHeight="1"/>
+    <row r="188" ht="12.0" customHeight="1"/>
+    <row r="189" ht="12.0" customHeight="1"/>
+    <row r="190" ht="12.0" customHeight="1"/>
+    <row r="191" ht="12.0" customHeight="1"/>
+    <row r="192" ht="12.0" customHeight="1"/>
+    <row r="193" ht="12.0" customHeight="1"/>
+    <row r="194" ht="12.0" customHeight="1"/>
+    <row r="195" ht="12.0" customHeight="1"/>
+    <row r="196" ht="12.0" customHeight="1"/>
+    <row r="197" ht="12.0" customHeight="1"/>
+    <row r="198" ht="12.0" customHeight="1"/>
+    <row r="199" ht="12.0" customHeight="1"/>
+    <row r="200" ht="12.0" customHeight="1"/>
+    <row r="201" ht="12.0" customHeight="1"/>
+    <row r="202" ht="12.0" customHeight="1"/>
+    <row r="203" ht="12.0" customHeight="1"/>
+    <row r="204" ht="12.0" customHeight="1"/>
+    <row r="205" ht="12.0" customHeight="1"/>
+    <row r="206" ht="12.0" customHeight="1"/>
+    <row r="207" ht="12.0" customHeight="1"/>
+    <row r="208" ht="12.0" customHeight="1"/>
+    <row r="209" ht="12.0" customHeight="1"/>
+    <row r="210" ht="12.0" customHeight="1"/>
+    <row r="211" ht="12.0" customHeight="1"/>
+    <row r="212" ht="12.0" customHeight="1"/>
+    <row r="213" ht="12.0" customHeight="1"/>
+    <row r="214" ht="12.0" customHeight="1"/>
+    <row r="215" ht="12.0" customHeight="1"/>
+    <row r="216" ht="12.0" customHeight="1"/>
+    <row r="217" ht="12.0" customHeight="1"/>
+    <row r="218" ht="12.0" customHeight="1"/>
+    <row r="219" ht="12.0" customHeight="1"/>
+    <row r="220" ht="12.0" customHeight="1"/>
+    <row r="221" ht="12.0" customHeight="1"/>
+    <row r="222" ht="12.0" customHeight="1"/>
+    <row r="223" ht="12.0" customHeight="1"/>
+    <row r="224" ht="12.0" customHeight="1"/>
+    <row r="225" ht="12.0" customHeight="1"/>
+    <row r="226" ht="12.0" customHeight="1"/>
+    <row r="227" ht="12.0" customHeight="1"/>
+    <row r="228" ht="12.0" customHeight="1"/>
+    <row r="229" ht="12.0" customHeight="1"/>
+    <row r="230" ht="12.0" customHeight="1"/>
+    <row r="231" ht="12.0" customHeight="1"/>
+    <row r="232" ht="12.0" customHeight="1"/>
+    <row r="233" ht="12.0" customHeight="1"/>
+    <row r="234" ht="12.0" customHeight="1"/>
+    <row r="235" ht="12.0" customHeight="1"/>
+    <row r="236" ht="12.0" customHeight="1"/>
+    <row r="237" ht="12.0" customHeight="1"/>
+    <row r="238" ht="12.0" customHeight="1"/>
+    <row r="239" ht="12.0" customHeight="1"/>
+    <row r="240" ht="12.0" customHeight="1"/>
+    <row r="241" ht="12.0" customHeight="1"/>
+    <row r="242" ht="12.0" customHeight="1"/>
+    <row r="243" ht="12.0" customHeight="1"/>
+    <row r="244" ht="12.0" customHeight="1"/>
+    <row r="245" ht="12.0" customHeight="1"/>
+    <row r="246" ht="12.0" customHeight="1"/>
+    <row r="247" ht="12.0" customHeight="1"/>
+    <row r="248" ht="12.0" customHeight="1"/>
+    <row r="249" ht="12.0" customHeight="1"/>
+    <row r="250" ht="12.0" customHeight="1"/>
+    <row r="251" ht="12.0" customHeight="1"/>
+    <row r="252" ht="12.0" customHeight="1"/>
+    <row r="253" ht="12.0" customHeight="1"/>
+    <row r="254" ht="12.0" customHeight="1"/>
+    <row r="255" ht="12.0" customHeight="1"/>
+    <row r="256" ht="12.0" customHeight="1"/>
+    <row r="257" ht="12.0" customHeight="1"/>
+    <row r="258" ht="12.0" customHeight="1"/>
+    <row r="259" ht="12.0" customHeight="1"/>
+    <row r="260" ht="12.0" customHeight="1"/>
+    <row r="261" ht="12.0" customHeight="1"/>
+    <row r="262" ht="12.0" customHeight="1"/>
+    <row r="263" ht="12.0" customHeight="1"/>
+    <row r="264" ht="12.0" customHeight="1"/>
+    <row r="265" ht="12.0" customHeight="1"/>
+    <row r="266" ht="12.0" customHeight="1"/>
+    <row r="267" ht="12.0" customHeight="1"/>
+    <row r="268" ht="12.0" customHeight="1"/>
+    <row r="269" ht="12.0" customHeight="1"/>
+    <row r="270" ht="12.0" customHeight="1"/>
+    <row r="271" ht="12.0" customHeight="1"/>
+    <row r="272" ht="12.0" customHeight="1"/>
+    <row r="273" ht="12.0" customHeight="1"/>
+    <row r="274" ht="12.0" customHeight="1"/>
+    <row r="275" ht="12.0" customHeight="1"/>
+    <row r="276" ht="12.0" customHeight="1"/>
+    <row r="277" ht="12.0" customHeight="1"/>
+    <row r="278" ht="12.0" customHeight="1"/>
+    <row r="279" ht="12.0" customHeight="1"/>
+    <row r="280" ht="12.0" customHeight="1"/>
+    <row r="281" ht="12.0" customHeight="1"/>
+    <row r="282" ht="12.0" customHeight="1"/>
+    <row r="283" ht="12.0" customHeight="1"/>
+    <row r="284" ht="12.0" customHeight="1"/>
+    <row r="285" ht="12.0" customHeight="1"/>
+    <row r="286" ht="12.0" customHeight="1"/>
+    <row r="287" ht="12.0" customHeight="1"/>
+    <row r="288" ht="12.0" customHeight="1"/>
+    <row r="289" ht="12.0" customHeight="1"/>
+    <row r="290" ht="12.0" customHeight="1"/>
+    <row r="291" ht="12.0" customHeight="1"/>
+    <row r="292" ht="12.0" customHeight="1"/>
+    <row r="293" ht="12.0" customHeight="1"/>
+    <row r="294" ht="12.0" customHeight="1"/>
+    <row r="295" ht="12.0" customHeight="1"/>
+    <row r="296" ht="12.0" customHeight="1"/>
+    <row r="297" ht="12.0" customHeight="1"/>
+    <row r="298" ht="12.0" customHeight="1"/>
+    <row r="299" ht="12.0" customHeight="1"/>
+    <row r="300" ht="12.0" customHeight="1"/>
+    <row r="301" ht="12.0" customHeight="1"/>
+    <row r="302" ht="12.0" customHeight="1"/>
+    <row r="303" ht="12.0" customHeight="1"/>
+    <row r="304" ht="12.0" customHeight="1"/>
+    <row r="305" ht="12.0" customHeight="1"/>
+    <row r="306" ht="12.0" customHeight="1"/>
+    <row r="307" ht="12.0" customHeight="1"/>
+    <row r="308" ht="12.0" customHeight="1"/>
+    <row r="309" ht="12.0" customHeight="1"/>
+    <row r="310" ht="12.0" customHeight="1"/>
+    <row r="311" ht="12.0" customHeight="1"/>
+    <row r="312" ht="12.0" customHeight="1"/>
+    <row r="313" ht="12.0" customHeight="1"/>
+    <row r="314" ht="12.0" customHeight="1"/>
+    <row r="315" ht="12.0" customHeight="1"/>
+    <row r="316" ht="12.0" customHeight="1"/>
+    <row r="317" ht="12.0" customHeight="1"/>
+    <row r="318" ht="12.0" customHeight="1"/>
+    <row r="319" ht="12.0" customHeight="1"/>
+    <row r="320" ht="12.0" customHeight="1"/>
+    <row r="321" ht="12.0" customHeight="1"/>
+    <row r="322" ht="12.0" customHeight="1"/>
+    <row r="323" ht="12.0" customHeight="1"/>
+    <row r="324" ht="12.0" customHeight="1"/>
+    <row r="325" ht="12.0" customHeight="1"/>
+    <row r="326" ht="12.0" customHeight="1"/>
+    <row r="327" ht="12.0" customHeight="1"/>
+    <row r="328" ht="12.0" customHeight="1"/>
+    <row r="329" ht="12.0" customHeight="1"/>
+    <row r="330" ht="12.0" customHeight="1"/>
+    <row r="331" ht="12.0" customHeight="1"/>
+    <row r="332" ht="12.0" customHeight="1"/>
+    <row r="333" ht="12.0" customHeight="1"/>
+    <row r="334" ht="12.0" customHeight="1"/>
+    <row r="335" ht="12.0" customHeight="1"/>
+    <row r="336" ht="12.0" customHeight="1"/>
+    <row r="337" ht="12.0" customHeight="1"/>
+    <row r="338" ht="12.0" customHeight="1"/>
+    <row r="339" ht="12.0" customHeight="1"/>
+    <row r="340" ht="12.0" customHeight="1"/>
+    <row r="341" ht="12.0" customHeight="1"/>
+    <row r="342" ht="12.0" customHeight="1"/>
+    <row r="343" ht="12.0" customHeight="1"/>
+    <row r="344" ht="12.0" customHeight="1"/>
+    <row r="345" ht="12.0" customHeight="1"/>
+    <row r="346" ht="12.0" customHeight="1"/>
+    <row r="347" ht="12.0" customHeight="1"/>
+    <row r="348" ht="12.0" customHeight="1"/>
+    <row r="349" ht="12.0" customHeight="1"/>
+    <row r="350" ht="12.0" customHeight="1"/>
+    <row r="351" ht="12.0" customHeight="1"/>
+    <row r="352" ht="12.0" customHeight="1"/>
+    <row r="353" ht="12.0" customHeight="1"/>
+    <row r="354" ht="12.0" customHeight="1"/>
+    <row r="355" ht="12.0" customHeight="1"/>
+    <row r="356" ht="12.0" customHeight="1"/>
+    <row r="357" ht="12.0" customHeight="1"/>
+    <row r="358" ht="12.0" customHeight="1"/>
+    <row r="359" ht="12.0" customHeight="1"/>
+    <row r="360" ht="12.0" customHeight="1"/>
+    <row r="361" ht="12.0" customHeight="1"/>
+    <row r="362" ht="12.0" customHeight="1"/>
+    <row r="363" ht="12.0" customHeight="1"/>
+    <row r="364" ht="12.0" customHeight="1"/>
+    <row r="365" ht="12.0" customHeight="1"/>
+    <row r="366" ht="12.0" customHeight="1"/>
+    <row r="367" ht="12.0" customHeight="1"/>
+    <row r="368" ht="12.0" customHeight="1"/>
+    <row r="369" ht="12.0" customHeight="1"/>
+    <row r="370" ht="12.0" customHeight="1"/>
+    <row r="371" ht="12.0" customHeight="1"/>
+    <row r="372" ht="12.0" customHeight="1"/>
+    <row r="373" ht="12.0" customHeight="1"/>
+    <row r="374" ht="12.0" customHeight="1"/>
+    <row r="375" ht="12.0" customHeight="1"/>
+    <row r="376" ht="12.0" customHeight="1"/>
+    <row r="377" ht="12.0" customHeight="1"/>
+    <row r="378" ht="12.0" customHeight="1"/>
+    <row r="379" ht="12.0" customHeight="1"/>
+    <row r="380" ht="12.0" customHeight="1"/>
+    <row r="381" ht="12.0" customHeight="1"/>
+    <row r="382" ht="12.0" customHeight="1"/>
+    <row r="383" ht="12.0" customHeight="1"/>
+    <row r="384" ht="12.0" customHeight="1"/>
+    <row r="385" ht="12.0" customHeight="1"/>
+    <row r="386" ht="12.0" customHeight="1"/>
+    <row r="387" ht="12.0" customHeight="1"/>
+    <row r="388" ht="12.0" customHeight="1"/>
+    <row r="389" ht="12.0" customHeight="1"/>
+    <row r="390" ht="12.0" customHeight="1"/>
+    <row r="391" ht="12.0" customHeight="1"/>
+    <row r="392" ht="12.0" customHeight="1"/>
+    <row r="393" ht="12.0" customHeight="1"/>
+    <row r="394" ht="12.0" customHeight="1"/>
+    <row r="395" ht="12.0" customHeight="1"/>
+    <row r="396" ht="12.0" customHeight="1"/>
+    <row r="397" ht="12.0" customHeight="1"/>
+    <row r="398" ht="12.0" customHeight="1"/>
+    <row r="399" ht="12.0" customHeight="1"/>
+    <row r="400" ht="12.0" customHeight="1"/>
+    <row r="401" ht="12.0" customHeight="1"/>
+    <row r="402" ht="12.0" customHeight="1"/>
+    <row r="403" ht="12.0" customHeight="1"/>
+    <row r="404" ht="12.0" customHeight="1"/>
+    <row r="405" ht="12.0" customHeight="1"/>
+    <row r="406" ht="12.0" customHeight="1"/>
+    <row r="407" ht="12.0" customHeight="1"/>
+    <row r="408" ht="12.0" customHeight="1"/>
+    <row r="409" ht="12.0" customHeight="1"/>
+    <row r="410" ht="12.0" customHeight="1"/>
+    <row r="411" ht="12.0" customHeight="1"/>
+    <row r="412" ht="12.0" customHeight="1"/>
+    <row r="413" ht="12.0" customHeight="1"/>
+    <row r="414" ht="12.0" customHeight="1"/>
+    <row r="415" ht="12.0" customHeight="1"/>
+    <row r="416" ht="12.0" customHeight="1"/>
+    <row r="417" ht="12.0" customHeight="1"/>
+    <row r="418" ht="12.0" customHeight="1"/>
+    <row r="419" ht="12.0" customHeight="1"/>
+    <row r="420" ht="12.0" customHeight="1"/>
+    <row r="421" ht="12.0" customHeight="1"/>
+    <row r="422" ht="12.0" customHeight="1"/>
+    <row r="423" ht="12.0" customHeight="1"/>
+    <row r="424" ht="12.0" customHeight="1"/>
+    <row r="425" ht="12.0" customHeight="1"/>
+    <row r="426" ht="12.0" customHeight="1"/>
+    <row r="427" ht="12.0" customHeight="1"/>
+    <row r="428" ht="12.0" customHeight="1"/>
+    <row r="429" ht="12.0" customHeight="1"/>
+    <row r="430" ht="12.0" customHeight="1"/>
+    <row r="431" ht="12.0" customHeight="1"/>
+    <row r="432" ht="12.0" customHeight="1"/>
+    <row r="433" ht="12.0" customHeight="1"/>
+    <row r="434" ht="12.0" customHeight="1"/>
+    <row r="435" ht="12.0" customHeight="1"/>
+    <row r="436" ht="12.0" customHeight="1"/>
+    <row r="437" ht="12.0" customHeight="1"/>
+    <row r="438" ht="12.0" customHeight="1"/>
+    <row r="439" ht="12.0" customHeight="1"/>
+    <row r="440" ht="12.0" customHeight="1"/>
+    <row r="441" ht="12.0" customHeight="1"/>
+    <row r="442" ht="12.0" customHeight="1"/>
+    <row r="443" ht="12.0" customHeight="1"/>
+    <row r="444" ht="12.0" customHeight="1"/>
+    <row r="445" ht="12.0" customHeight="1"/>
+    <row r="446" ht="12.0" customHeight="1"/>
+    <row r="447" ht="12.0" customHeight="1"/>
+    <row r="448" ht="12.0" customHeight="1"/>
+    <row r="449" ht="12.0" customHeight="1"/>
+    <row r="450" ht="12.0" customHeight="1"/>
+    <row r="451" ht="12.0" customHeight="1"/>
+    <row r="452" ht="12.0" customHeight="1"/>
+    <row r="453" ht="12.0" customHeight="1"/>
+    <row r="454" ht="12.0" customHeight="1"/>
+    <row r="455" ht="12.0" customHeight="1"/>
+    <row r="456" ht="12.0" customHeight="1"/>
+    <row r="457" ht="12.0" customHeight="1"/>
+    <row r="458" ht="12.0" customHeight="1"/>
+    <row r="459" ht="12.0" customHeight="1"/>
+    <row r="460" ht="12.0" customHeight="1"/>
+    <row r="461" ht="12.0" customHeight="1"/>
+    <row r="462" ht="12.0" customHeight="1"/>
+    <row r="463" ht="12.0" customHeight="1"/>
+    <row r="464" ht="12.0" customHeight="1"/>
+    <row r="465" ht="12.0" customHeight="1"/>
+    <row r="466" ht="12.0" customHeight="1"/>
+    <row r="467" ht="12.0" customHeight="1"/>
+    <row r="468" ht="12.0" customHeight="1"/>
+    <row r="469" ht="12.0" customHeight="1"/>
+    <row r="470" ht="12.0" customHeight="1"/>
+    <row r="471" ht="12.0" customHeight="1"/>
+    <row r="472" ht="12.0" customHeight="1"/>
+    <row r="473" ht="12.0" customHeight="1"/>
+    <row r="474" ht="12.0" customHeight="1"/>
+    <row r="475" ht="12.0" customHeight="1"/>
+    <row r="476" ht="12.0" customHeight="1"/>
+    <row r="477" ht="12.0" customHeight="1"/>
+    <row r="478" ht="12.0" customHeight="1"/>
+    <row r="479" ht="12.0" customHeight="1"/>
+    <row r="480" ht="12.0" customHeight="1"/>
+    <row r="481" ht="12.0" customHeight="1"/>
+    <row r="482" ht="12.0" customHeight="1"/>
+    <row r="483" ht="12.0" customHeight="1"/>
+    <row r="484" ht="12.0" customHeight="1"/>
+    <row r="485" ht="12.0" customHeight="1"/>
+    <row r="486" ht="12.0" customHeight="1"/>
+    <row r="487" ht="12.0" customHeight="1"/>
+    <row r="488" ht="12.0" customHeight="1"/>
+    <row r="489" ht="12.0" customHeight="1"/>
+    <row r="490" ht="12.0" customHeight="1"/>
+    <row r="491" ht="12.0" customHeight="1"/>
+    <row r="492" ht="12.0" customHeight="1"/>
+    <row r="493" ht="12.0" customHeight="1"/>
+    <row r="494" ht="12.0" customHeight="1"/>
+    <row r="495" ht="12.0" customHeight="1"/>
+    <row r="496" ht="12.0" customHeight="1"/>
+    <row r="497" ht="12.0" customHeight="1"/>
+    <row r="498" ht="12.0" customHeight="1"/>
+    <row r="499" ht="12.0" customHeight="1"/>
+    <row r="500" ht="12.0" customHeight="1"/>
+    <row r="501" ht="12.0" customHeight="1"/>
+    <row r="502" ht="12.0" customHeight="1"/>
+    <row r="503" ht="12.0" customHeight="1"/>
+    <row r="504" ht="12.0" customHeight="1"/>
+    <row r="505" ht="12.0" customHeight="1"/>
+    <row r="506" ht="12.0" customHeight="1"/>
+    <row r="507" ht="12.0" customHeight="1"/>
+    <row r="508" ht="12.0" customHeight="1"/>
+    <row r="509" ht="12.0" customHeight="1"/>
+    <row r="510" ht="12.0" customHeight="1"/>
+    <row r="511" ht="12.0" customHeight="1"/>
+    <row r="512" ht="12.0" customHeight="1"/>
+    <row r="513" ht="12.0" customHeight="1"/>
+    <row r="514" ht="12.0" customHeight="1"/>
+    <row r="515" ht="12.0" customHeight="1"/>
+    <row r="516" ht="12.0" customHeight="1"/>
+    <row r="517" ht="12.0" customHeight="1"/>
+    <row r="518" ht="12.0" customHeight="1"/>
+    <row r="519" ht="12.0" customHeight="1"/>
+    <row r="520" ht="12.0" customHeight="1"/>
+    <row r="521" ht="12.0" customHeight="1"/>
+    <row r="522" ht="12.0" customHeight="1"/>
+    <row r="523" ht="12.0" customHeight="1"/>
+    <row r="524" ht="12.0" customHeight="1"/>
+    <row r="525" ht="12.0" customHeight="1"/>
+    <row r="526" ht="12.0" customHeight="1"/>
+    <row r="527" ht="12.0" customHeight="1"/>
+    <row r="528" ht="12.0" customHeight="1"/>
+    <row r="529" ht="12.0" customHeight="1"/>
+    <row r="530" ht="12.0" customHeight="1"/>
+    <row r="531" ht="12.0" customHeight="1"/>
+    <row r="532" ht="12.0" customHeight="1"/>
+    <row r="533" ht="12.0" customHeight="1"/>
+    <row r="534" ht="12.0" customHeight="1"/>
+    <row r="535" ht="12.0" customHeight="1"/>
+    <row r="536" ht="12.0" customHeight="1"/>
+    <row r="537" ht="12.0" customHeight="1"/>
+    <row r="538" ht="12.0" customHeight="1"/>
+    <row r="539" ht="12.0" customHeight="1"/>
+    <row r="540" ht="12.0" customHeight="1"/>
+    <row r="541" ht="12.0" customHeight="1"/>
+    <row r="542" ht="12.0" customHeight="1"/>
+    <row r="543" ht="12.0" customHeight="1"/>
+    <row r="544" ht="12.0" customHeight="1"/>
+    <row r="545" ht="12.0" customHeight="1"/>
+    <row r="546" ht="12.0" customHeight="1"/>
+    <row r="547" ht="12.0" customHeight="1"/>
+    <row r="548" ht="12.0" customHeight="1"/>
+    <row r="549" ht="12.0" customHeight="1"/>
+    <row r="550" ht="12.0" customHeight="1"/>
+    <row r="551" ht="12.0" customHeight="1"/>
+    <row r="552" ht="12.0" customHeight="1"/>
+    <row r="553" ht="12.0" customHeight="1"/>
+    <row r="554" ht="12.0" customHeight="1"/>
+    <row r="555" ht="12.0" customHeight="1"/>
+    <row r="556" ht="12.0" customHeight="1"/>
+    <row r="557" ht="12.0" customHeight="1"/>
+    <row r="558" ht="12.0" customHeight="1"/>
+    <row r="559" ht="12.0" customHeight="1"/>
+    <row r="560" ht="12.0" customHeight="1"/>
+    <row r="561" ht="12.0" customHeight="1"/>
+    <row r="562" ht="12.0" customHeight="1"/>
+    <row r="563" ht="12.0" customHeight="1"/>
+    <row r="564" ht="12.0" customHeight="1"/>
+    <row r="565" ht="12.0" customHeight="1"/>
+    <row r="566" ht="12.0" customHeight="1"/>
+    <row r="567" ht="12.0" customHeight="1"/>
+    <row r="568" ht="12.0" customHeight="1"/>
+    <row r="569" ht="12.0" customHeight="1"/>
+    <row r="570" ht="12.0" customHeight="1"/>
+    <row r="571" ht="12.0" customHeight="1"/>
+    <row r="572" ht="12.0" customHeight="1"/>
+    <row r="573" ht="12.0" customHeight="1"/>
+    <row r="574" ht="12.0" customHeight="1"/>
+    <row r="575" ht="12.0" customHeight="1"/>
+    <row r="576" ht="12.0" customHeight="1"/>
+    <row r="577" ht="12.0" customHeight="1"/>
+    <row r="578" ht="12.0" customHeight="1"/>
+    <row r="579" ht="12.0" customHeight="1"/>
+    <row r="580" ht="12.0" customHeight="1"/>
+    <row r="581" ht="12.0" customHeight="1"/>
+    <row r="582" ht="12.0" customHeight="1"/>
+    <row r="583" ht="12.0" customHeight="1"/>
+    <row r="584" ht="12.0" customHeight="1"/>
+    <row r="585" ht="12.0" customHeight="1"/>
+    <row r="586" ht="12.0" customHeight="1"/>
+    <row r="587" ht="12.0" customHeight="1"/>
+    <row r="588" ht="12.0" customHeight="1"/>
+    <row r="589" ht="12.0" customHeight="1"/>
+    <row r="590" ht="12.0" customHeight="1"/>
+    <row r="591" ht="12.0" customHeight="1"/>
+    <row r="592" ht="12.0" customHeight="1"/>
+    <row r="593" ht="12.0" customHeight="1"/>
+    <row r="594" ht="12.0" customHeight="1"/>
+    <row r="595" ht="12.0" customHeight="1"/>
+    <row r="596" ht="12.0" customHeight="1"/>
+    <row r="597" ht="12.0" customHeight="1"/>
+    <row r="598" ht="12.0" customHeight="1"/>
+    <row r="599" ht="12.0" customHeight="1"/>
+    <row r="600" ht="12.0" customHeight="1"/>
+    <row r="601" ht="12.0" customHeight="1"/>
+    <row r="602" ht="12.0" customHeight="1"/>
+    <row r="603" ht="12.0" customHeight="1"/>
+    <row r="604" ht="12.0" customHeight="1"/>
+    <row r="605" ht="12.0" customHeight="1"/>
+    <row r="606" ht="12.0" customHeight="1"/>
+    <row r="607" ht="12.0" customHeight="1"/>
+    <row r="608" ht="12.0" customHeight="1"/>
+    <row r="609" ht="12.0" customHeight="1"/>
+    <row r="610" ht="12.0" customHeight="1"/>
+    <row r="611" ht="12.0" customHeight="1"/>
+    <row r="612" ht="12.0" customHeight="1"/>
+    <row r="613" ht="12.0" customHeight="1"/>
+    <row r="614" ht="12.0" customHeight="1"/>
+    <row r="615" ht="12.0" customHeight="1"/>
+    <row r="616" ht="12.0" customHeight="1"/>
+    <row r="617" ht="12.0" customHeight="1"/>
+    <row r="618" ht="12.0" customHeight="1"/>
+    <row r="619" ht="12.0" customHeight="1"/>
+    <row r="620" ht="12.0" customHeight="1"/>
+    <row r="621" ht="12.0" customHeight="1"/>
+    <row r="622" ht="12.0" customHeight="1"/>
+    <row r="623" ht="12.0" customHeight="1"/>
+    <row r="624" ht="12.0" customHeight="1"/>
+    <row r="625" ht="12.0" customHeight="1"/>
+    <row r="626" ht="12.0" customHeight="1"/>
+    <row r="627" ht="12.0" customHeight="1"/>
+    <row r="628" ht="12.0" customHeight="1"/>
+    <row r="629" ht="12.0" customHeight="1"/>
+    <row r="630" ht="12.0" customHeight="1"/>
+    <row r="631" ht="12.0" customHeight="1"/>
+    <row r="632" ht="12.0" customHeight="1"/>
+    <row r="633" ht="12.0" customHeight="1"/>
+    <row r="634" ht="12.0" customHeight="1"/>
+    <row r="635" ht="12.0" customHeight="1"/>
+    <row r="636" ht="12.0" customHeight="1"/>
+    <row r="637" ht="12.0" customHeight="1"/>
+    <row r="638" ht="12.0" customHeight="1"/>
+    <row r="639" ht="12.0" customHeight="1"/>
+    <row r="640" ht="12.0" customHeight="1"/>
+    <row r="641" ht="12.0" customHeight="1"/>
+    <row r="642" ht="12.0" customHeight="1"/>
+    <row r="643" ht="12.0" customHeight="1"/>
+    <row r="644" ht="12.0" customHeight="1"/>
+    <row r="645" ht="12.0" customHeight="1"/>
+    <row r="646" ht="12.0" customHeight="1"/>
+    <row r="647" ht="12.0" customHeight="1"/>
+    <row r="648" ht="12.0" customHeight="1"/>
+    <row r="649" ht="12.0" customHeight="1"/>
+    <row r="650" ht="12.0" customHeight="1"/>
+    <row r="651" ht="12.0" customHeight="1"/>
+    <row r="652" ht="12.0" customHeight="1"/>
+    <row r="653" ht="12.0" customHeight="1"/>
+    <row r="654" ht="12.0" customHeight="1"/>
+    <row r="655" ht="12.0" customHeight="1"/>
+    <row r="656" ht="12.0" customHeight="1"/>
+    <row r="657" ht="12.0" customHeight="1"/>
+    <row r="658" ht="12.0" customHeight="1"/>
+    <row r="659" ht="12.0" customHeight="1"/>
+    <row r="660" ht="12.0" customHeight="1"/>
+    <row r="661" ht="12.0" customHeight="1"/>
+    <row r="662" ht="12.0" customHeight="1"/>
+    <row r="663" ht="12.0" customHeight="1"/>
+    <row r="664" ht="12.0" customHeight="1"/>
+    <row r="665" ht="12.0" customHeight="1"/>
+    <row r="666" ht="12.0" customHeight="1"/>
+    <row r="667" ht="12.0" customHeight="1"/>
+    <row r="668" ht="12.0" customHeight="1"/>
+    <row r="669" ht="12.0" customHeight="1"/>
+    <row r="670" ht="12.0" customHeight="1"/>
+    <row r="671" ht="12.0" customHeight="1"/>
+    <row r="672" ht="12.0" customHeight="1"/>
+    <row r="673" ht="12.0" customHeight="1"/>
+    <row r="674" ht="12.0" customHeight="1"/>
+    <row r="675" ht="12.0" customHeight="1"/>
+    <row r="676" ht="12.0" customHeight="1"/>
+    <row r="677" ht="12.0" customHeight="1"/>
+    <row r="678" ht="12.0" customHeight="1"/>
+    <row r="679" ht="12.0" customHeight="1"/>
+    <row r="680" ht="12.0" customHeight="1"/>
+    <row r="681" ht="12.0" customHeight="1"/>
+    <row r="682" ht="12.0" customHeight="1"/>
+    <row r="683" ht="12.0" customHeight="1"/>
+    <row r="684" ht="12.0" customHeight="1"/>
+    <row r="685" ht="12.0" customHeight="1"/>
+    <row r="686" ht="12.0" customHeight="1"/>
+    <row r="687" ht="12.0" customHeight="1"/>
+    <row r="688" ht="12.0" customHeight="1"/>
+    <row r="689" ht="12.0" customHeight="1"/>
+    <row r="690" ht="12.0" customHeight="1"/>
+    <row r="691" ht="12.0" customHeight="1"/>
+    <row r="692" ht="12.0" customHeight="1"/>
+    <row r="693" ht="12.0" customHeight="1"/>
+    <row r="694" ht="12.0" customHeight="1"/>
+    <row r="695" ht="12.0" customHeight="1"/>
+    <row r="696" ht="12.0" customHeight="1"/>
+    <row r="697" ht="12.0" customHeight="1"/>
+    <row r="698" ht="12.0" customHeight="1"/>
+    <row r="699" ht="12.0" customHeight="1"/>
+    <row r="700" ht="12.0" customHeight="1"/>
+    <row r="701" ht="12.0" customHeight="1"/>
+    <row r="702" ht="12.0" customHeight="1"/>
+    <row r="703" ht="12.0" customHeight="1"/>
+    <row r="704" ht="12.0" customHeight="1"/>
+    <row r="705" ht="12.0" customHeight="1"/>
+    <row r="706" ht="12.0" customHeight="1"/>
+    <row r="707" ht="12.0" customHeight="1"/>
+    <row r="708" ht="12.0" customHeight="1"/>
+    <row r="709" ht="12.0" customHeight="1"/>
+    <row r="710" ht="12.0" customHeight="1"/>
+    <row r="711" ht="12.0" customHeight="1"/>
+    <row r="712" ht="12.0" customHeight="1"/>
+    <row r="713" ht="12.0" customHeight="1"/>
+    <row r="714" ht="12.0" customHeight="1"/>
+    <row r="715" ht="12.0" customHeight="1"/>
+    <row r="716" ht="12.0" customHeight="1"/>
+    <row r="717" ht="12.0" customHeight="1"/>
+    <row r="718" ht="12.0" customHeight="1"/>
+    <row r="719" ht="12.0" customHeight="1"/>
+    <row r="720" ht="12.0" customHeight="1"/>
+    <row r="721" ht="12.0" customHeight="1"/>
+    <row r="722" ht="12.0" customHeight="1"/>
+    <row r="723" ht="12.0" customHeight="1"/>
+    <row r="724" ht="12.0" customHeight="1"/>
+    <row r="725" ht="12.0" customHeight="1"/>
+    <row r="726" ht="12.0" customHeight="1"/>
+    <row r="727" ht="12.0" customHeight="1"/>
+    <row r="728" ht="12.0" customHeight="1"/>
+    <row r="729" ht="12.0" customHeight="1"/>
+    <row r="730" ht="12.0" customHeight="1"/>
+    <row r="731" ht="12.0" customHeight="1"/>
+    <row r="732" ht="12.0" customHeight="1"/>
+    <row r="733" ht="12.0" customHeight="1"/>
+    <row r="734" ht="12.0" customHeight="1"/>
+    <row r="735" ht="12.0" customHeight="1"/>
+    <row r="736" ht="12.0" customHeight="1"/>
+    <row r="737" ht="12.0" customHeight="1"/>
+    <row r="738" ht="12.0" customHeight="1"/>
+    <row r="739" ht="12.0" customHeight="1"/>
+    <row r="740" ht="12.0" customHeight="1"/>
+    <row r="741" ht="12.0" customHeight="1"/>
+    <row r="742" ht="12.0" customHeight="1"/>
+    <row r="743" ht="12.0" customHeight="1"/>
+    <row r="744" ht="12.0" customHeight="1"/>
+    <row r="745" ht="12.0" customHeight="1"/>
+    <row r="746" ht="12.0" customHeight="1"/>
+    <row r="747" ht="12.0" customHeight="1"/>
+    <row r="748" ht="12.0" customHeight="1"/>
+    <row r="749" ht="12.0" customHeight="1"/>
+    <row r="750" ht="12.0" customHeight="1"/>
+    <row r="751" ht="12.0" customHeight="1"/>
+    <row r="752" ht="12.0" customHeight="1"/>
+    <row r="753" ht="12.0" customHeight="1"/>
+    <row r="754" ht="12.0" customHeight="1"/>
+    <row r="755" ht="12.0" customHeight="1"/>
+    <row r="756" ht="12.0" customHeight="1"/>
+    <row r="757" ht="12.0" customHeight="1"/>
+    <row r="758" ht="12.0" customHeight="1"/>
+    <row r="759" ht="12.0" customHeight="1"/>
+    <row r="760" ht="12.0" customHeight="1"/>
+    <row r="761" ht="12.0" customHeight="1"/>
+    <row r="762" ht="12.0" customHeight="1"/>
+    <row r="763" ht="12.0" customHeight="1"/>
+    <row r="764" ht="12.0" customHeight="1"/>
+    <row r="765" ht="12.0" customHeight="1"/>
+    <row r="766" ht="12.0" customHeight="1"/>
+    <row r="767" ht="12.0" customHeight="1"/>
+    <row r="768" ht="12.0" customHeight="1"/>
+    <row r="769" ht="12.0" customHeight="1"/>
+    <row r="770" ht="12.0" customHeight="1"/>
+    <row r="771" ht="12.0" customHeight="1"/>
+    <row r="772" ht="12.0" customHeight="1"/>
+    <row r="773" ht="12.0" customHeight="1"/>
+    <row r="774" ht="12.0" customHeight="1"/>
+    <row r="775" ht="12.0" customHeight="1"/>
+    <row r="776" ht="12.0" customHeight="1"/>
+    <row r="777" ht="12.0" customHeight="1"/>
+    <row r="778" ht="12.0" customHeight="1"/>
+    <row r="779" ht="12.0" customHeight="1"/>
+    <row r="780" ht="12.0" customHeight="1"/>
+    <row r="781" ht="12.0" customHeight="1"/>
+    <row r="782" ht="12.0" customHeight="1"/>
+    <row r="783" ht="12.0" customHeight="1"/>
+    <row r="784" ht="12.0" customHeight="1"/>
+    <row r="785" ht="12.0" customHeight="1"/>
+    <row r="786" ht="12.0" customHeight="1"/>
+    <row r="787" ht="12.0" customHeight="1"/>
+    <row r="788" ht="12.0" customHeight="1"/>
+    <row r="789" ht="12.0" customHeight="1"/>
+    <row r="790" ht="12.0" customHeight="1"/>
+    <row r="791" ht="12.0" customHeight="1"/>
+    <row r="792" ht="12.0" customHeight="1"/>
+    <row r="793" ht="12.0" customHeight="1"/>
+    <row r="794" ht="12.0" customHeight="1"/>
+    <row r="795" ht="12.0" customHeight="1"/>
+    <row r="796" ht="12.0" customHeight="1"/>
+    <row r="797" ht="12.0" customHeight="1"/>
+    <row r="798" ht="12.0" customHeight="1"/>
+    <row r="799" ht="12.0" customHeight="1"/>
+    <row r="800" ht="12.0" customHeight="1"/>
+    <row r="801" ht="12.0" customHeight="1"/>
+    <row r="802" ht="12.0" customHeight="1"/>
+    <row r="803" ht="12.0" customHeight="1"/>
+    <row r="804" ht="12.0" customHeight="1"/>
+    <row r="805" ht="12.0" customHeight="1"/>
+    <row r="806" ht="12.0" customHeight="1"/>
+    <row r="807" ht="12.0" customHeight="1"/>
+    <row r="808" ht="12.0" customHeight="1"/>
+    <row r="809" ht="12.0" customHeight="1"/>
+    <row r="810" ht="12.0" customHeight="1"/>
+    <row r="811" ht="12.0" customHeight="1"/>
+    <row r="812" ht="12.0" customHeight="1"/>
+    <row r="813" ht="12.0" customHeight="1"/>
+    <row r="814" ht="12.0" customHeight="1"/>
+    <row r="815" ht="12.0" customHeight="1"/>
+    <row r="816" ht="12.0" customHeight="1"/>
+    <row r="817" ht="12.0" customHeight="1"/>
+    <row r="818" ht="12.0" customHeight="1"/>
+    <row r="819" ht="12.0" customHeight="1"/>
+    <row r="820" ht="12.0" customHeight="1"/>
+    <row r="821" ht="12.0" customHeight="1"/>
+    <row r="822" ht="12.0" customHeight="1"/>
+    <row r="823" ht="12.0" customHeight="1"/>
+    <row r="824" ht="12.0" customHeight="1"/>
+    <row r="825" ht="12.0" customHeight="1"/>
+    <row r="826" ht="12.0" customHeight="1"/>
+    <row r="827" ht="12.0" customHeight="1"/>
+    <row r="828" ht="12.0" customHeight="1"/>
+    <row r="829" ht="12.0" customHeight="1"/>
+    <row r="830" ht="12.0" customHeight="1"/>
+    <row r="831" ht="12.0" customHeight="1"/>
+    <row r="832" ht="12.0" customHeight="1"/>
+    <row r="833" ht="12.0" customHeight="1"/>
+    <row r="834" ht="12.0" customHeight="1"/>
+    <row r="835" ht="12.0" customHeight="1"/>
+    <row r="836" ht="12.0" customHeight="1"/>
+    <row r="837" ht="12.0" customHeight="1"/>
+    <row r="838" ht="12.0" customHeight="1"/>
+    <row r="839" ht="12.0" customHeight="1"/>
+    <row r="840" ht="12.0" customHeight="1"/>
+    <row r="841" ht="12.0" customHeight="1"/>
+    <row r="842" ht="12.0" customHeight="1"/>
+    <row r="843" ht="12.0" customHeight="1"/>
+    <row r="844" ht="12.0" customHeight="1"/>
+    <row r="845" ht="12.0" customHeight="1"/>
+    <row r="846" ht="12.0" customHeight="1"/>
+    <row r="847" ht="12.0" customHeight="1"/>
+    <row r="848" ht="12.0" customHeight="1"/>
+    <row r="849" ht="12.0" customHeight="1"/>
+    <row r="850" ht="12.0" customHeight="1"/>
+    <row r="851" ht="12.0" customHeight="1"/>
+    <row r="852" ht="12.0" customHeight="1"/>
+    <row r="853" ht="12.0" customHeight="1"/>
+    <row r="854" ht="12.0" customHeight="1"/>
+    <row r="855" ht="12.0" customHeight="1"/>
+    <row r="856" ht="12.0" customHeight="1"/>
+    <row r="857" ht="12.0" customHeight="1"/>
+    <row r="858" ht="12.0" customHeight="1"/>
+    <row r="859" ht="12.0" customHeight="1"/>
+    <row r="860" ht="12.0" customHeight="1"/>
+    <row r="861" ht="12.0" customHeight="1"/>
+    <row r="862" ht="12.0" customHeight="1"/>
+    <row r="863" ht="12.0" customHeight="1"/>
+    <row r="864" ht="12.0" customHeight="1"/>
+    <row r="865" ht="12.0" customHeight="1"/>
+    <row r="866" ht="12.0" customHeight="1"/>
+    <row r="867" ht="12.0" customHeight="1"/>
+    <row r="868" ht="12.0" customHeight="1"/>
+    <row r="869" ht="12.0" customHeight="1"/>
+    <row r="870" ht="12.0" customHeight="1"/>
+    <row r="871" ht="12.0" customHeight="1"/>
+    <row r="872" ht="12.0" customHeight="1"/>
+    <row r="873" ht="12.0" customHeight="1"/>
+    <row r="874" ht="12.0" customHeight="1"/>
+    <row r="875" ht="12.0" customHeight="1"/>
+    <row r="876" ht="12.0" customHeight="1"/>
+    <row r="877" ht="12.0" customHeight="1"/>
+    <row r="878" ht="12.0" customHeight="1"/>
+    <row r="879" ht="12.0" customHeight="1"/>
+    <row r="880" ht="12.0" customHeight="1"/>
+    <row r="881" ht="12.0" customHeight="1"/>
+    <row r="882" ht="12.0" customHeight="1"/>
+    <row r="883" ht="12.0" customHeight="1"/>
+    <row r="884" ht="12.0" customHeight="1"/>
+    <row r="885" ht="12.0" customHeight="1"/>
+    <row r="886" ht="12.0" customHeight="1"/>
+    <row r="887" ht="12.0" customHeight="1"/>
+    <row r="888" ht="12.0" customHeight="1"/>
+    <row r="889" ht="12.0" customHeight="1"/>
+    <row r="890" ht="12.0" customHeight="1"/>
+    <row r="891" ht="12.0" customHeight="1"/>
+    <row r="892" ht="12.0" customHeight="1"/>
+    <row r="893" ht="12.0" customHeight="1"/>
+    <row r="894" ht="12.0" customHeight="1"/>
+    <row r="895" ht="12.0" customHeight="1"/>
+    <row r="896" ht="12.0" customHeight="1"/>
+    <row r="897" ht="12.0" customHeight="1"/>
+    <row r="898" ht="12.0" customHeight="1"/>
+    <row r="899" ht="12.0" customHeight="1"/>
+    <row r="900" ht="12.0" customHeight="1"/>
+    <row r="901" ht="12.0" customHeight="1"/>
+    <row r="902" ht="12.0" customHeight="1"/>
+    <row r="903" ht="12.0" customHeight="1"/>
+    <row r="904" ht="12.0" customHeight="1"/>
+    <row r="905" ht="12.0" customHeight="1"/>
+    <row r="906" ht="12.0" customHeight="1"/>
+    <row r="907" ht="12.0" customHeight="1"/>
+    <row r="908" ht="12.0" customHeight="1"/>
+    <row r="909" ht="12.0" customHeight="1"/>
+    <row r="910" ht="12.0" customHeight="1"/>
+    <row r="911" ht="12.0" customHeight="1"/>
+    <row r="912" ht="12.0" customHeight="1"/>
+    <row r="913" ht="12.0" customHeight="1"/>
+    <row r="914" ht="12.0" customHeight="1"/>
+    <row r="915" ht="12.0" customHeight="1"/>
+    <row r="916" ht="12.0" customHeight="1"/>
+    <row r="917" ht="12.0" customHeight="1"/>
+    <row r="918" ht="12.0" customHeight="1"/>
+    <row r="919" ht="12.0" customHeight="1"/>
+    <row r="920" ht="12.0" customHeight="1"/>
+    <row r="921" ht="12.0" customHeight="1"/>
+    <row r="922" ht="12.0" customHeight="1"/>
+    <row r="923" ht="12.0" customHeight="1"/>
+    <row r="924" ht="12.0" customHeight="1"/>
+    <row r="925" ht="12.0" customHeight="1"/>
+    <row r="926" ht="12.0" customHeight="1"/>
+    <row r="927" ht="12.0" customHeight="1"/>
+    <row r="928" ht="12.0" customHeight="1"/>
+    <row r="929" ht="12.0" customHeight="1"/>
+    <row r="930" ht="12.0" customHeight="1"/>
+    <row r="931" ht="12.0" customHeight="1"/>
+    <row r="932" ht="12.0" customHeight="1"/>
+    <row r="933" ht="12.0" customHeight="1"/>
+    <row r="934" ht="12.0" customHeight="1"/>
+    <row r="935" ht="12.0" customHeight="1"/>
+    <row r="936" ht="12.0" customHeight="1"/>
+    <row r="937" ht="12.0" customHeight="1"/>
+    <row r="938" ht="12.0" customHeight="1"/>
+    <row r="939" ht="12.0" customHeight="1"/>
+    <row r="940" ht="12.0" customHeight="1"/>
+    <row r="941" ht="12.0" customHeight="1"/>
+    <row r="942" ht="12.0" customHeight="1"/>
+    <row r="943" ht="12.0" customHeight="1"/>
+    <row r="944" ht="12.0" customHeight="1"/>
+    <row r="945" ht="12.0" customHeight="1"/>
+    <row r="946" ht="12.0" customHeight="1"/>
+    <row r="947" ht="12.0" customHeight="1"/>
+    <row r="948" ht="12.0" customHeight="1"/>
+    <row r="949" ht="12.0" customHeight="1"/>
+    <row r="950" ht="12.0" customHeight="1"/>
+    <row r="951" ht="12.0" customHeight="1"/>
+    <row r="952" ht="12.0" customHeight="1"/>
+    <row r="953" ht="12.0" customHeight="1"/>
+    <row r="954" ht="12.0" customHeight="1"/>
+    <row r="955" ht="12.0" customHeight="1"/>
+    <row r="956" ht="12.0" customHeight="1"/>
+    <row r="957" ht="12.0" customHeight="1"/>
+    <row r="958" ht="12.0" customHeight="1"/>
+    <row r="959" ht="12.0" customHeight="1"/>
+    <row r="960" ht="12.0" customHeight="1"/>
+    <row r="961" ht="12.0" customHeight="1"/>
+    <row r="962" ht="12.0" customHeight="1"/>
+    <row r="963" ht="12.0" customHeight="1"/>
+    <row r="964" ht="12.0" customHeight="1"/>
+    <row r="965" ht="12.0" customHeight="1"/>
+    <row r="966" ht="12.0" customHeight="1"/>
+    <row r="967" ht="12.0" customHeight="1"/>
+    <row r="968" ht="12.0" customHeight="1"/>
+    <row r="969" ht="12.0" customHeight="1"/>
+    <row r="970" ht="12.0" customHeight="1"/>
+    <row r="971" ht="12.0" customHeight="1"/>
+    <row r="972" ht="12.0" customHeight="1"/>
+    <row r="973" ht="12.0" customHeight="1"/>
+    <row r="974" ht="12.0" customHeight="1"/>
+    <row r="975" ht="12.0" customHeight="1"/>
+    <row r="976" ht="12.0" customHeight="1"/>
+    <row r="977" ht="12.0" customHeight="1"/>
+    <row r="978" ht="12.0" customHeight="1"/>
+    <row r="979" ht="12.0" customHeight="1"/>
+    <row r="980" ht="12.0" customHeight="1"/>
+    <row r="981" ht="12.0" customHeight="1"/>
+    <row r="982" ht="12.0" customHeight="1"/>
+    <row r="983" ht="12.0" customHeight="1"/>
+    <row r="984" ht="12.0" customHeight="1"/>
+    <row r="985" ht="12.0" customHeight="1"/>
+    <row r="986" ht="12.0" customHeight="1"/>
+    <row r="987" ht="12.0" customHeight="1"/>
+    <row r="988" ht="12.0" customHeight="1"/>
+    <row r="989" ht="12.0" customHeight="1"/>
+    <row r="990" ht="12.0" customHeight="1"/>
+    <row r="991" ht="12.0" customHeight="1"/>
+    <row r="992" ht="12.0" customHeight="1"/>
+    <row r="993" ht="12.0" customHeight="1"/>
+    <row r="994" ht="12.0" customHeight="1"/>
+    <row r="995" ht="12.0" customHeight="1"/>
+    <row r="996" ht="12.0" customHeight="1"/>
+    <row r="997" ht="12.0" customHeight="1"/>
+    <row r="998" ht="12.0" customHeight="1"/>
+    <row r="999" ht="12.0" customHeight="1"/>
+    <row r="1000" ht="12.0" customHeight="1"/>
+  </sheetData>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -2646,15 +3849,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="49.43"/>
     <col customWidth="1" min="3" max="3" width="15.0"/>
     <col customWidth="1" min="4" max="4" width="31.14"/>
     <col customWidth="1" min="5" max="5" width="16.29"/>
-    <col customWidth="1" min="6" max="9" width="14.43"/>
     <col customWidth="1" min="10" max="10" width="11.86"/>
     <col customWidth="1" min="11" max="11" width="16.29"/>
-    <col customWidth="1" min="12" max="32" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -2977,7 +4177,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="28"/>
+      <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -3134,8 +4334,8 @@
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
-      <c r="AE14" s="29"/>
-      <c r="AF14" s="29"/>
+      <c r="AE14" s="28"/>
+      <c r="AF14" s="28"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3"/>
@@ -3202,8 +4402,8 @@
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
-      <c r="AE16" s="29"/>
-      <c r="AF16" s="29"/>
+      <c r="AE16" s="28"/>
+      <c r="AF16" s="28"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="3"/>
@@ -3338,8 +4538,8 @@
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
-      <c r="AE20" s="29"/>
-      <c r="AF20" s="29"/>
+      <c r="AE20" s="28"/>
+      <c r="AF20" s="28"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
@@ -3406,8 +4606,8 @@
       <c r="AB22" s="3"/>
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
-      <c r="AE22" s="29"/>
-      <c r="AF22" s="29"/>
+      <c r="AE22" s="28"/>
+      <c r="AF22" s="28"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="3"/>
@@ -3440,8 +4640,8 @@
       <c r="AB23" s="3"/>
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
-      <c r="AE23" s="29"/>
-      <c r="AF23" s="29"/>
+      <c r="AE23" s="28"/>
+      <c r="AF23" s="28"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="3"/>
@@ -3474,8 +4674,8 @@
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
-      <c r="AE24" s="29"/>
-      <c r="AF24" s="29"/>
+      <c r="AE24" s="28"/>
+      <c r="AF24" s="28"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="3"/>
@@ -3508,8 +4708,8 @@
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
-      <c r="AE25" s="29"/>
-      <c r="AF25" s="29"/>
+      <c r="AE25" s="28"/>
+      <c r="AF25" s="28"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3"/>
@@ -3542,8 +4742,8 @@
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
-      <c r="AE26" s="29"/>
-      <c r="AF26" s="29"/>
+      <c r="AE26" s="28"/>
+      <c r="AF26" s="28"/>
     </row>
     <row r="27" ht="12.0" customHeight="1"/>
     <row r="28" ht="12.0" customHeight="1"/>
@@ -4537,18 +5737,14 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="49.43"/>
     <col customWidth="1" min="3" max="3" width="15.14"/>
     <col customWidth="1" min="4" max="4" width="28.43"/>
     <col customWidth="1" min="5" max="5" width="13.86"/>
-    <col customWidth="1" min="6" max="9" width="14.43"/>
     <col customWidth="1" min="10" max="10" width="11.86"/>
     <col customWidth="1" min="11" max="11" width="16.29"/>
-    <col customWidth="1" min="12" max="12" width="14.43"/>
     <col customWidth="1" min="13" max="13" width="19.29"/>
     <col customWidth="1" min="14" max="14" width="48.29"/>
-    <col customWidth="1" min="15" max="32" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -4783,7 +5979,7 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="30"/>
+      <c r="N8" s="29"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -4837,10 +6033,10 @@
       <c r="K9" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="30" t="s">
         <v>40</v>
       </c>
       <c r="N9" s="24" t="s">
@@ -5874,20 +7070,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="25.71"/>
     <col customWidth="1" min="3" max="3" width="15.29"/>
     <col customWidth="1" min="4" max="4" width="26.57"/>
     <col customWidth="1" min="5" max="6" width="15.86"/>
     <col customWidth="1" min="7" max="7" width="12.43"/>
-    <col customWidth="1" min="8" max="8" width="14.43"/>
     <col customWidth="1" min="9" max="9" width="13.0"/>
     <col customWidth="1" min="10" max="10" width="11.86"/>
     <col customWidth="1" min="11" max="11" width="16.29"/>
     <col customWidth="1" min="12" max="12" width="10.14"/>
     <col customWidth="1" min="13" max="13" width="12.71"/>
     <col customWidth="1" min="14" max="14" width="50.0"/>
-    <col customWidth="1" min="15" max="27" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -6089,7 +7282,7 @@
       <c r="N7" s="3"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="9"/>
@@ -6143,7 +7336,7 @@
       <c r="L9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="30" t="s">
         <v>44</v>
       </c>
       <c r="N9" s="15" t="s">
@@ -6168,13 +7361,13 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="34"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="33"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
@@ -6184,14 +7377,14 @@
       <c r="C11" s="22"/>
       <c r="D11" s="3"/>
       <c r="E11" s="22"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="36"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="35"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="37"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="36"/>
       <c r="N11" s="3"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
@@ -6200,14 +7393,14 @@
       <c r="C12" s="22"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="36"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="35"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="37"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="36"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" ht="12.0" customHeight="1"/>
@@ -7216,18 +8409,15 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="52.0"/>
     <col customWidth="1" min="3" max="3" width="15.14"/>
     <col customWidth="1" min="4" max="4" width="33.71"/>
     <col customWidth="1" min="5" max="5" width="13.86"/>
-    <col customWidth="1" min="6" max="9" width="14.43"/>
     <col customWidth="1" min="10" max="10" width="11.86"/>
     <col customWidth="1" min="11" max="11" width="16.29"/>
     <col customWidth="1" min="12" max="12" width="12.0"/>
     <col customWidth="1" min="13" max="13" width="19.29"/>
     <col customWidth="1" min="14" max="14" width="43.71"/>
-    <col customWidth="1" min="15" max="30" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -7515,7 +8705,7 @@
       <c r="L9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="30" t="s">
         <v>40</v>
       </c>
       <c r="N9" s="15" t="s">
@@ -8547,20 +9737,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="66.71"/>
     <col customWidth="1" min="3" max="3" width="15.14"/>
     <col customWidth="1" min="4" max="4" width="30.14"/>
     <col customWidth="1" min="5" max="6" width="13.86"/>
     <col customWidth="1" min="7" max="7" width="12.86"/>
     <col customWidth="1" min="8" max="8" width="13.14"/>
-    <col customWidth="1" min="9" max="9" width="14.43"/>
     <col customWidth="1" min="10" max="10" width="11.86"/>
     <col customWidth="1" min="11" max="11" width="16.29"/>
     <col customWidth="1" min="12" max="12" width="13.43"/>
     <col customWidth="1" min="13" max="13" width="19.29"/>
     <col customWidth="1" min="14" max="14" width="50.14"/>
-    <col customWidth="1" min="15" max="30" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -8818,13 +10005,13 @@
       <c r="B9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="30" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="24" t="s">
@@ -8845,17 +10032,17 @@
       <c r="K9" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="30" t="s">
         <v>40</v>
       </c>
       <c r="N9" s="15" t="s">
         <v>41</v>
       </c>
       <c r="O9" s="3"/>
-      <c r="P9" s="29"/>
+      <c r="P9" s="28"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
@@ -9880,18 +11067,14 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="49.43"/>
     <col customWidth="1" min="3" max="3" width="15.14"/>
     <col customWidth="1" min="4" max="4" width="31.14"/>
     <col customWidth="1" min="5" max="5" width="13.86"/>
-    <col customWidth="1" min="6" max="6" width="14.43"/>
     <col customWidth="1" min="7" max="7" width="17.71"/>
     <col customWidth="1" min="8" max="8" width="16.86"/>
     <col customWidth="1" min="9" max="9" width="16.29"/>
-    <col customWidth="1" min="10" max="10" width="14.43"/>
     <col customWidth="1" min="11" max="11" width="40.86"/>
-    <col customWidth="1" min="12" max="30" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -10121,7 +11304,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="38"/>
+      <c r="K8" s="37"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -10158,13 +11341,13 @@
       <c r="E9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="38" t="s">
         <v>51</v>
       </c>
       <c r="I9" s="25" t="s">
@@ -10173,7 +11356,7 @@
       <c r="J9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="40" t="s">
+      <c r="K9" s="39" t="s">
         <v>41</v>
       </c>
       <c r="L9" s="3"/>
@@ -11211,13 +12394,10 @@
     <col customWidth="1" min="4" max="4" width="22.14"/>
     <col customWidth="1" min="5" max="5" width="14.71"/>
     <col customWidth="1" min="6" max="6" width="13.71"/>
-    <col customWidth="1" min="7" max="7" width="14.43"/>
     <col customWidth="1" min="8" max="8" width="17.71"/>
     <col customWidth="1" min="9" max="9" width="16.29"/>
     <col customWidth="1" min="10" max="10" width="15.86"/>
-    <col customWidth="1" min="11" max="11" width="14.43"/>
     <col customWidth="1" min="12" max="12" width="40.86"/>
-    <col customWidth="1" min="13" max="26" width="14.43"/>
     <col customWidth="1" min="27" max="27" width="8.71"/>
   </cols>
   <sheetData>
@@ -11417,7 +12597,7 @@
       <c r="C9" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="15" t="s">
         <v>54</v>
       </c>
       <c r="E9" s="15" t="s">
@@ -11426,12 +12606,12 @@
       <c r="F9" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="25"/>
       <c r="K9" s="26"/>
-      <c r="L9" s="40"/>
+      <c r="L9" s="39"/>
       <c r="M9" s="3"/>
       <c r="N9" s="25"/>
       <c r="O9" s="3"/>
@@ -12633,13 +13813,13 @@
     <row r="7" ht="12.0" customHeight="1"/>
     <row r="8" ht="12.0" customHeight="1"/>
     <row r="9" ht="12.0" customHeight="1">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="40" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add locations to download spreadsheet (#228)
* Add locations to download spreadsheet

* Respond to PR feedback

* Respond to PR feedback
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheets/JPC_template.xlsx
+++ b/src/main/resources/spreadsheets/JPC_template.xlsx
@@ -12,19 +12,20 @@
     <sheet state="visible" name="Cancelled" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="Journeys" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="JPC Price book" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Locations" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mhf6KaviNSFEQVjUwiLv57fp3v1eg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mjzzXmz8O8REGjAAviJultF+4l2uA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="60">
   <si>
     <t>Calculate Journey Variable Payments (S2B)</t>
   </si>
@@ -276,6 +277,15 @@
   <si>
     <t>Total price</t>
   </si>
+  <si>
+    <t>Nomis Agency ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
 </sst>
 </file>
 
@@ -389,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -474,9 +484,6 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -513,9 +520,7 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -528,6 +533,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -769,9 +778,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="35.71"/>
     <col customWidth="1" min="2" max="2" width="16.14"/>
-    <col customWidth="1" min="3" max="4" width="14.43"/>
     <col customWidth="1" min="5" max="5" width="16.14"/>
-    <col customWidth="1" min="6" max="25" width="14.43"/>
     <col customWidth="1" min="26" max="26" width="8.71"/>
   </cols>
   <sheetData>
@@ -2636,6 +2643,1202 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="35.86"/>
+    <col customWidth="1" min="2" max="2" width="37.43"/>
+    <col customWidth="1" min="3" max="3" width="15.14"/>
+    <col customWidth="1" min="4" max="4" width="11.57"/>
+    <col customWidth="1" min="5" max="25" width="10.71"/>
+    <col customWidth="1" min="26" max="26" width="8.71"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="7"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+    </row>
+    <row r="7" ht="12.0" customHeight="1"/>
+    <row r="8" ht="12.0" customHeight="1"/>
+    <row r="9" ht="12.0" customHeight="1">
+      <c r="A9" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" ht="12.0" customHeight="1"/>
+    <row r="11" ht="12.0" customHeight="1"/>
+    <row r="12" ht="12.0" customHeight="1"/>
+    <row r="13" ht="12.0" customHeight="1"/>
+    <row r="14" ht="12.0" customHeight="1"/>
+    <row r="15" ht="12.0" customHeight="1"/>
+    <row r="16" ht="12.0" customHeight="1"/>
+    <row r="17" ht="12.0" customHeight="1"/>
+    <row r="18" ht="12.0" customHeight="1"/>
+    <row r="19" ht="12.0" customHeight="1"/>
+    <row r="20" ht="12.0" customHeight="1"/>
+    <row r="21" ht="12.0" customHeight="1"/>
+    <row r="22" ht="12.0" customHeight="1"/>
+    <row r="23" ht="12.0" customHeight="1"/>
+    <row r="24" ht="12.0" customHeight="1"/>
+    <row r="25" ht="12.0" customHeight="1"/>
+    <row r="26" ht="12.0" customHeight="1"/>
+    <row r="27" ht="12.0" customHeight="1"/>
+    <row r="28" ht="12.0" customHeight="1"/>
+    <row r="29" ht="12.0" customHeight="1"/>
+    <row r="30" ht="12.0" customHeight="1"/>
+    <row r="31" ht="12.0" customHeight="1"/>
+    <row r="32" ht="12.0" customHeight="1"/>
+    <row r="33" ht="12.0" customHeight="1"/>
+    <row r="34" ht="12.0" customHeight="1"/>
+    <row r="35" ht="12.0" customHeight="1"/>
+    <row r="36" ht="12.0" customHeight="1"/>
+    <row r="37" ht="12.0" customHeight="1"/>
+    <row r="38" ht="12.0" customHeight="1"/>
+    <row r="39" ht="12.0" customHeight="1"/>
+    <row r="40" ht="12.0" customHeight="1"/>
+    <row r="41" ht="12.0" customHeight="1"/>
+    <row r="42" ht="12.0" customHeight="1"/>
+    <row r="43" ht="12.0" customHeight="1"/>
+    <row r="44" ht="12.0" customHeight="1"/>
+    <row r="45" ht="12.0" customHeight="1"/>
+    <row r="46" ht="12.0" customHeight="1"/>
+    <row r="47" ht="12.0" customHeight="1"/>
+    <row r="48" ht="12.0" customHeight="1"/>
+    <row r="49" ht="12.0" customHeight="1"/>
+    <row r="50" ht="12.0" customHeight="1"/>
+    <row r="51" ht="12.0" customHeight="1"/>
+    <row r="52" ht="12.0" customHeight="1"/>
+    <row r="53" ht="12.0" customHeight="1"/>
+    <row r="54" ht="12.0" customHeight="1"/>
+    <row r="55" ht="12.0" customHeight="1"/>
+    <row r="56" ht="12.0" customHeight="1"/>
+    <row r="57" ht="12.0" customHeight="1"/>
+    <row r="58" ht="12.0" customHeight="1"/>
+    <row r="59" ht="12.0" customHeight="1"/>
+    <row r="60" ht="12.0" customHeight="1"/>
+    <row r="61" ht="12.0" customHeight="1"/>
+    <row r="62" ht="12.0" customHeight="1"/>
+    <row r="63" ht="12.0" customHeight="1"/>
+    <row r="64" ht="12.0" customHeight="1"/>
+    <row r="65" ht="12.0" customHeight="1"/>
+    <row r="66" ht="12.0" customHeight="1"/>
+    <row r="67" ht="12.0" customHeight="1"/>
+    <row r="68" ht="12.0" customHeight="1"/>
+    <row r="69" ht="12.0" customHeight="1"/>
+    <row r="70" ht="12.0" customHeight="1"/>
+    <row r="71" ht="12.0" customHeight="1"/>
+    <row r="72" ht="12.0" customHeight="1"/>
+    <row r="73" ht="12.0" customHeight="1"/>
+    <row r="74" ht="12.0" customHeight="1"/>
+    <row r="75" ht="12.0" customHeight="1"/>
+    <row r="76" ht="12.0" customHeight="1"/>
+    <row r="77" ht="12.0" customHeight="1"/>
+    <row r="78" ht="12.0" customHeight="1"/>
+    <row r="79" ht="12.0" customHeight="1"/>
+    <row r="80" ht="12.0" customHeight="1"/>
+    <row r="81" ht="12.0" customHeight="1"/>
+    <row r="82" ht="12.0" customHeight="1"/>
+    <row r="83" ht="12.0" customHeight="1"/>
+    <row r="84" ht="12.0" customHeight="1"/>
+    <row r="85" ht="12.0" customHeight="1"/>
+    <row r="86" ht="12.0" customHeight="1"/>
+    <row r="87" ht="12.0" customHeight="1"/>
+    <row r="88" ht="12.0" customHeight="1"/>
+    <row r="89" ht="12.0" customHeight="1"/>
+    <row r="90" ht="12.0" customHeight="1"/>
+    <row r="91" ht="12.0" customHeight="1"/>
+    <row r="92" ht="12.0" customHeight="1"/>
+    <row r="93" ht="12.0" customHeight="1"/>
+    <row r="94" ht="12.0" customHeight="1"/>
+    <row r="95" ht="12.0" customHeight="1"/>
+    <row r="96" ht="12.0" customHeight="1"/>
+    <row r="97" ht="12.0" customHeight="1"/>
+    <row r="98" ht="12.0" customHeight="1"/>
+    <row r="99" ht="12.0" customHeight="1"/>
+    <row r="100" ht="12.0" customHeight="1"/>
+    <row r="101" ht="12.0" customHeight="1"/>
+    <row r="102" ht="12.0" customHeight="1"/>
+    <row r="103" ht="12.0" customHeight="1"/>
+    <row r="104" ht="12.0" customHeight="1"/>
+    <row r="105" ht="12.0" customHeight="1"/>
+    <row r="106" ht="12.0" customHeight="1"/>
+    <row r="107" ht="12.0" customHeight="1"/>
+    <row r="108" ht="12.0" customHeight="1"/>
+    <row r="109" ht="12.0" customHeight="1"/>
+    <row r="110" ht="12.0" customHeight="1"/>
+    <row r="111" ht="12.0" customHeight="1"/>
+    <row r="112" ht="12.0" customHeight="1"/>
+    <row r="113" ht="12.0" customHeight="1"/>
+    <row r="114" ht="12.0" customHeight="1"/>
+    <row r="115" ht="12.0" customHeight="1"/>
+    <row r="116" ht="12.0" customHeight="1"/>
+    <row r="117" ht="12.0" customHeight="1"/>
+    <row r="118" ht="12.0" customHeight="1"/>
+    <row r="119" ht="12.0" customHeight="1"/>
+    <row r="120" ht="12.0" customHeight="1"/>
+    <row r="121" ht="12.0" customHeight="1"/>
+    <row r="122" ht="12.0" customHeight="1"/>
+    <row r="123" ht="12.0" customHeight="1"/>
+    <row r="124" ht="12.0" customHeight="1"/>
+    <row r="125" ht="12.0" customHeight="1"/>
+    <row r="126" ht="12.0" customHeight="1"/>
+    <row r="127" ht="12.0" customHeight="1"/>
+    <row r="128" ht="12.0" customHeight="1"/>
+    <row r="129" ht="12.0" customHeight="1"/>
+    <row r="130" ht="12.0" customHeight="1"/>
+    <row r="131" ht="12.0" customHeight="1"/>
+    <row r="132" ht="12.0" customHeight="1"/>
+    <row r="133" ht="12.0" customHeight="1"/>
+    <row r="134" ht="12.0" customHeight="1"/>
+    <row r="135" ht="12.0" customHeight="1"/>
+    <row r="136" ht="12.0" customHeight="1"/>
+    <row r="137" ht="12.0" customHeight="1"/>
+    <row r="138" ht="12.0" customHeight="1"/>
+    <row r="139" ht="12.0" customHeight="1"/>
+    <row r="140" ht="12.0" customHeight="1"/>
+    <row r="141" ht="12.0" customHeight="1"/>
+    <row r="142" ht="12.0" customHeight="1"/>
+    <row r="143" ht="12.0" customHeight="1"/>
+    <row r="144" ht="12.0" customHeight="1"/>
+    <row r="145" ht="12.0" customHeight="1"/>
+    <row r="146" ht="12.0" customHeight="1"/>
+    <row r="147" ht="12.0" customHeight="1"/>
+    <row r="148" ht="12.0" customHeight="1"/>
+    <row r="149" ht="12.0" customHeight="1"/>
+    <row r="150" ht="12.0" customHeight="1"/>
+    <row r="151" ht="12.0" customHeight="1"/>
+    <row r="152" ht="12.0" customHeight="1"/>
+    <row r="153" ht="12.0" customHeight="1"/>
+    <row r="154" ht="12.0" customHeight="1"/>
+    <row r="155" ht="12.0" customHeight="1"/>
+    <row r="156" ht="12.0" customHeight="1"/>
+    <row r="157" ht="12.0" customHeight="1"/>
+    <row r="158" ht="12.0" customHeight="1"/>
+    <row r="159" ht="12.0" customHeight="1"/>
+    <row r="160" ht="12.0" customHeight="1"/>
+    <row r="161" ht="12.0" customHeight="1"/>
+    <row r="162" ht="12.0" customHeight="1"/>
+    <row r="163" ht="12.0" customHeight="1"/>
+    <row r="164" ht="12.0" customHeight="1"/>
+    <row r="165" ht="12.0" customHeight="1"/>
+    <row r="166" ht="12.0" customHeight="1"/>
+    <row r="167" ht="12.0" customHeight="1"/>
+    <row r="168" ht="12.0" customHeight="1"/>
+    <row r="169" ht="12.0" customHeight="1"/>
+    <row r="170" ht="12.0" customHeight="1"/>
+    <row r="171" ht="12.0" customHeight="1"/>
+    <row r="172" ht="12.0" customHeight="1"/>
+    <row r="173" ht="12.0" customHeight="1"/>
+    <row r="174" ht="12.0" customHeight="1"/>
+    <row r="175" ht="12.0" customHeight="1"/>
+    <row r="176" ht="12.0" customHeight="1"/>
+    <row r="177" ht="12.0" customHeight="1"/>
+    <row r="178" ht="12.0" customHeight="1"/>
+    <row r="179" ht="12.0" customHeight="1"/>
+    <row r="180" ht="12.0" customHeight="1"/>
+    <row r="181" ht="12.0" customHeight="1"/>
+    <row r="182" ht="12.0" customHeight="1"/>
+    <row r="183" ht="12.0" customHeight="1"/>
+    <row r="184" ht="12.0" customHeight="1"/>
+    <row r="185" ht="12.0" customHeight="1"/>
+    <row r="186" ht="12.0" customHeight="1"/>
+    <row r="187" ht="12.0" customHeight="1"/>
+    <row r="188" ht="12.0" customHeight="1"/>
+    <row r="189" ht="12.0" customHeight="1"/>
+    <row r="190" ht="12.0" customHeight="1"/>
+    <row r="191" ht="12.0" customHeight="1"/>
+    <row r="192" ht="12.0" customHeight="1"/>
+    <row r="193" ht="12.0" customHeight="1"/>
+    <row r="194" ht="12.0" customHeight="1"/>
+    <row r="195" ht="12.0" customHeight="1"/>
+    <row r="196" ht="12.0" customHeight="1"/>
+    <row r="197" ht="12.0" customHeight="1"/>
+    <row r="198" ht="12.0" customHeight="1"/>
+    <row r="199" ht="12.0" customHeight="1"/>
+    <row r="200" ht="12.0" customHeight="1"/>
+    <row r="201" ht="12.0" customHeight="1"/>
+    <row r="202" ht="12.0" customHeight="1"/>
+    <row r="203" ht="12.0" customHeight="1"/>
+    <row r="204" ht="12.0" customHeight="1"/>
+    <row r="205" ht="12.0" customHeight="1"/>
+    <row r="206" ht="12.0" customHeight="1"/>
+    <row r="207" ht="12.0" customHeight="1"/>
+    <row r="208" ht="12.0" customHeight="1"/>
+    <row r="209" ht="12.0" customHeight="1"/>
+    <row r="210" ht="12.0" customHeight="1"/>
+    <row r="211" ht="12.0" customHeight="1"/>
+    <row r="212" ht="12.0" customHeight="1"/>
+    <row r="213" ht="12.0" customHeight="1"/>
+    <row r="214" ht="12.0" customHeight="1"/>
+    <row r="215" ht="12.0" customHeight="1"/>
+    <row r="216" ht="12.0" customHeight="1"/>
+    <row r="217" ht="12.0" customHeight="1"/>
+    <row r="218" ht="12.0" customHeight="1"/>
+    <row r="219" ht="12.0" customHeight="1"/>
+    <row r="220" ht="12.0" customHeight="1"/>
+    <row r="221" ht="12.0" customHeight="1"/>
+    <row r="222" ht="12.0" customHeight="1"/>
+    <row r="223" ht="12.0" customHeight="1"/>
+    <row r="224" ht="12.0" customHeight="1"/>
+    <row r="225" ht="12.0" customHeight="1"/>
+    <row r="226" ht="12.0" customHeight="1"/>
+    <row r="227" ht="12.0" customHeight="1"/>
+    <row r="228" ht="12.0" customHeight="1"/>
+    <row r="229" ht="12.0" customHeight="1"/>
+    <row r="230" ht="12.0" customHeight="1"/>
+    <row r="231" ht="12.0" customHeight="1"/>
+    <row r="232" ht="12.0" customHeight="1"/>
+    <row r="233" ht="12.0" customHeight="1"/>
+    <row r="234" ht="12.0" customHeight="1"/>
+    <row r="235" ht="12.0" customHeight="1"/>
+    <row r="236" ht="12.0" customHeight="1"/>
+    <row r="237" ht="12.0" customHeight="1"/>
+    <row r="238" ht="12.0" customHeight="1"/>
+    <row r="239" ht="12.0" customHeight="1"/>
+    <row r="240" ht="12.0" customHeight="1"/>
+    <row r="241" ht="12.0" customHeight="1"/>
+    <row r="242" ht="12.0" customHeight="1"/>
+    <row r="243" ht="12.0" customHeight="1"/>
+    <row r="244" ht="12.0" customHeight="1"/>
+    <row r="245" ht="12.0" customHeight="1"/>
+    <row r="246" ht="12.0" customHeight="1"/>
+    <row r="247" ht="12.0" customHeight="1"/>
+    <row r="248" ht="12.0" customHeight="1"/>
+    <row r="249" ht="12.0" customHeight="1"/>
+    <row r="250" ht="12.0" customHeight="1"/>
+    <row r="251" ht="12.0" customHeight="1"/>
+    <row r="252" ht="12.0" customHeight="1"/>
+    <row r="253" ht="12.0" customHeight="1"/>
+    <row r="254" ht="12.0" customHeight="1"/>
+    <row r="255" ht="12.0" customHeight="1"/>
+    <row r="256" ht="12.0" customHeight="1"/>
+    <row r="257" ht="12.0" customHeight="1"/>
+    <row r="258" ht="12.0" customHeight="1"/>
+    <row r="259" ht="12.0" customHeight="1"/>
+    <row r="260" ht="12.0" customHeight="1"/>
+    <row r="261" ht="12.0" customHeight="1"/>
+    <row r="262" ht="12.0" customHeight="1"/>
+    <row r="263" ht="12.0" customHeight="1"/>
+    <row r="264" ht="12.0" customHeight="1"/>
+    <row r="265" ht="12.0" customHeight="1"/>
+    <row r="266" ht="12.0" customHeight="1"/>
+    <row r="267" ht="12.0" customHeight="1"/>
+    <row r="268" ht="12.0" customHeight="1"/>
+    <row r="269" ht="12.0" customHeight="1"/>
+    <row r="270" ht="12.0" customHeight="1"/>
+    <row r="271" ht="12.0" customHeight="1"/>
+    <row r="272" ht="12.0" customHeight="1"/>
+    <row r="273" ht="12.0" customHeight="1"/>
+    <row r="274" ht="12.0" customHeight="1"/>
+    <row r="275" ht="12.0" customHeight="1"/>
+    <row r="276" ht="12.0" customHeight="1"/>
+    <row r="277" ht="12.0" customHeight="1"/>
+    <row r="278" ht="12.0" customHeight="1"/>
+    <row r="279" ht="12.0" customHeight="1"/>
+    <row r="280" ht="12.0" customHeight="1"/>
+    <row r="281" ht="12.0" customHeight="1"/>
+    <row r="282" ht="12.0" customHeight="1"/>
+    <row r="283" ht="12.0" customHeight="1"/>
+    <row r="284" ht="12.0" customHeight="1"/>
+    <row r="285" ht="12.0" customHeight="1"/>
+    <row r="286" ht="12.0" customHeight="1"/>
+    <row r="287" ht="12.0" customHeight="1"/>
+    <row r="288" ht="12.0" customHeight="1"/>
+    <row r="289" ht="12.0" customHeight="1"/>
+    <row r="290" ht="12.0" customHeight="1"/>
+    <row r="291" ht="12.0" customHeight="1"/>
+    <row r="292" ht="12.0" customHeight="1"/>
+    <row r="293" ht="12.0" customHeight="1"/>
+    <row r="294" ht="12.0" customHeight="1"/>
+    <row r="295" ht="12.0" customHeight="1"/>
+    <row r="296" ht="12.0" customHeight="1"/>
+    <row r="297" ht="12.0" customHeight="1"/>
+    <row r="298" ht="12.0" customHeight="1"/>
+    <row r="299" ht="12.0" customHeight="1"/>
+    <row r="300" ht="12.0" customHeight="1"/>
+    <row r="301" ht="12.0" customHeight="1"/>
+    <row r="302" ht="12.0" customHeight="1"/>
+    <row r="303" ht="12.0" customHeight="1"/>
+    <row r="304" ht="12.0" customHeight="1"/>
+    <row r="305" ht="12.0" customHeight="1"/>
+    <row r="306" ht="12.0" customHeight="1"/>
+    <row r="307" ht="12.0" customHeight="1"/>
+    <row r="308" ht="12.0" customHeight="1"/>
+    <row r="309" ht="12.0" customHeight="1"/>
+    <row r="310" ht="12.0" customHeight="1"/>
+    <row r="311" ht="12.0" customHeight="1"/>
+    <row r="312" ht="12.0" customHeight="1"/>
+    <row r="313" ht="12.0" customHeight="1"/>
+    <row r="314" ht="12.0" customHeight="1"/>
+    <row r="315" ht="12.0" customHeight="1"/>
+    <row r="316" ht="12.0" customHeight="1"/>
+    <row r="317" ht="12.0" customHeight="1"/>
+    <row r="318" ht="12.0" customHeight="1"/>
+    <row r="319" ht="12.0" customHeight="1"/>
+    <row r="320" ht="12.0" customHeight="1"/>
+    <row r="321" ht="12.0" customHeight="1"/>
+    <row r="322" ht="12.0" customHeight="1"/>
+    <row r="323" ht="12.0" customHeight="1"/>
+    <row r="324" ht="12.0" customHeight="1"/>
+    <row r="325" ht="12.0" customHeight="1"/>
+    <row r="326" ht="12.0" customHeight="1"/>
+    <row r="327" ht="12.0" customHeight="1"/>
+    <row r="328" ht="12.0" customHeight="1"/>
+    <row r="329" ht="12.0" customHeight="1"/>
+    <row r="330" ht="12.0" customHeight="1"/>
+    <row r="331" ht="12.0" customHeight="1"/>
+    <row r="332" ht="12.0" customHeight="1"/>
+    <row r="333" ht="12.0" customHeight="1"/>
+    <row r="334" ht="12.0" customHeight="1"/>
+    <row r="335" ht="12.0" customHeight="1"/>
+    <row r="336" ht="12.0" customHeight="1"/>
+    <row r="337" ht="12.0" customHeight="1"/>
+    <row r="338" ht="12.0" customHeight="1"/>
+    <row r="339" ht="12.0" customHeight="1"/>
+    <row r="340" ht="12.0" customHeight="1"/>
+    <row r="341" ht="12.0" customHeight="1"/>
+    <row r="342" ht="12.0" customHeight="1"/>
+    <row r="343" ht="12.0" customHeight="1"/>
+    <row r="344" ht="12.0" customHeight="1"/>
+    <row r="345" ht="12.0" customHeight="1"/>
+    <row r="346" ht="12.0" customHeight="1"/>
+    <row r="347" ht="12.0" customHeight="1"/>
+    <row r="348" ht="12.0" customHeight="1"/>
+    <row r="349" ht="12.0" customHeight="1"/>
+    <row r="350" ht="12.0" customHeight="1"/>
+    <row r="351" ht="12.0" customHeight="1"/>
+    <row r="352" ht="12.0" customHeight="1"/>
+    <row r="353" ht="12.0" customHeight="1"/>
+    <row r="354" ht="12.0" customHeight="1"/>
+    <row r="355" ht="12.0" customHeight="1"/>
+    <row r="356" ht="12.0" customHeight="1"/>
+    <row r="357" ht="12.0" customHeight="1"/>
+    <row r="358" ht="12.0" customHeight="1"/>
+    <row r="359" ht="12.0" customHeight="1"/>
+    <row r="360" ht="12.0" customHeight="1"/>
+    <row r="361" ht="12.0" customHeight="1"/>
+    <row r="362" ht="12.0" customHeight="1"/>
+    <row r="363" ht="12.0" customHeight="1"/>
+    <row r="364" ht="12.0" customHeight="1"/>
+    <row r="365" ht="12.0" customHeight="1"/>
+    <row r="366" ht="12.0" customHeight="1"/>
+    <row r="367" ht="12.0" customHeight="1"/>
+    <row r="368" ht="12.0" customHeight="1"/>
+    <row r="369" ht="12.0" customHeight="1"/>
+    <row r="370" ht="12.0" customHeight="1"/>
+    <row r="371" ht="12.0" customHeight="1"/>
+    <row r="372" ht="12.0" customHeight="1"/>
+    <row r="373" ht="12.0" customHeight="1"/>
+    <row r="374" ht="12.0" customHeight="1"/>
+    <row r="375" ht="12.0" customHeight="1"/>
+    <row r="376" ht="12.0" customHeight="1"/>
+    <row r="377" ht="12.0" customHeight="1"/>
+    <row r="378" ht="12.0" customHeight="1"/>
+    <row r="379" ht="12.0" customHeight="1"/>
+    <row r="380" ht="12.0" customHeight="1"/>
+    <row r="381" ht="12.0" customHeight="1"/>
+    <row r="382" ht="12.0" customHeight="1"/>
+    <row r="383" ht="12.0" customHeight="1"/>
+    <row r="384" ht="12.0" customHeight="1"/>
+    <row r="385" ht="12.0" customHeight="1"/>
+    <row r="386" ht="12.0" customHeight="1"/>
+    <row r="387" ht="12.0" customHeight="1"/>
+    <row r="388" ht="12.0" customHeight="1"/>
+    <row r="389" ht="12.0" customHeight="1"/>
+    <row r="390" ht="12.0" customHeight="1"/>
+    <row r="391" ht="12.0" customHeight="1"/>
+    <row r="392" ht="12.0" customHeight="1"/>
+    <row r="393" ht="12.0" customHeight="1"/>
+    <row r="394" ht="12.0" customHeight="1"/>
+    <row r="395" ht="12.0" customHeight="1"/>
+    <row r="396" ht="12.0" customHeight="1"/>
+    <row r="397" ht="12.0" customHeight="1"/>
+    <row r="398" ht="12.0" customHeight="1"/>
+    <row r="399" ht="12.0" customHeight="1"/>
+    <row r="400" ht="12.0" customHeight="1"/>
+    <row r="401" ht="12.0" customHeight="1"/>
+    <row r="402" ht="12.0" customHeight="1"/>
+    <row r="403" ht="12.0" customHeight="1"/>
+    <row r="404" ht="12.0" customHeight="1"/>
+    <row r="405" ht="12.0" customHeight="1"/>
+    <row r="406" ht="12.0" customHeight="1"/>
+    <row r="407" ht="12.0" customHeight="1"/>
+    <row r="408" ht="12.0" customHeight="1"/>
+    <row r="409" ht="12.0" customHeight="1"/>
+    <row r="410" ht="12.0" customHeight="1"/>
+    <row r="411" ht="12.0" customHeight="1"/>
+    <row r="412" ht="12.0" customHeight="1"/>
+    <row r="413" ht="12.0" customHeight="1"/>
+    <row r="414" ht="12.0" customHeight="1"/>
+    <row r="415" ht="12.0" customHeight="1"/>
+    <row r="416" ht="12.0" customHeight="1"/>
+    <row r="417" ht="12.0" customHeight="1"/>
+    <row r="418" ht="12.0" customHeight="1"/>
+    <row r="419" ht="12.0" customHeight="1"/>
+    <row r="420" ht="12.0" customHeight="1"/>
+    <row r="421" ht="12.0" customHeight="1"/>
+    <row r="422" ht="12.0" customHeight="1"/>
+    <row r="423" ht="12.0" customHeight="1"/>
+    <row r="424" ht="12.0" customHeight="1"/>
+    <row r="425" ht="12.0" customHeight="1"/>
+    <row r="426" ht="12.0" customHeight="1"/>
+    <row r="427" ht="12.0" customHeight="1"/>
+    <row r="428" ht="12.0" customHeight="1"/>
+    <row r="429" ht="12.0" customHeight="1"/>
+    <row r="430" ht="12.0" customHeight="1"/>
+    <row r="431" ht="12.0" customHeight="1"/>
+    <row r="432" ht="12.0" customHeight="1"/>
+    <row r="433" ht="12.0" customHeight="1"/>
+    <row r="434" ht="12.0" customHeight="1"/>
+    <row r="435" ht="12.0" customHeight="1"/>
+    <row r="436" ht="12.0" customHeight="1"/>
+    <row r="437" ht="12.0" customHeight="1"/>
+    <row r="438" ht="12.0" customHeight="1"/>
+    <row r="439" ht="12.0" customHeight="1"/>
+    <row r="440" ht="12.0" customHeight="1"/>
+    <row r="441" ht="12.0" customHeight="1"/>
+    <row r="442" ht="12.0" customHeight="1"/>
+    <row r="443" ht="12.0" customHeight="1"/>
+    <row r="444" ht="12.0" customHeight="1"/>
+    <row r="445" ht="12.0" customHeight="1"/>
+    <row r="446" ht="12.0" customHeight="1"/>
+    <row r="447" ht="12.0" customHeight="1"/>
+    <row r="448" ht="12.0" customHeight="1"/>
+    <row r="449" ht="12.0" customHeight="1"/>
+    <row r="450" ht="12.0" customHeight="1"/>
+    <row r="451" ht="12.0" customHeight="1"/>
+    <row r="452" ht="12.0" customHeight="1"/>
+    <row r="453" ht="12.0" customHeight="1"/>
+    <row r="454" ht="12.0" customHeight="1"/>
+    <row r="455" ht="12.0" customHeight="1"/>
+    <row r="456" ht="12.0" customHeight="1"/>
+    <row r="457" ht="12.0" customHeight="1"/>
+    <row r="458" ht="12.0" customHeight="1"/>
+    <row r="459" ht="12.0" customHeight="1"/>
+    <row r="460" ht="12.0" customHeight="1"/>
+    <row r="461" ht="12.0" customHeight="1"/>
+    <row r="462" ht="12.0" customHeight="1"/>
+    <row r="463" ht="12.0" customHeight="1"/>
+    <row r="464" ht="12.0" customHeight="1"/>
+    <row r="465" ht="12.0" customHeight="1"/>
+    <row r="466" ht="12.0" customHeight="1"/>
+    <row r="467" ht="12.0" customHeight="1"/>
+    <row r="468" ht="12.0" customHeight="1"/>
+    <row r="469" ht="12.0" customHeight="1"/>
+    <row r="470" ht="12.0" customHeight="1"/>
+    <row r="471" ht="12.0" customHeight="1"/>
+    <row r="472" ht="12.0" customHeight="1"/>
+    <row r="473" ht="12.0" customHeight="1"/>
+    <row r="474" ht="12.0" customHeight="1"/>
+    <row r="475" ht="12.0" customHeight="1"/>
+    <row r="476" ht="12.0" customHeight="1"/>
+    <row r="477" ht="12.0" customHeight="1"/>
+    <row r="478" ht="12.0" customHeight="1"/>
+    <row r="479" ht="12.0" customHeight="1"/>
+    <row r="480" ht="12.0" customHeight="1"/>
+    <row r="481" ht="12.0" customHeight="1"/>
+    <row r="482" ht="12.0" customHeight="1"/>
+    <row r="483" ht="12.0" customHeight="1"/>
+    <row r="484" ht="12.0" customHeight="1"/>
+    <row r="485" ht="12.0" customHeight="1"/>
+    <row r="486" ht="12.0" customHeight="1"/>
+    <row r="487" ht="12.0" customHeight="1"/>
+    <row r="488" ht="12.0" customHeight="1"/>
+    <row r="489" ht="12.0" customHeight="1"/>
+    <row r="490" ht="12.0" customHeight="1"/>
+    <row r="491" ht="12.0" customHeight="1"/>
+    <row r="492" ht="12.0" customHeight="1"/>
+    <row r="493" ht="12.0" customHeight="1"/>
+    <row r="494" ht="12.0" customHeight="1"/>
+    <row r="495" ht="12.0" customHeight="1"/>
+    <row r="496" ht="12.0" customHeight="1"/>
+    <row r="497" ht="12.0" customHeight="1"/>
+    <row r="498" ht="12.0" customHeight="1"/>
+    <row r="499" ht="12.0" customHeight="1"/>
+    <row r="500" ht="12.0" customHeight="1"/>
+    <row r="501" ht="12.0" customHeight="1"/>
+    <row r="502" ht="12.0" customHeight="1"/>
+    <row r="503" ht="12.0" customHeight="1"/>
+    <row r="504" ht="12.0" customHeight="1"/>
+    <row r="505" ht="12.0" customHeight="1"/>
+    <row r="506" ht="12.0" customHeight="1"/>
+    <row r="507" ht="12.0" customHeight="1"/>
+    <row r="508" ht="12.0" customHeight="1"/>
+    <row r="509" ht="12.0" customHeight="1"/>
+    <row r="510" ht="12.0" customHeight="1"/>
+    <row r="511" ht="12.0" customHeight="1"/>
+    <row r="512" ht="12.0" customHeight="1"/>
+    <row r="513" ht="12.0" customHeight="1"/>
+    <row r="514" ht="12.0" customHeight="1"/>
+    <row r="515" ht="12.0" customHeight="1"/>
+    <row r="516" ht="12.0" customHeight="1"/>
+    <row r="517" ht="12.0" customHeight="1"/>
+    <row r="518" ht="12.0" customHeight="1"/>
+    <row r="519" ht="12.0" customHeight="1"/>
+    <row r="520" ht="12.0" customHeight="1"/>
+    <row r="521" ht="12.0" customHeight="1"/>
+    <row r="522" ht="12.0" customHeight="1"/>
+    <row r="523" ht="12.0" customHeight="1"/>
+    <row r="524" ht="12.0" customHeight="1"/>
+    <row r="525" ht="12.0" customHeight="1"/>
+    <row r="526" ht="12.0" customHeight="1"/>
+    <row r="527" ht="12.0" customHeight="1"/>
+    <row r="528" ht="12.0" customHeight="1"/>
+    <row r="529" ht="12.0" customHeight="1"/>
+    <row r="530" ht="12.0" customHeight="1"/>
+    <row r="531" ht="12.0" customHeight="1"/>
+    <row r="532" ht="12.0" customHeight="1"/>
+    <row r="533" ht="12.0" customHeight="1"/>
+    <row r="534" ht="12.0" customHeight="1"/>
+    <row r="535" ht="12.0" customHeight="1"/>
+    <row r="536" ht="12.0" customHeight="1"/>
+    <row r="537" ht="12.0" customHeight="1"/>
+    <row r="538" ht="12.0" customHeight="1"/>
+    <row r="539" ht="12.0" customHeight="1"/>
+    <row r="540" ht="12.0" customHeight="1"/>
+    <row r="541" ht="12.0" customHeight="1"/>
+    <row r="542" ht="12.0" customHeight="1"/>
+    <row r="543" ht="12.0" customHeight="1"/>
+    <row r="544" ht="12.0" customHeight="1"/>
+    <row r="545" ht="12.0" customHeight="1"/>
+    <row r="546" ht="12.0" customHeight="1"/>
+    <row r="547" ht="12.0" customHeight="1"/>
+    <row r="548" ht="12.0" customHeight="1"/>
+    <row r="549" ht="12.0" customHeight="1"/>
+    <row r="550" ht="12.0" customHeight="1"/>
+    <row r="551" ht="12.0" customHeight="1"/>
+    <row r="552" ht="12.0" customHeight="1"/>
+    <row r="553" ht="12.0" customHeight="1"/>
+    <row r="554" ht="12.0" customHeight="1"/>
+    <row r="555" ht="12.0" customHeight="1"/>
+    <row r="556" ht="12.0" customHeight="1"/>
+    <row r="557" ht="12.0" customHeight="1"/>
+    <row r="558" ht="12.0" customHeight="1"/>
+    <row r="559" ht="12.0" customHeight="1"/>
+    <row r="560" ht="12.0" customHeight="1"/>
+    <row r="561" ht="12.0" customHeight="1"/>
+    <row r="562" ht="12.0" customHeight="1"/>
+    <row r="563" ht="12.0" customHeight="1"/>
+    <row r="564" ht="12.0" customHeight="1"/>
+    <row r="565" ht="12.0" customHeight="1"/>
+    <row r="566" ht="12.0" customHeight="1"/>
+    <row r="567" ht="12.0" customHeight="1"/>
+    <row r="568" ht="12.0" customHeight="1"/>
+    <row r="569" ht="12.0" customHeight="1"/>
+    <row r="570" ht="12.0" customHeight="1"/>
+    <row r="571" ht="12.0" customHeight="1"/>
+    <row r="572" ht="12.0" customHeight="1"/>
+    <row r="573" ht="12.0" customHeight="1"/>
+    <row r="574" ht="12.0" customHeight="1"/>
+    <row r="575" ht="12.0" customHeight="1"/>
+    <row r="576" ht="12.0" customHeight="1"/>
+    <row r="577" ht="12.0" customHeight="1"/>
+    <row r="578" ht="12.0" customHeight="1"/>
+    <row r="579" ht="12.0" customHeight="1"/>
+    <row r="580" ht="12.0" customHeight="1"/>
+    <row r="581" ht="12.0" customHeight="1"/>
+    <row r="582" ht="12.0" customHeight="1"/>
+    <row r="583" ht="12.0" customHeight="1"/>
+    <row r="584" ht="12.0" customHeight="1"/>
+    <row r="585" ht="12.0" customHeight="1"/>
+    <row r="586" ht="12.0" customHeight="1"/>
+    <row r="587" ht="12.0" customHeight="1"/>
+    <row r="588" ht="12.0" customHeight="1"/>
+    <row r="589" ht="12.0" customHeight="1"/>
+    <row r="590" ht="12.0" customHeight="1"/>
+    <row r="591" ht="12.0" customHeight="1"/>
+    <row r="592" ht="12.0" customHeight="1"/>
+    <row r="593" ht="12.0" customHeight="1"/>
+    <row r="594" ht="12.0" customHeight="1"/>
+    <row r="595" ht="12.0" customHeight="1"/>
+    <row r="596" ht="12.0" customHeight="1"/>
+    <row r="597" ht="12.0" customHeight="1"/>
+    <row r="598" ht="12.0" customHeight="1"/>
+    <row r="599" ht="12.0" customHeight="1"/>
+    <row r="600" ht="12.0" customHeight="1"/>
+    <row r="601" ht="12.0" customHeight="1"/>
+    <row r="602" ht="12.0" customHeight="1"/>
+    <row r="603" ht="12.0" customHeight="1"/>
+    <row r="604" ht="12.0" customHeight="1"/>
+    <row r="605" ht="12.0" customHeight="1"/>
+    <row r="606" ht="12.0" customHeight="1"/>
+    <row r="607" ht="12.0" customHeight="1"/>
+    <row r="608" ht="12.0" customHeight="1"/>
+    <row r="609" ht="12.0" customHeight="1"/>
+    <row r="610" ht="12.0" customHeight="1"/>
+    <row r="611" ht="12.0" customHeight="1"/>
+    <row r="612" ht="12.0" customHeight="1"/>
+    <row r="613" ht="12.0" customHeight="1"/>
+    <row r="614" ht="12.0" customHeight="1"/>
+    <row r="615" ht="12.0" customHeight="1"/>
+    <row r="616" ht="12.0" customHeight="1"/>
+    <row r="617" ht="12.0" customHeight="1"/>
+    <row r="618" ht="12.0" customHeight="1"/>
+    <row r="619" ht="12.0" customHeight="1"/>
+    <row r="620" ht="12.0" customHeight="1"/>
+    <row r="621" ht="12.0" customHeight="1"/>
+    <row r="622" ht="12.0" customHeight="1"/>
+    <row r="623" ht="12.0" customHeight="1"/>
+    <row r="624" ht="12.0" customHeight="1"/>
+    <row r="625" ht="12.0" customHeight="1"/>
+    <row r="626" ht="12.0" customHeight="1"/>
+    <row r="627" ht="12.0" customHeight="1"/>
+    <row r="628" ht="12.0" customHeight="1"/>
+    <row r="629" ht="12.0" customHeight="1"/>
+    <row r="630" ht="12.0" customHeight="1"/>
+    <row r="631" ht="12.0" customHeight="1"/>
+    <row r="632" ht="12.0" customHeight="1"/>
+    <row r="633" ht="12.0" customHeight="1"/>
+    <row r="634" ht="12.0" customHeight="1"/>
+    <row r="635" ht="12.0" customHeight="1"/>
+    <row r="636" ht="12.0" customHeight="1"/>
+    <row r="637" ht="12.0" customHeight="1"/>
+    <row r="638" ht="12.0" customHeight="1"/>
+    <row r="639" ht="12.0" customHeight="1"/>
+    <row r="640" ht="12.0" customHeight="1"/>
+    <row r="641" ht="12.0" customHeight="1"/>
+    <row r="642" ht="12.0" customHeight="1"/>
+    <row r="643" ht="12.0" customHeight="1"/>
+    <row r="644" ht="12.0" customHeight="1"/>
+    <row r="645" ht="12.0" customHeight="1"/>
+    <row r="646" ht="12.0" customHeight="1"/>
+    <row r="647" ht="12.0" customHeight="1"/>
+    <row r="648" ht="12.0" customHeight="1"/>
+    <row r="649" ht="12.0" customHeight="1"/>
+    <row r="650" ht="12.0" customHeight="1"/>
+    <row r="651" ht="12.0" customHeight="1"/>
+    <row r="652" ht="12.0" customHeight="1"/>
+    <row r="653" ht="12.0" customHeight="1"/>
+    <row r="654" ht="12.0" customHeight="1"/>
+    <row r="655" ht="12.0" customHeight="1"/>
+    <row r="656" ht="12.0" customHeight="1"/>
+    <row r="657" ht="12.0" customHeight="1"/>
+    <row r="658" ht="12.0" customHeight="1"/>
+    <row r="659" ht="12.0" customHeight="1"/>
+    <row r="660" ht="12.0" customHeight="1"/>
+    <row r="661" ht="12.0" customHeight="1"/>
+    <row r="662" ht="12.0" customHeight="1"/>
+    <row r="663" ht="12.0" customHeight="1"/>
+    <row r="664" ht="12.0" customHeight="1"/>
+    <row r="665" ht="12.0" customHeight="1"/>
+    <row r="666" ht="12.0" customHeight="1"/>
+    <row r="667" ht="12.0" customHeight="1"/>
+    <row r="668" ht="12.0" customHeight="1"/>
+    <row r="669" ht="12.0" customHeight="1"/>
+    <row r="670" ht="12.0" customHeight="1"/>
+    <row r="671" ht="12.0" customHeight="1"/>
+    <row r="672" ht="12.0" customHeight="1"/>
+    <row r="673" ht="12.0" customHeight="1"/>
+    <row r="674" ht="12.0" customHeight="1"/>
+    <row r="675" ht="12.0" customHeight="1"/>
+    <row r="676" ht="12.0" customHeight="1"/>
+    <row r="677" ht="12.0" customHeight="1"/>
+    <row r="678" ht="12.0" customHeight="1"/>
+    <row r="679" ht="12.0" customHeight="1"/>
+    <row r="680" ht="12.0" customHeight="1"/>
+    <row r="681" ht="12.0" customHeight="1"/>
+    <row r="682" ht="12.0" customHeight="1"/>
+    <row r="683" ht="12.0" customHeight="1"/>
+    <row r="684" ht="12.0" customHeight="1"/>
+    <row r="685" ht="12.0" customHeight="1"/>
+    <row r="686" ht="12.0" customHeight="1"/>
+    <row r="687" ht="12.0" customHeight="1"/>
+    <row r="688" ht="12.0" customHeight="1"/>
+    <row r="689" ht="12.0" customHeight="1"/>
+    <row r="690" ht="12.0" customHeight="1"/>
+    <row r="691" ht="12.0" customHeight="1"/>
+    <row r="692" ht="12.0" customHeight="1"/>
+    <row r="693" ht="12.0" customHeight="1"/>
+    <row r="694" ht="12.0" customHeight="1"/>
+    <row r="695" ht="12.0" customHeight="1"/>
+    <row r="696" ht="12.0" customHeight="1"/>
+    <row r="697" ht="12.0" customHeight="1"/>
+    <row r="698" ht="12.0" customHeight="1"/>
+    <row r="699" ht="12.0" customHeight="1"/>
+    <row r="700" ht="12.0" customHeight="1"/>
+    <row r="701" ht="12.0" customHeight="1"/>
+    <row r="702" ht="12.0" customHeight="1"/>
+    <row r="703" ht="12.0" customHeight="1"/>
+    <row r="704" ht="12.0" customHeight="1"/>
+    <row r="705" ht="12.0" customHeight="1"/>
+    <row r="706" ht="12.0" customHeight="1"/>
+    <row r="707" ht="12.0" customHeight="1"/>
+    <row r="708" ht="12.0" customHeight="1"/>
+    <row r="709" ht="12.0" customHeight="1"/>
+    <row r="710" ht="12.0" customHeight="1"/>
+    <row r="711" ht="12.0" customHeight="1"/>
+    <row r="712" ht="12.0" customHeight="1"/>
+    <row r="713" ht="12.0" customHeight="1"/>
+    <row r="714" ht="12.0" customHeight="1"/>
+    <row r="715" ht="12.0" customHeight="1"/>
+    <row r="716" ht="12.0" customHeight="1"/>
+    <row r="717" ht="12.0" customHeight="1"/>
+    <row r="718" ht="12.0" customHeight="1"/>
+    <row r="719" ht="12.0" customHeight="1"/>
+    <row r="720" ht="12.0" customHeight="1"/>
+    <row r="721" ht="12.0" customHeight="1"/>
+    <row r="722" ht="12.0" customHeight="1"/>
+    <row r="723" ht="12.0" customHeight="1"/>
+    <row r="724" ht="12.0" customHeight="1"/>
+    <row r="725" ht="12.0" customHeight="1"/>
+    <row r="726" ht="12.0" customHeight="1"/>
+    <row r="727" ht="12.0" customHeight="1"/>
+    <row r="728" ht="12.0" customHeight="1"/>
+    <row r="729" ht="12.0" customHeight="1"/>
+    <row r="730" ht="12.0" customHeight="1"/>
+    <row r="731" ht="12.0" customHeight="1"/>
+    <row r="732" ht="12.0" customHeight="1"/>
+    <row r="733" ht="12.0" customHeight="1"/>
+    <row r="734" ht="12.0" customHeight="1"/>
+    <row r="735" ht="12.0" customHeight="1"/>
+    <row r="736" ht="12.0" customHeight="1"/>
+    <row r="737" ht="12.0" customHeight="1"/>
+    <row r="738" ht="12.0" customHeight="1"/>
+    <row r="739" ht="12.0" customHeight="1"/>
+    <row r="740" ht="12.0" customHeight="1"/>
+    <row r="741" ht="12.0" customHeight="1"/>
+    <row r="742" ht="12.0" customHeight="1"/>
+    <row r="743" ht="12.0" customHeight="1"/>
+    <row r="744" ht="12.0" customHeight="1"/>
+    <row r="745" ht="12.0" customHeight="1"/>
+    <row r="746" ht="12.0" customHeight="1"/>
+    <row r="747" ht="12.0" customHeight="1"/>
+    <row r="748" ht="12.0" customHeight="1"/>
+    <row r="749" ht="12.0" customHeight="1"/>
+    <row r="750" ht="12.0" customHeight="1"/>
+    <row r="751" ht="12.0" customHeight="1"/>
+    <row r="752" ht="12.0" customHeight="1"/>
+    <row r="753" ht="12.0" customHeight="1"/>
+    <row r="754" ht="12.0" customHeight="1"/>
+    <row r="755" ht="12.0" customHeight="1"/>
+    <row r="756" ht="12.0" customHeight="1"/>
+    <row r="757" ht="12.0" customHeight="1"/>
+    <row r="758" ht="12.0" customHeight="1"/>
+    <row r="759" ht="12.0" customHeight="1"/>
+    <row r="760" ht="12.0" customHeight="1"/>
+    <row r="761" ht="12.0" customHeight="1"/>
+    <row r="762" ht="12.0" customHeight="1"/>
+    <row r="763" ht="12.0" customHeight="1"/>
+    <row r="764" ht="12.0" customHeight="1"/>
+    <row r="765" ht="12.0" customHeight="1"/>
+    <row r="766" ht="12.0" customHeight="1"/>
+    <row r="767" ht="12.0" customHeight="1"/>
+    <row r="768" ht="12.0" customHeight="1"/>
+    <row r="769" ht="12.0" customHeight="1"/>
+    <row r="770" ht="12.0" customHeight="1"/>
+    <row r="771" ht="12.0" customHeight="1"/>
+    <row r="772" ht="12.0" customHeight="1"/>
+    <row r="773" ht="12.0" customHeight="1"/>
+    <row r="774" ht="12.0" customHeight="1"/>
+    <row r="775" ht="12.0" customHeight="1"/>
+    <row r="776" ht="12.0" customHeight="1"/>
+    <row r="777" ht="12.0" customHeight="1"/>
+    <row r="778" ht="12.0" customHeight="1"/>
+    <row r="779" ht="12.0" customHeight="1"/>
+    <row r="780" ht="12.0" customHeight="1"/>
+    <row r="781" ht="12.0" customHeight="1"/>
+    <row r="782" ht="12.0" customHeight="1"/>
+    <row r="783" ht="12.0" customHeight="1"/>
+    <row r="784" ht="12.0" customHeight="1"/>
+    <row r="785" ht="12.0" customHeight="1"/>
+    <row r="786" ht="12.0" customHeight="1"/>
+    <row r="787" ht="12.0" customHeight="1"/>
+    <row r="788" ht="12.0" customHeight="1"/>
+    <row r="789" ht="12.0" customHeight="1"/>
+    <row r="790" ht="12.0" customHeight="1"/>
+    <row r="791" ht="12.0" customHeight="1"/>
+    <row r="792" ht="12.0" customHeight="1"/>
+    <row r="793" ht="12.0" customHeight="1"/>
+    <row r="794" ht="12.0" customHeight="1"/>
+    <row r="795" ht="12.0" customHeight="1"/>
+    <row r="796" ht="12.0" customHeight="1"/>
+    <row r="797" ht="12.0" customHeight="1"/>
+    <row r="798" ht="12.0" customHeight="1"/>
+    <row r="799" ht="12.0" customHeight="1"/>
+    <row r="800" ht="12.0" customHeight="1"/>
+    <row r="801" ht="12.0" customHeight="1"/>
+    <row r="802" ht="12.0" customHeight="1"/>
+    <row r="803" ht="12.0" customHeight="1"/>
+    <row r="804" ht="12.0" customHeight="1"/>
+    <row r="805" ht="12.0" customHeight="1"/>
+    <row r="806" ht="12.0" customHeight="1"/>
+    <row r="807" ht="12.0" customHeight="1"/>
+    <row r="808" ht="12.0" customHeight="1"/>
+    <row r="809" ht="12.0" customHeight="1"/>
+    <row r="810" ht="12.0" customHeight="1"/>
+    <row r="811" ht="12.0" customHeight="1"/>
+    <row r="812" ht="12.0" customHeight="1"/>
+    <row r="813" ht="12.0" customHeight="1"/>
+    <row r="814" ht="12.0" customHeight="1"/>
+    <row r="815" ht="12.0" customHeight="1"/>
+    <row r="816" ht="12.0" customHeight="1"/>
+    <row r="817" ht="12.0" customHeight="1"/>
+    <row r="818" ht="12.0" customHeight="1"/>
+    <row r="819" ht="12.0" customHeight="1"/>
+    <row r="820" ht="12.0" customHeight="1"/>
+    <row r="821" ht="12.0" customHeight="1"/>
+    <row r="822" ht="12.0" customHeight="1"/>
+    <row r="823" ht="12.0" customHeight="1"/>
+    <row r="824" ht="12.0" customHeight="1"/>
+    <row r="825" ht="12.0" customHeight="1"/>
+    <row r="826" ht="12.0" customHeight="1"/>
+    <row r="827" ht="12.0" customHeight="1"/>
+    <row r="828" ht="12.0" customHeight="1"/>
+    <row r="829" ht="12.0" customHeight="1"/>
+    <row r="830" ht="12.0" customHeight="1"/>
+    <row r="831" ht="12.0" customHeight="1"/>
+    <row r="832" ht="12.0" customHeight="1"/>
+    <row r="833" ht="12.0" customHeight="1"/>
+    <row r="834" ht="12.0" customHeight="1"/>
+    <row r="835" ht="12.0" customHeight="1"/>
+    <row r="836" ht="12.0" customHeight="1"/>
+    <row r="837" ht="12.0" customHeight="1"/>
+    <row r="838" ht="12.0" customHeight="1"/>
+    <row r="839" ht="12.0" customHeight="1"/>
+    <row r="840" ht="12.0" customHeight="1"/>
+    <row r="841" ht="12.0" customHeight="1"/>
+    <row r="842" ht="12.0" customHeight="1"/>
+    <row r="843" ht="12.0" customHeight="1"/>
+    <row r="844" ht="12.0" customHeight="1"/>
+    <row r="845" ht="12.0" customHeight="1"/>
+    <row r="846" ht="12.0" customHeight="1"/>
+    <row r="847" ht="12.0" customHeight="1"/>
+    <row r="848" ht="12.0" customHeight="1"/>
+    <row r="849" ht="12.0" customHeight="1"/>
+    <row r="850" ht="12.0" customHeight="1"/>
+    <row r="851" ht="12.0" customHeight="1"/>
+    <row r="852" ht="12.0" customHeight="1"/>
+    <row r="853" ht="12.0" customHeight="1"/>
+    <row r="854" ht="12.0" customHeight="1"/>
+    <row r="855" ht="12.0" customHeight="1"/>
+    <row r="856" ht="12.0" customHeight="1"/>
+    <row r="857" ht="12.0" customHeight="1"/>
+    <row r="858" ht="12.0" customHeight="1"/>
+    <row r="859" ht="12.0" customHeight="1"/>
+    <row r="860" ht="12.0" customHeight="1"/>
+    <row r="861" ht="12.0" customHeight="1"/>
+    <row r="862" ht="12.0" customHeight="1"/>
+    <row r="863" ht="12.0" customHeight="1"/>
+    <row r="864" ht="12.0" customHeight="1"/>
+    <row r="865" ht="12.0" customHeight="1"/>
+    <row r="866" ht="12.0" customHeight="1"/>
+    <row r="867" ht="12.0" customHeight="1"/>
+    <row r="868" ht="12.0" customHeight="1"/>
+    <row r="869" ht="12.0" customHeight="1"/>
+    <row r="870" ht="12.0" customHeight="1"/>
+    <row r="871" ht="12.0" customHeight="1"/>
+    <row r="872" ht="12.0" customHeight="1"/>
+    <row r="873" ht="12.0" customHeight="1"/>
+    <row r="874" ht="12.0" customHeight="1"/>
+    <row r="875" ht="12.0" customHeight="1"/>
+    <row r="876" ht="12.0" customHeight="1"/>
+    <row r="877" ht="12.0" customHeight="1"/>
+    <row r="878" ht="12.0" customHeight="1"/>
+    <row r="879" ht="12.0" customHeight="1"/>
+    <row r="880" ht="12.0" customHeight="1"/>
+    <row r="881" ht="12.0" customHeight="1"/>
+    <row r="882" ht="12.0" customHeight="1"/>
+    <row r="883" ht="12.0" customHeight="1"/>
+    <row r="884" ht="12.0" customHeight="1"/>
+    <row r="885" ht="12.0" customHeight="1"/>
+    <row r="886" ht="12.0" customHeight="1"/>
+    <row r="887" ht="12.0" customHeight="1"/>
+    <row r="888" ht="12.0" customHeight="1"/>
+    <row r="889" ht="12.0" customHeight="1"/>
+    <row r="890" ht="12.0" customHeight="1"/>
+    <row r="891" ht="12.0" customHeight="1"/>
+    <row r="892" ht="12.0" customHeight="1"/>
+    <row r="893" ht="12.0" customHeight="1"/>
+    <row r="894" ht="12.0" customHeight="1"/>
+    <row r="895" ht="12.0" customHeight="1"/>
+    <row r="896" ht="12.0" customHeight="1"/>
+    <row r="897" ht="12.0" customHeight="1"/>
+    <row r="898" ht="12.0" customHeight="1"/>
+    <row r="899" ht="12.0" customHeight="1"/>
+    <row r="900" ht="12.0" customHeight="1"/>
+    <row r="901" ht="12.0" customHeight="1"/>
+    <row r="902" ht="12.0" customHeight="1"/>
+    <row r="903" ht="12.0" customHeight="1"/>
+    <row r="904" ht="12.0" customHeight="1"/>
+    <row r="905" ht="12.0" customHeight="1"/>
+    <row r="906" ht="12.0" customHeight="1"/>
+    <row r="907" ht="12.0" customHeight="1"/>
+    <row r="908" ht="12.0" customHeight="1"/>
+    <row r="909" ht="12.0" customHeight="1"/>
+    <row r="910" ht="12.0" customHeight="1"/>
+    <row r="911" ht="12.0" customHeight="1"/>
+    <row r="912" ht="12.0" customHeight="1"/>
+    <row r="913" ht="12.0" customHeight="1"/>
+    <row r="914" ht="12.0" customHeight="1"/>
+    <row r="915" ht="12.0" customHeight="1"/>
+    <row r="916" ht="12.0" customHeight="1"/>
+    <row r="917" ht="12.0" customHeight="1"/>
+    <row r="918" ht="12.0" customHeight="1"/>
+    <row r="919" ht="12.0" customHeight="1"/>
+    <row r="920" ht="12.0" customHeight="1"/>
+    <row r="921" ht="12.0" customHeight="1"/>
+    <row r="922" ht="12.0" customHeight="1"/>
+    <row r="923" ht="12.0" customHeight="1"/>
+    <row r="924" ht="12.0" customHeight="1"/>
+    <row r="925" ht="12.0" customHeight="1"/>
+    <row r="926" ht="12.0" customHeight="1"/>
+    <row r="927" ht="12.0" customHeight="1"/>
+    <row r="928" ht="12.0" customHeight="1"/>
+    <row r="929" ht="12.0" customHeight="1"/>
+    <row r="930" ht="12.0" customHeight="1"/>
+    <row r="931" ht="12.0" customHeight="1"/>
+    <row r="932" ht="12.0" customHeight="1"/>
+    <row r="933" ht="12.0" customHeight="1"/>
+    <row r="934" ht="12.0" customHeight="1"/>
+    <row r="935" ht="12.0" customHeight="1"/>
+    <row r="936" ht="12.0" customHeight="1"/>
+    <row r="937" ht="12.0" customHeight="1"/>
+    <row r="938" ht="12.0" customHeight="1"/>
+    <row r="939" ht="12.0" customHeight="1"/>
+    <row r="940" ht="12.0" customHeight="1"/>
+    <row r="941" ht="12.0" customHeight="1"/>
+    <row r="942" ht="12.0" customHeight="1"/>
+    <row r="943" ht="12.0" customHeight="1"/>
+    <row r="944" ht="12.0" customHeight="1"/>
+    <row r="945" ht="12.0" customHeight="1"/>
+    <row r="946" ht="12.0" customHeight="1"/>
+    <row r="947" ht="12.0" customHeight="1"/>
+    <row r="948" ht="12.0" customHeight="1"/>
+    <row r="949" ht="12.0" customHeight="1"/>
+    <row r="950" ht="12.0" customHeight="1"/>
+    <row r="951" ht="12.0" customHeight="1"/>
+    <row r="952" ht="12.0" customHeight="1"/>
+    <row r="953" ht="12.0" customHeight="1"/>
+    <row r="954" ht="12.0" customHeight="1"/>
+    <row r="955" ht="12.0" customHeight="1"/>
+    <row r="956" ht="12.0" customHeight="1"/>
+    <row r="957" ht="12.0" customHeight="1"/>
+    <row r="958" ht="12.0" customHeight="1"/>
+    <row r="959" ht="12.0" customHeight="1"/>
+    <row r="960" ht="12.0" customHeight="1"/>
+    <row r="961" ht="12.0" customHeight="1"/>
+    <row r="962" ht="12.0" customHeight="1"/>
+    <row r="963" ht="12.0" customHeight="1"/>
+    <row r="964" ht="12.0" customHeight="1"/>
+    <row r="965" ht="12.0" customHeight="1"/>
+    <row r="966" ht="12.0" customHeight="1"/>
+    <row r="967" ht="12.0" customHeight="1"/>
+    <row r="968" ht="12.0" customHeight="1"/>
+    <row r="969" ht="12.0" customHeight="1"/>
+    <row r="970" ht="12.0" customHeight="1"/>
+    <row r="971" ht="12.0" customHeight="1"/>
+    <row r="972" ht="12.0" customHeight="1"/>
+    <row r="973" ht="12.0" customHeight="1"/>
+    <row r="974" ht="12.0" customHeight="1"/>
+    <row r="975" ht="12.0" customHeight="1"/>
+    <row r="976" ht="12.0" customHeight="1"/>
+    <row r="977" ht="12.0" customHeight="1"/>
+    <row r="978" ht="12.0" customHeight="1"/>
+    <row r="979" ht="12.0" customHeight="1"/>
+    <row r="980" ht="12.0" customHeight="1"/>
+    <row r="981" ht="12.0" customHeight="1"/>
+    <row r="982" ht="12.0" customHeight="1"/>
+    <row r="983" ht="12.0" customHeight="1"/>
+    <row r="984" ht="12.0" customHeight="1"/>
+    <row r="985" ht="12.0" customHeight="1"/>
+    <row r="986" ht="12.0" customHeight="1"/>
+    <row r="987" ht="12.0" customHeight="1"/>
+    <row r="988" ht="12.0" customHeight="1"/>
+    <row r="989" ht="12.0" customHeight="1"/>
+    <row r="990" ht="12.0" customHeight="1"/>
+    <row r="991" ht="12.0" customHeight="1"/>
+    <row r="992" ht="12.0" customHeight="1"/>
+    <row r="993" ht="12.0" customHeight="1"/>
+    <row r="994" ht="12.0" customHeight="1"/>
+    <row r="995" ht="12.0" customHeight="1"/>
+    <row r="996" ht="12.0" customHeight="1"/>
+    <row r="997" ht="12.0" customHeight="1"/>
+    <row r="998" ht="12.0" customHeight="1"/>
+    <row r="999" ht="12.0" customHeight="1"/>
+    <row r="1000" ht="12.0" customHeight="1"/>
+  </sheetData>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -2646,15 +3849,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="49.43"/>
     <col customWidth="1" min="3" max="3" width="15.0"/>
     <col customWidth="1" min="4" max="4" width="31.14"/>
     <col customWidth="1" min="5" max="5" width="16.29"/>
-    <col customWidth="1" min="6" max="9" width="14.43"/>
     <col customWidth="1" min="10" max="10" width="11.86"/>
     <col customWidth="1" min="11" max="11" width="16.29"/>
-    <col customWidth="1" min="12" max="32" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -2977,7 +4177,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="28"/>
+      <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -3134,8 +4334,8 @@
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
-      <c r="AE14" s="29"/>
-      <c r="AF14" s="29"/>
+      <c r="AE14" s="28"/>
+      <c r="AF14" s="28"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3"/>
@@ -3202,8 +4402,8 @@
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
-      <c r="AE16" s="29"/>
-      <c r="AF16" s="29"/>
+      <c r="AE16" s="28"/>
+      <c r="AF16" s="28"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="3"/>
@@ -3338,8 +4538,8 @@
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
-      <c r="AE20" s="29"/>
-      <c r="AF20" s="29"/>
+      <c r="AE20" s="28"/>
+      <c r="AF20" s="28"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
@@ -3406,8 +4606,8 @@
       <c r="AB22" s="3"/>
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
-      <c r="AE22" s="29"/>
-      <c r="AF22" s="29"/>
+      <c r="AE22" s="28"/>
+      <c r="AF22" s="28"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="3"/>
@@ -3440,8 +4640,8 @@
       <c r="AB23" s="3"/>
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
-      <c r="AE23" s="29"/>
-      <c r="AF23" s="29"/>
+      <c r="AE23" s="28"/>
+      <c r="AF23" s="28"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="3"/>
@@ -3474,8 +4674,8 @@
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
-      <c r="AE24" s="29"/>
-      <c r="AF24" s="29"/>
+      <c r="AE24" s="28"/>
+      <c r="AF24" s="28"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="3"/>
@@ -3508,8 +4708,8 @@
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
-      <c r="AE25" s="29"/>
-      <c r="AF25" s="29"/>
+      <c r="AE25" s="28"/>
+      <c r="AF25" s="28"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3"/>
@@ -3542,8 +4742,8 @@
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
-      <c r="AE26" s="29"/>
-      <c r="AF26" s="29"/>
+      <c r="AE26" s="28"/>
+      <c r="AF26" s="28"/>
     </row>
     <row r="27" ht="12.0" customHeight="1"/>
     <row r="28" ht="12.0" customHeight="1"/>
@@ -4537,18 +5737,14 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="49.43"/>
     <col customWidth="1" min="3" max="3" width="15.14"/>
     <col customWidth="1" min="4" max="4" width="28.43"/>
     <col customWidth="1" min="5" max="5" width="13.86"/>
-    <col customWidth="1" min="6" max="9" width="14.43"/>
     <col customWidth="1" min="10" max="10" width="11.86"/>
     <col customWidth="1" min="11" max="11" width="16.29"/>
-    <col customWidth="1" min="12" max="12" width="14.43"/>
     <col customWidth="1" min="13" max="13" width="19.29"/>
     <col customWidth="1" min="14" max="14" width="48.29"/>
-    <col customWidth="1" min="15" max="32" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -4783,7 +5979,7 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="30"/>
+      <c r="N8" s="29"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -4837,10 +6033,10 @@
       <c r="K9" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="30" t="s">
         <v>40</v>
       </c>
       <c r="N9" s="24" t="s">
@@ -5874,20 +7070,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="25.71"/>
     <col customWidth="1" min="3" max="3" width="15.29"/>
     <col customWidth="1" min="4" max="4" width="26.57"/>
     <col customWidth="1" min="5" max="6" width="15.86"/>
     <col customWidth="1" min="7" max="7" width="12.43"/>
-    <col customWidth="1" min="8" max="8" width="14.43"/>
     <col customWidth="1" min="9" max="9" width="13.0"/>
     <col customWidth="1" min="10" max="10" width="11.86"/>
     <col customWidth="1" min="11" max="11" width="16.29"/>
     <col customWidth="1" min="12" max="12" width="10.14"/>
     <col customWidth="1" min="13" max="13" width="12.71"/>
     <col customWidth="1" min="14" max="14" width="50.0"/>
-    <col customWidth="1" min="15" max="27" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -6089,7 +7282,7 @@
       <c r="N7" s="3"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="9"/>
@@ -6143,7 +7336,7 @@
       <c r="L9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="30" t="s">
         <v>44</v>
       </c>
       <c r="N9" s="15" t="s">
@@ -6168,13 +7361,13 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="34"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="33"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
@@ -6184,14 +7377,14 @@
       <c r="C11" s="22"/>
       <c r="D11" s="3"/>
       <c r="E11" s="22"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="36"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="35"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="37"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="36"/>
       <c r="N11" s="3"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
@@ -6200,14 +7393,14 @@
       <c r="C12" s="22"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="36"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="35"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="37"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="36"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" ht="12.0" customHeight="1"/>
@@ -7216,18 +8409,15 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="52.0"/>
     <col customWidth="1" min="3" max="3" width="15.14"/>
     <col customWidth="1" min="4" max="4" width="33.71"/>
     <col customWidth="1" min="5" max="5" width="13.86"/>
-    <col customWidth="1" min="6" max="9" width="14.43"/>
     <col customWidth="1" min="10" max="10" width="11.86"/>
     <col customWidth="1" min="11" max="11" width="16.29"/>
     <col customWidth="1" min="12" max="12" width="12.0"/>
     <col customWidth="1" min="13" max="13" width="19.29"/>
     <col customWidth="1" min="14" max="14" width="43.71"/>
-    <col customWidth="1" min="15" max="30" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -7515,7 +8705,7 @@
       <c r="L9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="30" t="s">
         <v>40</v>
       </c>
       <c r="N9" s="15" t="s">
@@ -8547,20 +9737,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="66.71"/>
     <col customWidth="1" min="3" max="3" width="15.14"/>
     <col customWidth="1" min="4" max="4" width="30.14"/>
     <col customWidth="1" min="5" max="6" width="13.86"/>
     <col customWidth="1" min="7" max="7" width="12.86"/>
     <col customWidth="1" min="8" max="8" width="13.14"/>
-    <col customWidth="1" min="9" max="9" width="14.43"/>
     <col customWidth="1" min="10" max="10" width="11.86"/>
     <col customWidth="1" min="11" max="11" width="16.29"/>
     <col customWidth="1" min="12" max="12" width="13.43"/>
     <col customWidth="1" min="13" max="13" width="19.29"/>
     <col customWidth="1" min="14" max="14" width="50.14"/>
-    <col customWidth="1" min="15" max="30" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -8818,13 +10005,13 @@
       <c r="B9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="30" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="24" t="s">
@@ -8845,17 +10032,17 @@
       <c r="K9" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="30" t="s">
         <v>40</v>
       </c>
       <c r="N9" s="15" t="s">
         <v>41</v>
       </c>
       <c r="O9" s="3"/>
-      <c r="P9" s="29"/>
+      <c r="P9" s="28"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
@@ -9880,18 +11067,14 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="49.43"/>
     <col customWidth="1" min="3" max="3" width="15.14"/>
     <col customWidth="1" min="4" max="4" width="31.14"/>
     <col customWidth="1" min="5" max="5" width="13.86"/>
-    <col customWidth="1" min="6" max="6" width="14.43"/>
     <col customWidth="1" min="7" max="7" width="17.71"/>
     <col customWidth="1" min="8" max="8" width="16.86"/>
     <col customWidth="1" min="9" max="9" width="16.29"/>
-    <col customWidth="1" min="10" max="10" width="14.43"/>
     <col customWidth="1" min="11" max="11" width="40.86"/>
-    <col customWidth="1" min="12" max="30" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -10121,7 +11304,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="38"/>
+      <c r="K8" s="37"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -10158,13 +11341,13 @@
       <c r="E9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="38" t="s">
         <v>51</v>
       </c>
       <c r="I9" s="25" t="s">
@@ -10173,7 +11356,7 @@
       <c r="J9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="40" t="s">
+      <c r="K9" s="39" t="s">
         <v>41</v>
       </c>
       <c r="L9" s="3"/>
@@ -11211,13 +12394,10 @@
     <col customWidth="1" min="4" max="4" width="22.14"/>
     <col customWidth="1" min="5" max="5" width="14.71"/>
     <col customWidth="1" min="6" max="6" width="13.71"/>
-    <col customWidth="1" min="7" max="7" width="14.43"/>
     <col customWidth="1" min="8" max="8" width="17.71"/>
     <col customWidth="1" min="9" max="9" width="16.29"/>
     <col customWidth="1" min="10" max="10" width="15.86"/>
-    <col customWidth="1" min="11" max="11" width="14.43"/>
     <col customWidth="1" min="12" max="12" width="40.86"/>
-    <col customWidth="1" min="13" max="26" width="14.43"/>
     <col customWidth="1" min="27" max="27" width="8.71"/>
   </cols>
   <sheetData>
@@ -11417,7 +12597,7 @@
       <c r="C9" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="15" t="s">
         <v>54</v>
       </c>
       <c r="E9" s="15" t="s">
@@ -11426,12 +12606,12 @@
       <c r="F9" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="25"/>
       <c r="K9" s="26"/>
-      <c r="L9" s="40"/>
+      <c r="L9" s="39"/>
       <c r="M9" s="3"/>
       <c r="N9" s="25"/>
       <c r="O9" s="3"/>
@@ -12633,13 +13813,13 @@
     <row r="7" ht="12.0" customHeight="1"/>
     <row r="8" ht="12.0" customHeight="1"/>
     <row r="9" ht="12.0" customHeight="1">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="40" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>